<commit_message>
Completed two more practices.
</commit_message>
<xml_diff>
--- a/LeetCode Techniques.xlsx
+++ b/LeetCode Techniques.xlsx
@@ -8,7 +8,7 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\jack.yao\Desktop\LeetCode\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{45949CCF-5102-4F88-BAB8-A0B350565402}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{49F06EA2-BD74-4252-B02C-F04CA4EB665D}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="-120" yWindow="-120" windowWidth="20640" windowHeight="11040" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
@@ -36,7 +36,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="141" uniqueCount="63">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="153" uniqueCount="68">
   <si>
     <t>Name</t>
   </si>
@@ -265,6 +265,22 @@
   </si>
   <si>
     <t>https://leetcode.com/problems/decode-string/</t>
+  </si>
+  <si>
+    <t>Find in Mountain Array</t>
+  </si>
+  <si>
+    <t>Create Sorted Array through Instructions</t>
+  </si>
+  <si>
+    <t>https://leetcode.com/problems/find-in-mountain-array/description/</t>
+  </si>
+  <si>
+    <t>https://leetcode.com/problems/create-sorted-array-through-instructions/description/</t>
+  </si>
+  <si>
+    <t>Use hash table to speed up
+calculation of bigger count.</t>
   </si>
 </sst>
 </file>
@@ -873,14 +889,14 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0000-000000000000}">
-  <dimension ref="A1:K13"/>
+  <dimension ref="A1:K15"/>
   <sheetViews>
     <sheetView tabSelected="1" zoomScaleNormal="100" workbookViewId="0"/>
   </sheetViews>
   <sheetFormatPr defaultColWidth="9" defaultRowHeight="15"/>
   <cols>
     <col min="1" max="1" width="11" customWidth="1"/>
-    <col min="2" max="2" width="35.7109375" customWidth="1"/>
+    <col min="2" max="2" width="38.28515625" customWidth="1"/>
     <col min="3" max="3" width="71" customWidth="1"/>
     <col min="4" max="4" width="16" customWidth="1"/>
     <col min="5" max="5" width="36" customWidth="1"/>
@@ -978,7 +994,7 @@
       <c r="J3" s="3"/>
       <c r="K3" s="2"/>
     </row>
-    <row r="4" spans="1:11" ht="39.950000000000003" customHeight="1">
+    <row r="4" spans="1:11" ht="30" customHeight="1">
       <c r="A4" s="4">
         <v>300</v>
       </c>
@@ -1175,71 +1191,71 @@
     </row>
     <row r="11" spans="1:11" ht="20.100000000000001" customHeight="1">
       <c r="A11" s="4">
-        <v>1825</v>
+        <v>1095</v>
       </c>
       <c r="B11" s="4" t="s">
-        <v>33</v>
+        <v>63</v>
       </c>
       <c r="C11" s="7" t="s">
-        <v>34</v>
+        <v>65</v>
       </c>
       <c r="D11" s="4" t="s">
-        <v>16</v>
+        <v>59</v>
       </c>
       <c r="E11" s="4"/>
-      <c r="F11" s="4" t="s">
-        <v>35</v>
-      </c>
+      <c r="F11" s="4"/>
       <c r="G11" s="4" t="s">
         <v>14</v>
       </c>
       <c r="H11" s="4" t="s">
-        <v>11</v>
+        <v>29</v>
       </c>
       <c r="I11" s="5">
-        <v>45400</v>
+        <v>45482</v>
       </c>
       <c r="J11" s="5"/>
       <c r="K11" s="4"/>
     </row>
-    <row r="12" spans="1:11" ht="20.100000000000001" customHeight="1">
+    <row r="12" spans="1:11" ht="30" customHeight="1">
       <c r="A12" s="4">
-        <v>2034</v>
+        <v>1649</v>
       </c>
       <c r="B12" s="4" t="s">
-        <v>25</v>
+        <v>64</v>
       </c>
       <c r="C12" s="7" t="s">
-        <v>26</v>
+        <v>66</v>
       </c>
       <c r="D12" s="4" t="s">
-        <v>10</v>
-      </c>
-      <c r="E12" s="4"/>
+        <v>59</v>
+      </c>
+      <c r="E12" s="6" t="s">
+        <v>67</v>
+      </c>
       <c r="F12" s="4" t="s">
-        <v>35</v>
+        <v>60</v>
       </c>
       <c r="G12" s="4" t="s">
-        <v>14</v>
+        <v>12</v>
       </c>
       <c r="H12" s="4" t="s">
         <v>11</v>
       </c>
       <c r="I12" s="5">
-        <v>45400</v>
+        <v>45482</v>
       </c>
       <c r="J12" s="5"/>
       <c r="K12" s="4"/>
     </row>
     <row r="13" spans="1:11" ht="20.100000000000001" customHeight="1">
       <c r="A13" s="4">
-        <v>2102</v>
+        <v>1825</v>
       </c>
       <c r="B13" s="4" t="s">
-        <v>23</v>
+        <v>33</v>
       </c>
       <c r="C13" s="7" t="s">
-        <v>24</v>
+        <v>34</v>
       </c>
       <c r="D13" s="4" t="s">
         <v>16</v>
@@ -1255,17 +1271,75 @@
         <v>11</v>
       </c>
       <c r="I13" s="5">
-        <v>45420</v>
+        <v>45400</v>
       </c>
       <c r="J13" s="5"/>
       <c r="K13" s="4"/>
     </row>
+    <row r="14" spans="1:11" ht="20.100000000000001" customHeight="1">
+      <c r="A14" s="4">
+        <v>2034</v>
+      </c>
+      <c r="B14" s="4" t="s">
+        <v>25</v>
+      </c>
+      <c r="C14" s="7" t="s">
+        <v>26</v>
+      </c>
+      <c r="D14" s="4" t="s">
+        <v>10</v>
+      </c>
+      <c r="E14" s="4"/>
+      <c r="F14" s="4" t="s">
+        <v>35</v>
+      </c>
+      <c r="G14" s="4" t="s">
+        <v>14</v>
+      </c>
+      <c r="H14" s="4" t="s">
+        <v>11</v>
+      </c>
+      <c r="I14" s="5">
+        <v>45400</v>
+      </c>
+      <c r="J14" s="5"/>
+      <c r="K14" s="4"/>
+    </row>
+    <row r="15" spans="1:11" ht="20.100000000000001" customHeight="1">
+      <c r="A15" s="4">
+        <v>2102</v>
+      </c>
+      <c r="B15" s="4" t="s">
+        <v>23</v>
+      </c>
+      <c r="C15" s="7" t="s">
+        <v>24</v>
+      </c>
+      <c r="D15" s="4" t="s">
+        <v>16</v>
+      </c>
+      <c r="E15" s="4"/>
+      <c r="F15" s="4" t="s">
+        <v>35</v>
+      </c>
+      <c r="G15" s="4" t="s">
+        <v>14</v>
+      </c>
+      <c r="H15" s="4" t="s">
+        <v>11</v>
+      </c>
+      <c r="I15" s="5">
+        <v>45420</v>
+      </c>
+      <c r="J15" s="5"/>
+      <c r="K15" s="4"/>
+    </row>
   </sheetData>
-  <sortState xmlns:xlrd2="http://schemas.microsoft.com/office/spreadsheetml/2017/richdata2" ref="A2:K13">
-    <sortCondition ref="A2:A13"/>
+  <sortState xmlns:xlrd2="http://schemas.microsoft.com/office/spreadsheetml/2017/richdata2" ref="A2:K15">
+    <sortCondition ref="A2:A15"/>
   </sortState>
   <phoneticPr fontId="1" type="noConversion"/>
-  <conditionalFormatting sqref="D4:E13">
+  <conditionalFormatting sqref="D4:E15">
     <cfRule type="expression" dxfId="17" priority="4">
       <formula>D4="Easy"</formula>
     </cfRule>
@@ -1291,16 +1365,19 @@
     <hyperlink ref="C7" r:id="rId1" xr:uid="{98DA09B4-ED1E-9841-BFC0-AD6132AF476B}"/>
     <hyperlink ref="C9" r:id="rId2" xr:uid="{355AB06F-F372-E64C-BB34-3D68811E6B00}"/>
     <hyperlink ref="C5" r:id="rId3" xr:uid="{A97C1B49-93D0-D74A-BF3C-F925EFE9FD83}"/>
-    <hyperlink ref="C13" r:id="rId4" xr:uid="{4C375694-D494-514B-B747-D72CA94420E6}"/>
-    <hyperlink ref="C12" r:id="rId5" xr:uid="{5E8F7E04-6349-4D42-B16F-92BF0082A8EC}"/>
+    <hyperlink ref="C15" r:id="rId4" xr:uid="{4C375694-D494-514B-B747-D72CA94420E6}"/>
+    <hyperlink ref="C14" r:id="rId5" xr:uid="{5E8F7E04-6349-4D42-B16F-92BF0082A8EC}"/>
     <hyperlink ref="C4" r:id="rId6" xr:uid="{C06E2E2A-F9EA-2C41-A2A2-0110BB4FE089}"/>
     <hyperlink ref="C8" r:id="rId7" xr:uid="{88F29B63-471E-1745-ABA5-15B0EE490696}"/>
-    <hyperlink ref="C11" r:id="rId8" xr:uid="{77B0B942-637D-9846-B52B-162446D656B7}"/>
+    <hyperlink ref="C13" r:id="rId8" xr:uid="{77B0B942-637D-9846-B52B-162446D656B7}"/>
     <hyperlink ref="C2" r:id="rId9" xr:uid="{FC6DC5BC-3B79-3A47-AD69-9FD63EE06424}"/>
     <hyperlink ref="C6" r:id="rId10" xr:uid="{82F4789C-38A4-1A4D-BA41-951136E51502}"/>
     <hyperlink ref="C10" r:id="rId11" xr:uid="{87D58C84-2A2E-5243-AD6C-F126296F2572}"/>
+    <hyperlink ref="C11" r:id="rId12" xr:uid="{E17A87F3-1678-4780-AF58-F4783F4A7A65}"/>
+    <hyperlink ref="C12" r:id="rId13" xr:uid="{AB427796-2FCF-4F37-AC47-998ADDB37E09}"/>
   </hyperlinks>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
+  <pageSetup paperSize="9" orientation="portrait" verticalDpi="0" r:id="rId14"/>
   <headerFooter>
     <oddFooter>&amp;L_x000D_&amp;1#&amp;"Calibri"&amp;10&amp;K000000 General</oddFooter>
   </headerFooter>

</xml_diff>

<commit_message>
Completed two DFS practices.
</commit_message>
<xml_diff>
--- a/LeetCode Techniques.xlsx
+++ b/LeetCode Techniques.xlsx
@@ -8,9 +8,9 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="/Users/blackjack625/Desktop/LeetCode/"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{A96C8C3E-6C34-5E48-816C-40342B8CE225}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{49444300-7889-7C45-BBE5-FAE34250899B}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="0" yWindow="500" windowWidth="20640" windowHeight="11040" activeTab="4" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
+    <workbookView xWindow="0" yWindow="500" windowWidth="20640" windowHeight="11040" activeTab="5" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
   <sheets>
     <sheet name="Binary Search" sheetId="1" r:id="rId1"/>
@@ -18,6 +18,7 @@
     <sheet name="Set Maneuver" sheetId="3" r:id="rId3"/>
     <sheet name="Recursion" sheetId="5" r:id="rId4"/>
     <sheet name="Trie" sheetId="4" r:id="rId5"/>
+    <sheet name="Depth First Search" sheetId="6" r:id="rId6"/>
   </sheets>
   <calcPr calcId="191029"/>
   <extLst>
@@ -37,7 +38,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="216" uniqueCount="92">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="239" uniqueCount="97">
   <si>
     <t>Name</t>
   </si>
@@ -375,6 +376,26 @@
   <si>
     <t>During trie storage,
 use a mark to count prefixes.</t>
+    <phoneticPr fontId="1" type="noConversion"/>
+  </si>
+  <si>
+    <t>Path Sum II</t>
+    <phoneticPr fontId="1" type="noConversion"/>
+  </si>
+  <si>
+    <t>Flatten Binary Tree to Linked List</t>
+    <phoneticPr fontId="1" type="noConversion"/>
+  </si>
+  <si>
+    <t>https://leetcode.com/problems/path-sum-ii/description/</t>
+    <phoneticPr fontId="1" type="noConversion"/>
+  </si>
+  <si>
+    <t>https://leetcode.com/problems/flatten-binary-tree-to-linked-list/description/</t>
+    <phoneticPr fontId="1" type="noConversion"/>
+  </si>
+  <si>
+    <t>Linked List</t>
     <phoneticPr fontId="1" type="noConversion"/>
   </si>
 </sst>
@@ -424,14 +445,6 @@
       <scheme val="minor"/>
     </font>
     <font>
-      <u/>
-      <sz val="10"/>
-      <color theme="10"/>
-      <name val="新細明體"/>
-      <family val="2"/>
-      <scheme val="minor"/>
-    </font>
-    <font>
       <sz val="10"/>
       <color theme="1"/>
       <name val="Microsoft YaHei"/>
@@ -441,10 +454,16 @@
       <u/>
       <sz val="10"/>
       <color theme="10"/>
-      <name val="新細明體"/>
-      <family val="1"/>
-      <charset val="136"/>
-      <scheme val="minor"/>
+      <name val="Microsoft YaHei"/>
+      <family val="2"/>
+      <charset val="134"/>
+    </font>
+    <font>
+      <sz val="11"/>
+      <color theme="1"/>
+      <name val="Microsoft YaHei"/>
+      <family val="2"/>
+      <charset val="134"/>
     </font>
   </fonts>
   <fills count="2">
@@ -501,21 +520,49 @@
     <xf numFmtId="0" fontId="3" fillId="0" borderId="1" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center" wrapText="1"/>
     </xf>
-    <xf numFmtId="0" fontId="5" fillId="0" borderId="1" xfId="1" applyFont="1" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="5" fillId="0" borderId="1" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="6" fillId="0" borderId="1" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="6" fillId="0" borderId="1" xfId="1" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="7" fillId="0" borderId="1" xfId="1" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
+    <xf numFmtId="0" fontId="7" fillId="0" borderId="0" xfId="0" applyFont="1"/>
   </cellXfs>
   <cellStyles count="2">
     <cellStyle name="一般" xfId="0" builtinId="0"/>
     <cellStyle name="超連結" xfId="1" builtinId="8"/>
   </cellStyles>
-  <dxfs count="21">
+  <dxfs count="24">
+    <dxf>
+      <font>
+        <color rgb="FFFFFF00"/>
+      </font>
+      <fill>
+        <patternFill>
+          <bgColor rgb="FFFF0000"/>
+        </patternFill>
+      </fill>
+    </dxf>
+    <dxf>
+      <font>
+        <color theme="1"/>
+      </font>
+      <fill>
+        <patternFill>
+          <bgColor rgb="FFFFFF00"/>
+        </patternFill>
+      </fill>
+    </dxf>
+    <dxf>
+      <font>
+        <color theme="0"/>
+      </font>
+      <fill>
+        <patternFill>
+          <bgColor rgb="FF00B050"/>
+        </patternFill>
+      </fill>
+    </dxf>
     <dxf>
       <font>
         <color rgb="FFFFFF00"/>
@@ -1030,11 +1077,11 @@
   <sheetViews>
     <sheetView zoomScaleNormal="100" workbookViewId="0"/>
   </sheetViews>
-  <sheetFormatPr baseColWidth="10" defaultColWidth="9" defaultRowHeight="14"/>
+  <sheetFormatPr baseColWidth="10" defaultColWidth="9" defaultRowHeight="17"/>
   <cols>
     <col min="1" max="1" width="11" customWidth="1"/>
     <col min="2" max="2" width="38.19921875" customWidth="1"/>
-    <col min="3" max="3" width="71" customWidth="1"/>
+    <col min="3" max="3" width="71" style="9" customWidth="1"/>
     <col min="4" max="4" width="16" customWidth="1"/>
     <col min="5" max="5" width="36" customWidth="1"/>
     <col min="6" max="8" width="21" customWidth="1"/>
@@ -1084,7 +1131,7 @@
       <c r="B2" s="4" t="s">
         <v>37</v>
       </c>
-      <c r="C2" s="7" t="s">
+      <c r="C2" s="8" t="s">
         <v>36</v>
       </c>
       <c r="D2" s="4" t="s">
@@ -1111,7 +1158,7 @@
       <c r="B3" s="4" t="s">
         <v>42</v>
       </c>
-      <c r="C3" s="7" t="s">
+      <c r="C3" s="8" t="s">
         <v>43</v>
       </c>
       <c r="D3" s="4" t="s">
@@ -1138,7 +1185,7 @@
       <c r="B4" s="4" t="s">
         <v>28</v>
       </c>
-      <c r="C4" s="7" t="s">
+      <c r="C4" s="8" t="s">
         <v>27</v>
       </c>
       <c r="D4" s="4" t="s">
@@ -1167,7 +1214,7 @@
       <c r="B5" s="4" t="s">
         <v>20</v>
       </c>
-      <c r="C5" s="7" t="s">
+      <c r="C5" s="8" t="s">
         <v>21</v>
       </c>
       <c r="D5" s="4" t="s">
@@ -1194,7 +1241,7 @@
       <c r="B6" s="4" t="s">
         <v>38</v>
       </c>
-      <c r="C6" s="7" t="s">
+      <c r="C6" s="8" t="s">
         <v>39</v>
       </c>
       <c r="D6" s="4" t="s">
@@ -1223,7 +1270,7 @@
       <c r="B7" s="4" t="s">
         <v>9</v>
       </c>
-      <c r="C7" s="7" t="s">
+      <c r="C7" s="8" t="s">
         <v>17</v>
       </c>
       <c r="D7" s="4" t="s">
@@ -1250,7 +1297,7 @@
       <c r="B8" s="4" t="s">
         <v>31</v>
       </c>
-      <c r="C8" s="7" t="s">
+      <c r="C8" s="8" t="s">
         <v>32</v>
       </c>
       <c r="D8" s="4" t="s">
@@ -1277,7 +1324,7 @@
       <c r="B9" s="4" t="s">
         <v>19</v>
       </c>
-      <c r="C9" s="7" t="s">
+      <c r="C9" s="8" t="s">
         <v>18</v>
       </c>
       <c r="D9" s="4" t="s">
@@ -1306,7 +1353,7 @@
       <c r="B10" s="4" t="s">
         <v>40</v>
       </c>
-      <c r="C10" s="7" t="s">
+      <c r="C10" s="8" t="s">
         <v>41</v>
       </c>
       <c r="D10" s="4" t="s">
@@ -1333,7 +1380,7 @@
       <c r="B11" s="4" t="s">
         <v>62</v>
       </c>
-      <c r="C11" s="7" t="s">
+      <c r="C11" s="8" t="s">
         <v>64</v>
       </c>
       <c r="D11" s="4" t="s">
@@ -1360,7 +1407,7 @@
       <c r="B12" s="4" t="s">
         <v>63</v>
       </c>
-      <c r="C12" s="7" t="s">
+      <c r="C12" s="8" t="s">
         <v>65</v>
       </c>
       <c r="D12" s="4" t="s">
@@ -1391,7 +1438,7 @@
       <c r="B13" s="4" t="s">
         <v>33</v>
       </c>
-      <c r="C13" s="7" t="s">
+      <c r="C13" s="8" t="s">
         <v>34</v>
       </c>
       <c r="D13" s="4" t="s">
@@ -1420,7 +1467,7 @@
       <c r="B14" s="4" t="s">
         <v>25</v>
       </c>
-      <c r="C14" s="7" t="s">
+      <c r="C14" s="8" t="s">
         <v>26</v>
       </c>
       <c r="D14" s="4" t="s">
@@ -1449,7 +1496,7 @@
       <c r="B15" s="4" t="s">
         <v>23</v>
       </c>
-      <c r="C15" s="7" t="s">
+      <c r="C15" s="8" t="s">
         <v>24</v>
       </c>
       <c r="D15" s="4" t="s">
@@ -1477,24 +1524,24 @@
   </sortState>
   <phoneticPr fontId="1" type="noConversion"/>
   <conditionalFormatting sqref="D2:D3">
-    <cfRule type="expression" dxfId="20" priority="1">
+    <cfRule type="expression" dxfId="23" priority="1">
       <formula>D2="Easy"</formula>
     </cfRule>
-    <cfRule type="expression" dxfId="19" priority="2">
+    <cfRule type="expression" dxfId="22" priority="2">
       <formula>D2="Medium"</formula>
     </cfRule>
-    <cfRule type="expression" dxfId="18" priority="3">
+    <cfRule type="expression" dxfId="21" priority="3">
       <formula>D2="Hard"</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="D4:E15">
-    <cfRule type="expression" dxfId="17" priority="4">
+    <cfRule type="expression" dxfId="20" priority="4">
       <formula>D4="Easy"</formula>
     </cfRule>
-    <cfRule type="expression" dxfId="16" priority="5">
+    <cfRule type="expression" dxfId="19" priority="5">
       <formula>D4="Medium"</formula>
     </cfRule>
-    <cfRule type="expression" dxfId="15" priority="6">
+    <cfRule type="expression" dxfId="18" priority="6">
       <formula>D4="Hard"</formula>
     </cfRule>
   </conditionalFormatting>
@@ -1527,11 +1574,11 @@
   <sheetViews>
     <sheetView zoomScaleNormal="100" workbookViewId="0"/>
   </sheetViews>
-  <sheetFormatPr baseColWidth="10" defaultColWidth="9" defaultRowHeight="14"/>
+  <sheetFormatPr baseColWidth="10" defaultColWidth="9" defaultRowHeight="17"/>
   <cols>
     <col min="1" max="1" width="11" customWidth="1"/>
     <col min="2" max="2" width="45.796875" customWidth="1"/>
-    <col min="3" max="3" width="71" customWidth="1"/>
+    <col min="3" max="3" width="71" style="9" customWidth="1"/>
     <col min="4" max="4" width="16" customWidth="1"/>
     <col min="5" max="5" width="36" customWidth="1"/>
     <col min="6" max="8" width="21" customWidth="1"/>
@@ -1581,7 +1628,7 @@
       <c r="B2" s="4" t="s">
         <v>47</v>
       </c>
-      <c r="C2" s="7" t="s">
+      <c r="C2" s="8" t="s">
         <v>46</v>
       </c>
       <c r="D2" s="4" t="s">
@@ -1608,7 +1655,7 @@
       <c r="B3" s="6" t="s">
         <v>48</v>
       </c>
-      <c r="C3" s="7" t="s">
+      <c r="C3" s="8" t="s">
         <v>50</v>
       </c>
       <c r="D3" s="4" t="s">
@@ -1631,13 +1678,13 @@
   </sheetData>
   <phoneticPr fontId="1" type="noConversion"/>
   <conditionalFormatting sqref="D2:E3">
-    <cfRule type="expression" dxfId="14" priority="4">
+    <cfRule type="expression" dxfId="17" priority="4">
       <formula>D2="Easy"</formula>
     </cfRule>
-    <cfRule type="expression" dxfId="13" priority="5">
+    <cfRule type="expression" dxfId="16" priority="5">
       <formula>D2="Medium"</formula>
     </cfRule>
-    <cfRule type="expression" dxfId="12" priority="6">
+    <cfRule type="expression" dxfId="15" priority="6">
       <formula>D2="Hard"</formula>
     </cfRule>
   </conditionalFormatting>
@@ -1658,11 +1705,11 @@
   <sheetViews>
     <sheetView zoomScaleNormal="100" workbookViewId="0"/>
   </sheetViews>
-  <sheetFormatPr baseColWidth="10" defaultColWidth="9" defaultRowHeight="14"/>
+  <sheetFormatPr baseColWidth="10" defaultColWidth="9" defaultRowHeight="17"/>
   <cols>
     <col min="1" max="1" width="11" customWidth="1"/>
     <col min="2" max="2" width="25.796875" customWidth="1"/>
-    <col min="3" max="3" width="65.796875" customWidth="1"/>
+    <col min="3" max="3" width="65.796875" style="9" customWidth="1"/>
     <col min="4" max="4" width="16" customWidth="1"/>
     <col min="5" max="5" width="36" customWidth="1"/>
     <col min="6" max="8" width="21" customWidth="1"/>
@@ -1709,10 +1756,10 @@
       <c r="A2" s="4">
         <v>41</v>
       </c>
-      <c r="B2" s="8" t="s">
+      <c r="B2" s="7" t="s">
         <v>56</v>
       </c>
-      <c r="C2" s="7" t="s">
+      <c r="C2" s="8" t="s">
         <v>57</v>
       </c>
       <c r="D2" s="4" t="s">
@@ -1743,7 +1790,7 @@
       <c r="B3" s="4" t="s">
         <v>52</v>
       </c>
-      <c r="C3" s="7" t="s">
+      <c r="C3" s="8" t="s">
         <v>51</v>
       </c>
       <c r="D3" s="4" t="s">
@@ -1770,7 +1817,7 @@
       <c r="B4" s="4" t="s">
         <v>53</v>
       </c>
-      <c r="C4" s="7" t="s">
+      <c r="C4" s="8" t="s">
         <v>55</v>
       </c>
       <c r="D4" s="4" t="s">
@@ -1793,24 +1840,24 @@
   </sheetData>
   <phoneticPr fontId="1" type="noConversion"/>
   <conditionalFormatting sqref="D2">
-    <cfRule type="expression" dxfId="11" priority="1">
+    <cfRule type="expression" dxfId="14" priority="1">
       <formula>D2="Easy"</formula>
     </cfRule>
-    <cfRule type="expression" dxfId="10" priority="2">
+    <cfRule type="expression" dxfId="13" priority="2">
       <formula>D2="Medium"</formula>
     </cfRule>
-    <cfRule type="expression" dxfId="9" priority="3">
+    <cfRule type="expression" dxfId="12" priority="3">
       <formula>D2="Hard"</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="D3:E4">
-    <cfRule type="expression" dxfId="8" priority="4">
+    <cfRule type="expression" dxfId="11" priority="4">
       <formula>D3="Easy"</formula>
     </cfRule>
-    <cfRule type="expression" dxfId="7" priority="5">
+    <cfRule type="expression" dxfId="10" priority="5">
       <formula>D3="Medium"</formula>
     </cfRule>
-    <cfRule type="expression" dxfId="6" priority="6">
+    <cfRule type="expression" dxfId="9" priority="6">
       <formula>D3="Hard"</formula>
     </cfRule>
   </conditionalFormatting>
@@ -1833,11 +1880,11 @@
   <sheetViews>
     <sheetView zoomScaleNormal="100" workbookViewId="0"/>
   </sheetViews>
-  <sheetFormatPr baseColWidth="10" defaultColWidth="9" defaultRowHeight="14"/>
+  <sheetFormatPr baseColWidth="10" defaultColWidth="9" defaultRowHeight="17"/>
   <cols>
     <col min="1" max="1" width="11" customWidth="1"/>
-    <col min="2" max="2" width="15.796875" customWidth="1"/>
-    <col min="3" max="3" width="35.796875" customWidth="1"/>
+    <col min="2" max="2" width="16" customWidth="1"/>
+    <col min="3" max="3" width="35.796875" style="9" customWidth="1"/>
     <col min="4" max="4" width="16" customWidth="1"/>
     <col min="5" max="5" width="36" customWidth="1"/>
     <col min="6" max="8" width="21" customWidth="1"/>
@@ -1884,10 +1931,10 @@
       <c r="A2" s="4">
         <v>394</v>
       </c>
-      <c r="B2" s="8" t="s">
+      <c r="B2" s="7" t="s">
         <v>60</v>
       </c>
-      <c r="C2" s="7" t="s">
+      <c r="C2" s="8" t="s">
         <v>61</v>
       </c>
       <c r="D2" s="4" t="s">
@@ -1910,13 +1957,13 @@
   </sheetData>
   <phoneticPr fontId="1" type="noConversion"/>
   <conditionalFormatting sqref="D2">
-    <cfRule type="expression" dxfId="5" priority="1">
+    <cfRule type="expression" dxfId="8" priority="1">
       <formula>D2="Easy"</formula>
     </cfRule>
-    <cfRule type="expression" dxfId="4" priority="2">
+    <cfRule type="expression" dxfId="7" priority="2">
       <formula>D2="Medium"</formula>
     </cfRule>
-    <cfRule type="expression" dxfId="3" priority="3">
+    <cfRule type="expression" dxfId="6" priority="3">
       <formula>D2="Hard"</formula>
     </cfRule>
   </conditionalFormatting>
@@ -1935,13 +1982,13 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{52261E16-6011-467F-965D-8624702367C9}">
   <dimension ref="A1:K10"/>
   <sheetViews>
-    <sheetView tabSelected="1" zoomScaleNormal="100" workbookViewId="0"/>
+    <sheetView zoomScaleNormal="100" workbookViewId="0"/>
   </sheetViews>
-  <sheetFormatPr baseColWidth="10" defaultColWidth="9" defaultRowHeight="14"/>
+  <sheetFormatPr baseColWidth="10" defaultColWidth="9" defaultRowHeight="17"/>
   <cols>
     <col min="1" max="1" width="11" customWidth="1"/>
     <col min="2" max="2" width="46" customWidth="1"/>
-    <col min="3" max="3" width="65.796875" customWidth="1"/>
+    <col min="3" max="3" width="65.796875" style="9" customWidth="1"/>
     <col min="4" max="4" width="16" customWidth="1"/>
     <col min="5" max="5" width="36" customWidth="1"/>
     <col min="6" max="8" width="21" customWidth="1"/>
@@ -1988,10 +2035,10 @@
       <c r="A2" s="4">
         <v>208</v>
       </c>
-      <c r="B2" s="8" t="s">
+      <c r="B2" s="7" t="s">
         <v>66</v>
       </c>
-      <c r="C2" s="7" t="s">
+      <c r="C2" s="8" t="s">
         <v>68</v>
       </c>
       <c r="D2" s="4" t="s">
@@ -2015,10 +2062,10 @@
       <c r="A3" s="4">
         <v>211</v>
       </c>
-      <c r="B3" s="8" t="s">
+      <c r="B3" s="7" t="s">
         <v>67</v>
       </c>
-      <c r="C3" s="9" t="s">
+      <c r="C3" s="8" t="s">
         <v>69</v>
       </c>
       <c r="D3" s="4" t="s">
@@ -2047,7 +2094,7 @@
       <c r="B4" s="4" t="s">
         <v>73</v>
       </c>
-      <c r="C4" s="9" t="s">
+      <c r="C4" s="8" t="s">
         <v>74</v>
       </c>
       <c r="D4" s="4" t="s">
@@ -2076,7 +2123,7 @@
       <c r="B5" s="4" t="s">
         <v>76</v>
       </c>
-      <c r="C5" s="9" t="s">
+      <c r="C5" s="8" t="s">
         <v>77</v>
       </c>
       <c r="D5" s="4" t="s">
@@ -2103,7 +2150,7 @@
       <c r="B6" s="4" t="s">
         <v>78</v>
       </c>
-      <c r="C6" s="9" t="s">
+      <c r="C6" s="8" t="s">
         <v>79</v>
       </c>
       <c r="D6" s="4" t="s">
@@ -2132,7 +2179,7 @@
       <c r="B7" s="4" t="s">
         <v>80</v>
       </c>
-      <c r="C7" s="9" t="s">
+      <c r="C7" s="8" t="s">
         <v>81</v>
       </c>
       <c r="D7" s="4" t="s">
@@ -2161,7 +2208,7 @@
       <c r="B8" s="4" t="s">
         <v>83</v>
       </c>
-      <c r="C8" s="9" t="s">
+      <c r="C8" s="8" t="s">
         <v>82</v>
       </c>
       <c r="D8" s="4" t="s">
@@ -2190,7 +2237,7 @@
       <c r="B9" s="4" t="s">
         <v>87</v>
       </c>
-      <c r="C9" s="9" t="s">
+      <c r="C9" s="8" t="s">
         <v>88</v>
       </c>
       <c r="D9" s="4" t="s">
@@ -2219,7 +2266,7 @@
       <c r="B10" s="4" t="s">
         <v>89</v>
       </c>
-      <c r="C10" s="9" t="s">
+      <c r="C10" s="8" t="s">
         <v>90</v>
       </c>
       <c r="D10" s="4" t="s">
@@ -2244,13 +2291,13 @@
   </sheetData>
   <phoneticPr fontId="1" type="noConversion"/>
   <conditionalFormatting sqref="D2:D10">
-    <cfRule type="expression" dxfId="2" priority="1">
+    <cfRule type="expression" dxfId="5" priority="1">
       <formula>D2="Easy"</formula>
     </cfRule>
-    <cfRule type="expression" dxfId="1" priority="2">
+    <cfRule type="expression" dxfId="4" priority="2">
       <formula>D2="Medium"</formula>
     </cfRule>
-    <cfRule type="expression" dxfId="0" priority="3">
+    <cfRule type="expression" dxfId="3" priority="3">
       <formula>D2="Hard"</formula>
     </cfRule>
   </conditionalFormatting>
@@ -2273,6 +2320,142 @@
 </worksheet>
 </file>
 
+<file path=xl/worksheets/sheet6.xml><?xml version="1.0" encoding="utf-8"?>
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{C287181F-E765-1C4E-B964-9C9FDBE62A17}">
+  <dimension ref="A1:K3"/>
+  <sheetViews>
+    <sheetView tabSelected="1" zoomScaleNormal="100" workbookViewId="0"/>
+  </sheetViews>
+  <sheetFormatPr baseColWidth="10" defaultColWidth="9" defaultRowHeight="17"/>
+  <cols>
+    <col min="1" max="1" width="11" customWidth="1"/>
+    <col min="2" max="2" width="36" customWidth="1"/>
+    <col min="3" max="3" width="35.796875" style="9" customWidth="1"/>
+    <col min="4" max="4" width="16" customWidth="1"/>
+    <col min="5" max="5" width="36" customWidth="1"/>
+    <col min="6" max="8" width="21" customWidth="1"/>
+    <col min="9" max="10" width="16" style="1" customWidth="1"/>
+    <col min="11" max="11" width="16" customWidth="1"/>
+  </cols>
+  <sheetData>
+    <row r="1" spans="1:11" ht="20" customHeight="1">
+      <c r="A1" s="2" t="s">
+        <v>4</v>
+      </c>
+      <c r="B1" s="2" t="s">
+        <v>0</v>
+      </c>
+      <c r="C1" s="2" t="s">
+        <v>1</v>
+      </c>
+      <c r="D1" s="2" t="s">
+        <v>2</v>
+      </c>
+      <c r="E1" s="2" t="s">
+        <v>30</v>
+      </c>
+      <c r="F1" s="2" t="s">
+        <v>22</v>
+      </c>
+      <c r="G1" s="2" t="s">
+        <v>5</v>
+      </c>
+      <c r="H1" s="2" t="s">
+        <v>6</v>
+      </c>
+      <c r="I1" s="3" t="s">
+        <v>8</v>
+      </c>
+      <c r="J1" s="3" t="s">
+        <v>7</v>
+      </c>
+      <c r="K1" s="2" t="s">
+        <v>3</v>
+      </c>
+    </row>
+    <row r="2" spans="1:11" ht="20" customHeight="1">
+      <c r="A2" s="4">
+        <v>113</v>
+      </c>
+      <c r="B2" s="4" t="s">
+        <v>92</v>
+      </c>
+      <c r="C2" s="8" t="s">
+        <v>94</v>
+      </c>
+      <c r="D2" s="4" t="s">
+        <v>49</v>
+      </c>
+      <c r="E2" s="4"/>
+      <c r="F2" s="4" t="s">
+        <v>96</v>
+      </c>
+      <c r="G2" s="4" t="s">
+        <v>44</v>
+      </c>
+      <c r="H2" s="4" t="s">
+        <v>44</v>
+      </c>
+      <c r="I2" s="5">
+        <v>45486</v>
+      </c>
+      <c r="J2" s="5"/>
+      <c r="K2" s="4"/>
+    </row>
+    <row r="3" spans="1:11" ht="20" customHeight="1">
+      <c r="A3" s="4">
+        <v>114</v>
+      </c>
+      <c r="B3" s="4" t="s">
+        <v>93</v>
+      </c>
+      <c r="C3" s="8" t="s">
+        <v>95</v>
+      </c>
+      <c r="D3" s="4" t="s">
+        <v>49</v>
+      </c>
+      <c r="E3" s="4"/>
+      <c r="F3" s="4" t="s">
+        <v>96</v>
+      </c>
+      <c r="G3" s="4" t="s">
+        <v>44</v>
+      </c>
+      <c r="H3" s="4" t="s">
+        <v>44</v>
+      </c>
+      <c r="I3" s="5">
+        <v>45486</v>
+      </c>
+      <c r="J3" s="5"/>
+      <c r="K3" s="4"/>
+    </row>
+  </sheetData>
+  <phoneticPr fontId="1" type="noConversion"/>
+  <conditionalFormatting sqref="D2:D3">
+    <cfRule type="expression" dxfId="2" priority="1">
+      <formula>D2="Easy"</formula>
+    </cfRule>
+    <cfRule type="expression" dxfId="1" priority="2">
+      <formula>D2="Medium"</formula>
+    </cfRule>
+    <cfRule type="expression" dxfId="0" priority="3">
+      <formula>D2="Hard"</formula>
+    </cfRule>
+  </conditionalFormatting>
+  <hyperlinks>
+    <hyperlink ref="C2" r:id="rId1" xr:uid="{6D7B591D-348C-3F48-8F5D-0CC1D7D323A3}"/>
+    <hyperlink ref="C3" r:id="rId2" xr:uid="{75408504-4022-5F46-87C2-C45DD0C84D7E}"/>
+  </hyperlinks>
+  <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
+  <pageSetup paperSize="9" orientation="portrait" verticalDpi="0" r:id="rId3"/>
+  <headerFooter>
+    <oddFooter>&amp;L_x000D_&amp;1#&amp;"Calibri"&amp;10&amp;K000000 General</oddFooter>
+  </headerFooter>
+</worksheet>
+</file>
+
 <file path=docMetadata/LabelInfo.xml><?xml version="1.0" encoding="utf-8"?>
 <clbl:labelList xmlns:clbl="http://schemas.microsoft.com/office/2020/mipLabelMetadata">
   <clbl:label id="{04d09258-035b-4e4f-ae3e-d79ff3d418d8}" enabled="1" method="Standard" siteId="{f4a12867-922d-4b9d-bb85-9ee7898512a0}" contentBits="2" removed="0"/>

</xml_diff>

<commit_message>
Completed some DFS practices.
</commit_message>
<xml_diff>
--- a/LeetCode Techniques.xlsx
+++ b/LeetCode Techniques.xlsx
@@ -8,7 +8,7 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="/Users/blackjack625/Desktop/LeetCode/"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{49444300-7889-7C45-BBE5-FAE34250899B}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{D077E055-E5FC-7042-AD27-E3A5ED77F8EF}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="0" yWindow="500" windowWidth="20640" windowHeight="11040" activeTab="5" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
@@ -19,6 +19,7 @@
     <sheet name="Recursion" sheetId="5" r:id="rId4"/>
     <sheet name="Trie" sheetId="4" r:id="rId5"/>
     <sheet name="Depth First Search" sheetId="6" r:id="rId6"/>
+    <sheet name="Breadth First Search" sheetId="7" r:id="rId7"/>
   </sheets>
   <calcPr calcId="191029"/>
   <extLst>
@@ -38,7 +39,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="239" uniqueCount="97">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="279" uniqueCount="109">
   <si>
     <t>Name</t>
   </si>
@@ -396,6 +397,54 @@
   </si>
   <si>
     <t>Linked List</t>
+    <phoneticPr fontId="1" type="noConversion"/>
+  </si>
+  <si>
+    <t>https://leetcode.com/problems/populating-next-right-pointers-in-each-node/</t>
+    <phoneticPr fontId="1" type="noConversion"/>
+  </si>
+  <si>
+    <t>Populating Next Right Pointers in Each Node</t>
+    <phoneticPr fontId="1" type="noConversion"/>
+  </si>
+  <si>
+    <t>Sum Root to Leaf Numbers</t>
+    <phoneticPr fontId="1" type="noConversion"/>
+  </si>
+  <si>
+    <t>https://leetcode.com/problems/sum-root-to-leaf-numbers/description/</t>
+    <phoneticPr fontId="1" type="noConversion"/>
+  </si>
+  <si>
+    <t>Flatten Nested List Iterator</t>
+    <phoneticPr fontId="1" type="noConversion"/>
+  </si>
+  <si>
+    <t>https://leetcode.com/problems/flatten-nested-list-iterator/description/</t>
+    <phoneticPr fontId="1" type="noConversion"/>
+  </si>
+  <si>
+    <t>Nested List</t>
+    <phoneticPr fontId="1" type="noConversion"/>
+  </si>
+  <si>
+    <t>Find Bottom Left Tree Value</t>
+    <phoneticPr fontId="1" type="noConversion"/>
+  </si>
+  <si>
+    <t>https://leetcode.com/problems/find-bottom-left-tree-value/description/</t>
+    <phoneticPr fontId="1" type="noConversion"/>
+  </si>
+  <si>
+    <t>Binary Tree</t>
+    <phoneticPr fontId="1" type="noConversion"/>
+  </si>
+  <si>
+    <t>Path Sum III</t>
+    <phoneticPr fontId="1" type="noConversion"/>
+  </si>
+  <si>
+    <t>https://leetcode.com/problems/path-sum-iii/description/</t>
     <phoneticPr fontId="1" type="noConversion"/>
   </si>
 </sst>
@@ -532,7 +581,37 @@
     <cellStyle name="一般" xfId="0" builtinId="0"/>
     <cellStyle name="超連結" xfId="1" builtinId="8"/>
   </cellStyles>
-  <dxfs count="24">
+  <dxfs count="27">
+    <dxf>
+      <font>
+        <color rgb="FFFFFF00"/>
+      </font>
+      <fill>
+        <patternFill>
+          <bgColor rgb="FFFF0000"/>
+        </patternFill>
+      </fill>
+    </dxf>
+    <dxf>
+      <font>
+        <color theme="1"/>
+      </font>
+      <fill>
+        <patternFill>
+          <bgColor rgb="FFFFFF00"/>
+        </patternFill>
+      </fill>
+    </dxf>
+    <dxf>
+      <font>
+        <color theme="0"/>
+      </font>
+      <fill>
+        <patternFill>
+          <bgColor rgb="FF00B050"/>
+        </patternFill>
+      </fill>
+    </dxf>
     <dxf>
       <font>
         <color rgb="FFFFFF00"/>
@@ -1524,24 +1603,24 @@
   </sortState>
   <phoneticPr fontId="1" type="noConversion"/>
   <conditionalFormatting sqref="D2:D3">
-    <cfRule type="expression" dxfId="23" priority="1">
+    <cfRule type="expression" dxfId="26" priority="1">
       <formula>D2="Easy"</formula>
     </cfRule>
-    <cfRule type="expression" dxfId="22" priority="2">
+    <cfRule type="expression" dxfId="25" priority="2">
       <formula>D2="Medium"</formula>
     </cfRule>
-    <cfRule type="expression" dxfId="21" priority="3">
+    <cfRule type="expression" dxfId="24" priority="3">
       <formula>D2="Hard"</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="D4:E15">
-    <cfRule type="expression" dxfId="20" priority="4">
+    <cfRule type="expression" dxfId="23" priority="4">
       <formula>D4="Easy"</formula>
     </cfRule>
-    <cfRule type="expression" dxfId="19" priority="5">
+    <cfRule type="expression" dxfId="22" priority="5">
       <formula>D4="Medium"</formula>
     </cfRule>
-    <cfRule type="expression" dxfId="18" priority="6">
+    <cfRule type="expression" dxfId="21" priority="6">
       <formula>D4="Hard"</formula>
     </cfRule>
   </conditionalFormatting>
@@ -1678,13 +1757,13 @@
   </sheetData>
   <phoneticPr fontId="1" type="noConversion"/>
   <conditionalFormatting sqref="D2:E3">
-    <cfRule type="expression" dxfId="17" priority="4">
+    <cfRule type="expression" dxfId="20" priority="4">
       <formula>D2="Easy"</formula>
     </cfRule>
-    <cfRule type="expression" dxfId="16" priority="5">
+    <cfRule type="expression" dxfId="19" priority="5">
       <formula>D2="Medium"</formula>
     </cfRule>
-    <cfRule type="expression" dxfId="15" priority="6">
+    <cfRule type="expression" dxfId="18" priority="6">
       <formula>D2="Hard"</formula>
     </cfRule>
   </conditionalFormatting>
@@ -1840,24 +1919,24 @@
   </sheetData>
   <phoneticPr fontId="1" type="noConversion"/>
   <conditionalFormatting sqref="D2">
-    <cfRule type="expression" dxfId="14" priority="1">
+    <cfRule type="expression" dxfId="17" priority="1">
       <formula>D2="Easy"</formula>
     </cfRule>
-    <cfRule type="expression" dxfId="13" priority="2">
+    <cfRule type="expression" dxfId="16" priority="2">
       <formula>D2="Medium"</formula>
     </cfRule>
-    <cfRule type="expression" dxfId="12" priority="3">
+    <cfRule type="expression" dxfId="15" priority="3">
       <formula>D2="Hard"</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="D3:E4">
-    <cfRule type="expression" dxfId="11" priority="4">
+    <cfRule type="expression" dxfId="14" priority="4">
       <formula>D3="Easy"</formula>
     </cfRule>
-    <cfRule type="expression" dxfId="10" priority="5">
+    <cfRule type="expression" dxfId="13" priority="5">
       <formula>D3="Medium"</formula>
     </cfRule>
-    <cfRule type="expression" dxfId="9" priority="6">
+    <cfRule type="expression" dxfId="12" priority="6">
       <formula>D3="Hard"</formula>
     </cfRule>
   </conditionalFormatting>
@@ -1957,13 +2036,13 @@
   </sheetData>
   <phoneticPr fontId="1" type="noConversion"/>
   <conditionalFormatting sqref="D2">
-    <cfRule type="expression" dxfId="8" priority="1">
+    <cfRule type="expression" dxfId="11" priority="1">
       <formula>D2="Easy"</formula>
     </cfRule>
-    <cfRule type="expression" dxfId="7" priority="2">
+    <cfRule type="expression" dxfId="10" priority="2">
       <formula>D2="Medium"</formula>
     </cfRule>
-    <cfRule type="expression" dxfId="6" priority="3">
+    <cfRule type="expression" dxfId="9" priority="3">
       <formula>D2="Hard"</formula>
     </cfRule>
   </conditionalFormatting>
@@ -2291,13 +2370,13 @@
   </sheetData>
   <phoneticPr fontId="1" type="noConversion"/>
   <conditionalFormatting sqref="D2:D10">
-    <cfRule type="expression" dxfId="5" priority="1">
+    <cfRule type="expression" dxfId="8" priority="1">
       <formula>D2="Easy"</formula>
     </cfRule>
-    <cfRule type="expression" dxfId="4" priority="2">
+    <cfRule type="expression" dxfId="7" priority="2">
       <formula>D2="Medium"</formula>
     </cfRule>
-    <cfRule type="expression" dxfId="3" priority="3">
+    <cfRule type="expression" dxfId="6" priority="3">
       <formula>D2="Hard"</formula>
     </cfRule>
   </conditionalFormatting>
@@ -2322,7 +2401,7 @@
 
 <file path=xl/worksheets/sheet6.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{C287181F-E765-1C4E-B964-9C9FDBE62A17}">
-  <dimension ref="A1:K3"/>
+  <dimension ref="A1:K7"/>
   <sheetViews>
     <sheetView tabSelected="1" zoomScaleNormal="100" workbookViewId="0"/>
   </sheetViews>
@@ -2431,9 +2510,234 @@
       <c r="J3" s="5"/>
       <c r="K3" s="4"/>
     </row>
+    <row r="4" spans="1:11" ht="20" customHeight="1">
+      <c r="A4" s="4">
+        <v>129</v>
+      </c>
+      <c r="B4" s="4" t="s">
+        <v>99</v>
+      </c>
+      <c r="C4" s="8" t="s">
+        <v>100</v>
+      </c>
+      <c r="D4" s="4" t="s">
+        <v>49</v>
+      </c>
+      <c r="E4" s="4"/>
+      <c r="F4" s="4" t="s">
+        <v>106</v>
+      </c>
+      <c r="G4" s="4" t="s">
+        <v>44</v>
+      </c>
+      <c r="H4" s="4" t="s">
+        <v>29</v>
+      </c>
+      <c r="I4" s="5">
+        <v>45487</v>
+      </c>
+      <c r="J4" s="5"/>
+      <c r="K4" s="4"/>
+    </row>
+    <row r="5" spans="1:11" ht="20" customHeight="1">
+      <c r="A5" s="4">
+        <v>341</v>
+      </c>
+      <c r="B5" s="4" t="s">
+        <v>101</v>
+      </c>
+      <c r="C5" s="8" t="s">
+        <v>102</v>
+      </c>
+      <c r="D5" s="4" t="s">
+        <v>49</v>
+      </c>
+      <c r="E5" s="4"/>
+      <c r="F5" s="4" t="s">
+        <v>103</v>
+      </c>
+      <c r="G5" s="4" t="s">
+        <v>44</v>
+      </c>
+      <c r="H5" s="4" t="s">
+        <v>44</v>
+      </c>
+      <c r="I5" s="5">
+        <v>45487</v>
+      </c>
+      <c r="J5" s="5"/>
+      <c r="K5" s="4"/>
+    </row>
+    <row r="6" spans="1:11" ht="20" customHeight="1">
+      <c r="A6" s="4">
+        <v>437</v>
+      </c>
+      <c r="B6" s="4" t="s">
+        <v>107</v>
+      </c>
+      <c r="C6" s="8" t="s">
+        <v>108</v>
+      </c>
+      <c r="D6" s="4" t="s">
+        <v>49</v>
+      </c>
+      <c r="E6" s="4"/>
+      <c r="F6" s="4" t="s">
+        <v>106</v>
+      </c>
+      <c r="G6" s="4" t="s">
+        <v>44</v>
+      </c>
+      <c r="H6" s="4" t="s">
+        <v>44</v>
+      </c>
+      <c r="I6" s="5">
+        <v>45487</v>
+      </c>
+      <c r="J6" s="5"/>
+      <c r="K6" s="4"/>
+    </row>
+    <row r="7" spans="1:11" ht="20" customHeight="1">
+      <c r="A7" s="4">
+        <v>513</v>
+      </c>
+      <c r="B7" s="4" t="s">
+        <v>104</v>
+      </c>
+      <c r="C7" s="8" t="s">
+        <v>105</v>
+      </c>
+      <c r="D7" s="4" t="s">
+        <v>49</v>
+      </c>
+      <c r="E7" s="4"/>
+      <c r="F7" s="4" t="s">
+        <v>106</v>
+      </c>
+      <c r="G7" s="4" t="s">
+        <v>44</v>
+      </c>
+      <c r="H7" s="4" t="s">
+        <v>29</v>
+      </c>
+      <c r="I7" s="5">
+        <v>45487</v>
+      </c>
+      <c r="J7" s="5"/>
+      <c r="K7" s="4"/>
+    </row>
   </sheetData>
   <phoneticPr fontId="1" type="noConversion"/>
-  <conditionalFormatting sqref="D2:D3">
+  <conditionalFormatting sqref="D2:D7">
+    <cfRule type="expression" dxfId="5" priority="1">
+      <formula>D2="Easy"</formula>
+    </cfRule>
+    <cfRule type="expression" dxfId="4" priority="2">
+      <formula>D2="Medium"</formula>
+    </cfRule>
+    <cfRule type="expression" dxfId="3" priority="3">
+      <formula>D2="Hard"</formula>
+    </cfRule>
+  </conditionalFormatting>
+  <hyperlinks>
+    <hyperlink ref="C2" r:id="rId1" xr:uid="{6D7B591D-348C-3F48-8F5D-0CC1D7D323A3}"/>
+    <hyperlink ref="C3" r:id="rId2" xr:uid="{75408504-4022-5F46-87C2-C45DD0C84D7E}"/>
+    <hyperlink ref="C4" r:id="rId3" xr:uid="{58EBA3C8-38C3-AD4D-86B6-2BD56DBBCDCD}"/>
+    <hyperlink ref="C5" r:id="rId4" xr:uid="{63AC3368-EC03-1949-9ACD-8B642757EADB}"/>
+    <hyperlink ref="C7" r:id="rId5" xr:uid="{2E17F9D2-5401-784D-B0AE-3D6983893C12}"/>
+    <hyperlink ref="C6" r:id="rId6" xr:uid="{5CC483BA-CBD2-634B-808B-DA60BB15872A}"/>
+  </hyperlinks>
+  <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
+  <pageSetup paperSize="9" orientation="portrait" verticalDpi="0" r:id="rId7"/>
+  <headerFooter>
+    <oddFooter>&amp;L_x000D_&amp;1#&amp;"Calibri"&amp;10&amp;K000000 General</oddFooter>
+  </headerFooter>
+</worksheet>
+</file>
+
+<file path=xl/worksheets/sheet7.xml><?xml version="1.0" encoding="utf-8"?>
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{75AC292A-7720-E145-9563-F6FD48AA33E3}">
+  <dimension ref="A1:K2"/>
+  <sheetViews>
+    <sheetView zoomScaleNormal="100" workbookViewId="0"/>
+  </sheetViews>
+  <sheetFormatPr baseColWidth="10" defaultColWidth="9" defaultRowHeight="17"/>
+  <cols>
+    <col min="1" max="1" width="11" customWidth="1"/>
+    <col min="2" max="2" width="36" customWidth="1"/>
+    <col min="3" max="3" width="35.796875" style="9" customWidth="1"/>
+    <col min="4" max="4" width="16" customWidth="1"/>
+    <col min="5" max="5" width="36" customWidth="1"/>
+    <col min="6" max="8" width="21" customWidth="1"/>
+    <col min="9" max="10" width="16" style="1" customWidth="1"/>
+    <col min="11" max="11" width="16" customWidth="1"/>
+  </cols>
+  <sheetData>
+    <row r="1" spans="1:11" ht="20" customHeight="1">
+      <c r="A1" s="2" t="s">
+        <v>4</v>
+      </c>
+      <c r="B1" s="2" t="s">
+        <v>0</v>
+      </c>
+      <c r="C1" s="2" t="s">
+        <v>1</v>
+      </c>
+      <c r="D1" s="2" t="s">
+        <v>2</v>
+      </c>
+      <c r="E1" s="2" t="s">
+        <v>30</v>
+      </c>
+      <c r="F1" s="2" t="s">
+        <v>22</v>
+      </c>
+      <c r="G1" s="2" t="s">
+        <v>5</v>
+      </c>
+      <c r="H1" s="2" t="s">
+        <v>6</v>
+      </c>
+      <c r="I1" s="3" t="s">
+        <v>8</v>
+      </c>
+      <c r="J1" s="3" t="s">
+        <v>7</v>
+      </c>
+      <c r="K1" s="2" t="s">
+        <v>3</v>
+      </c>
+    </row>
+    <row r="2" spans="1:11" ht="20" customHeight="1">
+      <c r="A2" s="4">
+        <v>116</v>
+      </c>
+      <c r="B2" s="4" t="s">
+        <v>98</v>
+      </c>
+      <c r="C2" s="8" t="s">
+        <v>97</v>
+      </c>
+      <c r="D2" s="4" t="s">
+        <v>49</v>
+      </c>
+      <c r="E2" s="4"/>
+      <c r="F2" s="4"/>
+      <c r="G2" s="4" t="s">
+        <v>44</v>
+      </c>
+      <c r="H2" s="4" t="s">
+        <v>44</v>
+      </c>
+      <c r="I2" s="5">
+        <v>45487</v>
+      </c>
+      <c r="J2" s="5"/>
+      <c r="K2" s="4"/>
+    </row>
+  </sheetData>
+  <phoneticPr fontId="1" type="noConversion"/>
+  <conditionalFormatting sqref="D2">
     <cfRule type="expression" dxfId="2" priority="1">
       <formula>D2="Easy"</formula>
     </cfRule>
@@ -2445,11 +2749,10 @@
     </cfRule>
   </conditionalFormatting>
   <hyperlinks>
-    <hyperlink ref="C2" r:id="rId1" xr:uid="{6D7B591D-348C-3F48-8F5D-0CC1D7D323A3}"/>
-    <hyperlink ref="C3" r:id="rId2" xr:uid="{75408504-4022-5F46-87C2-C45DD0C84D7E}"/>
+    <hyperlink ref="C2" r:id="rId1" xr:uid="{13210F83-F6EB-B544-ABBA-8F955E2F9194}"/>
   </hyperlinks>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
-  <pageSetup paperSize="9" orientation="portrait" verticalDpi="0" r:id="rId3"/>
+  <pageSetup paperSize="9" orientation="portrait" verticalDpi="0" r:id="rId2"/>
   <headerFooter>
     <oddFooter>&amp;L_x000D_&amp;1#&amp;"Calibri"&amp;10&amp;K000000 General</oddFooter>
   </headerFooter>

</xml_diff>

<commit_message>
Completed unique value path.
</commit_message>
<xml_diff>
--- a/LeetCode Techniques.xlsx
+++ b/LeetCode Techniques.xlsx
@@ -8,7 +8,7 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="/Users/blackjack625/Desktop/LeetCode/"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{3B1F16C6-CA04-5F43-A0A1-8BC8A7819605}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{05703622-093F-5D45-8EA5-7796245C69F1}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="0" yWindow="500" windowWidth="20640" windowHeight="11040" activeTab="5" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
@@ -39,7 +39,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="285" uniqueCount="111">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="311" uniqueCount="121">
   <si>
     <t>Name</t>
   </si>
@@ -453,6 +453,48 @@
   </si>
   <si>
     <t>https://leetcode.com/problems/most-frequent-subtree-sum/description/</t>
+    <phoneticPr fontId="1" type="noConversion"/>
+  </si>
+  <si>
+    <t>Find Largest Value in Each Tree Row</t>
+    <phoneticPr fontId="1" type="noConversion"/>
+  </si>
+  <si>
+    <t>https://leetcode.com/problems/find-largest-value-in-each-tree-row/description/</t>
+    <phoneticPr fontId="1" type="noConversion"/>
+  </si>
+  <si>
+    <t>Add One Row to Tree</t>
+    <phoneticPr fontId="1" type="noConversion"/>
+  </si>
+  <si>
+    <t>https://leetcode.com/problems/add-one-row-to-tree/description/</t>
+    <phoneticPr fontId="1" type="noConversion"/>
+  </si>
+  <si>
+    <t>Find Duplicate Subtrees</t>
+    <phoneticPr fontId="1" type="noConversion"/>
+  </si>
+  <si>
+    <t>https://leetcode.com/problems/find-duplicate-subtrees/description/</t>
+    <phoneticPr fontId="1" type="noConversion"/>
+  </si>
+  <si>
+    <t>When marking null child nodes,
+use a slash to help denote left or right.</t>
+    <phoneticPr fontId="1" type="noConversion"/>
+  </si>
+  <si>
+    <t>Longest Univalue Path</t>
+    <phoneticPr fontId="1" type="noConversion"/>
+  </si>
+  <si>
+    <t>https://leetcode.com/problems/longest-univalue-path/description/</t>
+    <phoneticPr fontId="1" type="noConversion"/>
+  </si>
+  <si>
+    <t>Beware of "semi-cycles" in longest 
+univalue paths.</t>
     <phoneticPr fontId="1" type="noConversion"/>
   </si>
 </sst>
@@ -2409,7 +2451,7 @@
 
 <file path=xl/worksheets/sheet6.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{C287181F-E765-1C4E-B964-9C9FDBE62A17}">
-  <dimension ref="A1:K8"/>
+  <dimension ref="A1:K12"/>
   <sheetViews>
     <sheetView tabSelected="1" zoomScaleNormal="100" workbookViewId="0"/>
   </sheetViews>
@@ -2663,9 +2705,129 @@
       <c r="J8" s="5"/>
       <c r="K8" s="4"/>
     </row>
+    <row r="9" spans="1:11" ht="20" customHeight="1">
+      <c r="A9" s="4">
+        <v>515</v>
+      </c>
+      <c r="B9" s="4" t="s">
+        <v>111</v>
+      </c>
+      <c r="C9" s="8" t="s">
+        <v>112</v>
+      </c>
+      <c r="D9" s="4" t="s">
+        <v>49</v>
+      </c>
+      <c r="E9" s="4"/>
+      <c r="F9" s="4" t="s">
+        <v>106</v>
+      </c>
+      <c r="G9" s="4" t="s">
+        <v>44</v>
+      </c>
+      <c r="H9" s="4" t="s">
+        <v>14</v>
+      </c>
+      <c r="I9" s="5">
+        <v>45488</v>
+      </c>
+      <c r="J9" s="5"/>
+      <c r="K9" s="4"/>
+    </row>
+    <row r="10" spans="1:11" ht="20" customHeight="1">
+      <c r="A10" s="4">
+        <v>623</v>
+      </c>
+      <c r="B10" s="4" t="s">
+        <v>113</v>
+      </c>
+      <c r="C10" s="8" t="s">
+        <v>114</v>
+      </c>
+      <c r="D10" s="4" t="s">
+        <v>49</v>
+      </c>
+      <c r="E10" s="4"/>
+      <c r="F10" s="4" t="s">
+        <v>106</v>
+      </c>
+      <c r="G10" s="4" t="s">
+        <v>44</v>
+      </c>
+      <c r="H10" s="4" t="s">
+        <v>29</v>
+      </c>
+      <c r="I10" s="5">
+        <v>45488</v>
+      </c>
+      <c r="J10" s="5"/>
+      <c r="K10" s="4"/>
+    </row>
+    <row r="11" spans="1:11" ht="30" customHeight="1">
+      <c r="A11" s="4">
+        <v>652</v>
+      </c>
+      <c r="B11" s="4" t="s">
+        <v>115</v>
+      </c>
+      <c r="C11" s="8" t="s">
+        <v>116</v>
+      </c>
+      <c r="D11" s="4" t="s">
+        <v>49</v>
+      </c>
+      <c r="E11" s="6" t="s">
+        <v>117</v>
+      </c>
+      <c r="F11" s="4" t="s">
+        <v>106</v>
+      </c>
+      <c r="G11" s="4" t="s">
+        <v>44</v>
+      </c>
+      <c r="H11" s="4" t="s">
+        <v>44</v>
+      </c>
+      <c r="I11" s="5">
+        <v>45488</v>
+      </c>
+      <c r="J11" s="5"/>
+      <c r="K11" s="4"/>
+    </row>
+    <row r="12" spans="1:11" ht="30" customHeight="1">
+      <c r="A12" s="4">
+        <v>687</v>
+      </c>
+      <c r="B12" s="4" t="s">
+        <v>118</v>
+      </c>
+      <c r="C12" s="8" t="s">
+        <v>119</v>
+      </c>
+      <c r="D12" s="4" t="s">
+        <v>49</v>
+      </c>
+      <c r="E12" s="6" t="s">
+        <v>120</v>
+      </c>
+      <c r="F12" s="4" t="s">
+        <v>106</v>
+      </c>
+      <c r="G12" s="4" t="s">
+        <v>44</v>
+      </c>
+      <c r="H12" s="4" t="s">
+        <v>29</v>
+      </c>
+      <c r="I12" s="5">
+        <v>45488</v>
+      </c>
+      <c r="J12" s="5"/>
+      <c r="K12" s="4"/>
+    </row>
   </sheetData>
   <phoneticPr fontId="1" type="noConversion"/>
-  <conditionalFormatting sqref="D2:D8">
+  <conditionalFormatting sqref="D2:D12">
     <cfRule type="expression" dxfId="5" priority="1">
       <formula>D2="Easy"</formula>
     </cfRule>
@@ -2684,9 +2846,13 @@
     <hyperlink ref="C8" r:id="rId5" xr:uid="{2E17F9D2-5401-784D-B0AE-3D6983893C12}"/>
     <hyperlink ref="C6" r:id="rId6" xr:uid="{5CC483BA-CBD2-634B-808B-DA60BB15872A}"/>
     <hyperlink ref="C7" r:id="rId7" xr:uid="{3C24C6AF-34E6-D142-95AA-D541F8679AD8}"/>
+    <hyperlink ref="C9" r:id="rId8" xr:uid="{8EE9509C-DFBF-7B45-85D3-B7096029C524}"/>
+    <hyperlink ref="C10" r:id="rId9" xr:uid="{DC0AB236-A846-624D-8598-9984C67224C0}"/>
+    <hyperlink ref="C11" r:id="rId10" xr:uid="{92D47051-6BA8-D549-944F-00B0154554E6}"/>
+    <hyperlink ref="C12" r:id="rId11" xr:uid="{CBAD603C-7336-874C-B3F7-58227D327CE0}"/>
   </hyperlinks>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
-  <pageSetup paperSize="9" orientation="portrait" verticalDpi="0" r:id="rId8"/>
+  <pageSetup paperSize="9" orientation="portrait" verticalDpi="0" r:id="rId12"/>
   <headerFooter>
     <oddFooter>&amp;L_x000D_&amp;1#&amp;"Calibri"&amp;10&amp;K000000 General</oddFooter>
   </headerFooter>

</xml_diff>

<commit_message>
Completed some BFS practices.
</commit_message>
<xml_diff>
--- a/LeetCode Techniques.xlsx
+++ b/LeetCode Techniques.xlsx
@@ -8,7 +8,7 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\jack.yao\Desktop\LeetCode\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{C91C00D4-085B-47A4-ACD1-F82078E79D8B}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{35CC21E4-04BF-413C-8152-F663C1057A0F}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="-120" yWindow="-120" windowWidth="20640" windowHeight="11040" firstSheet="1" activeTab="6" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
@@ -39,7 +39,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="320" uniqueCount="125">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="334" uniqueCount="130">
   <si>
     <t>Name</t>
   </si>
@@ -509,6 +509,22 @@
   <si>
     <t>Use a deck to ensure queue
 always has nodes of same level.</t>
+  </si>
+  <si>
+    <t>If needed, use .copy() to prevent
+storage modification during iteration.</t>
+  </si>
+  <si>
+    <t>Binary Tree Level Order Traversal</t>
+  </si>
+  <si>
+    <t>https://leetcode.com/problems/binary-tree-level-order-traversal/description/</t>
+  </si>
+  <si>
+    <t xml:space="preserve">	Binary Tree Level Order Traversal II</t>
+  </si>
+  <si>
+    <t>https://leetcode.com/problems/binary-tree-level-order-traversal-ii/description/</t>
   </si>
 </sst>
 </file>
@@ -2877,7 +2893,7 @@
 
 <file path=xl/worksheets/sheet7.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{75AC292A-7720-E145-9563-F6FD48AA33E3}">
-  <dimension ref="A1:K3"/>
+  <dimension ref="A1:K5"/>
   <sheetViews>
     <sheetView tabSelected="1" zoomScaleNormal="100" workbookViewId="0"/>
   </sheetViews>
@@ -2930,19 +2946,19 @@
     </row>
     <row r="2" spans="1:11" ht="30" customHeight="1">
       <c r="A2" s="4">
-        <v>116</v>
+        <v>102</v>
       </c>
       <c r="B2" s="4" t="s">
-        <v>98</v>
-      </c>
-      <c r="C2" s="8" t="s">
-        <v>97</v>
+        <v>126</v>
+      </c>
+      <c r="C2" s="10" t="s">
+        <v>127</v>
       </c>
       <c r="D2" s="4" t="s">
         <v>49</v>
       </c>
       <c r="E2" s="6" t="s">
-        <v>124</v>
+        <v>125</v>
       </c>
       <c r="F2" s="4" t="s">
         <v>123</v>
@@ -2954,26 +2970,26 @@
         <v>44</v>
       </c>
       <c r="I2" s="5">
-        <v>45487</v>
+        <v>45489</v>
       </c>
       <c r="J2" s="5"/>
       <c r="K2" s="4"/>
     </row>
     <row r="3" spans="1:11" ht="30" customHeight="1">
       <c r="A3" s="4">
-        <v>117</v>
-      </c>
-      <c r="B3" s="4" t="s">
-        <v>121</v>
+        <v>107</v>
+      </c>
+      <c r="B3" s="6" t="s">
+        <v>128</v>
       </c>
       <c r="C3" s="10" t="s">
-        <v>122</v>
+        <v>129</v>
       </c>
       <c r="D3" s="4" t="s">
         <v>49</v>
       </c>
       <c r="E3" s="6" t="s">
-        <v>124</v>
+        <v>125</v>
       </c>
       <c r="F3" s="4" t="s">
         <v>123</v>
@@ -2990,9 +3006,71 @@
       <c r="J3" s="5"/>
       <c r="K3" s="4"/>
     </row>
+    <row r="4" spans="1:11" ht="30" customHeight="1">
+      <c r="A4" s="4">
+        <v>116</v>
+      </c>
+      <c r="B4" s="4" t="s">
+        <v>98</v>
+      </c>
+      <c r="C4" s="8" t="s">
+        <v>97</v>
+      </c>
+      <c r="D4" s="4" t="s">
+        <v>49</v>
+      </c>
+      <c r="E4" s="6" t="s">
+        <v>124</v>
+      </c>
+      <c r="F4" s="4" t="s">
+        <v>123</v>
+      </c>
+      <c r="G4" s="4" t="s">
+        <v>44</v>
+      </c>
+      <c r="H4" s="4" t="s">
+        <v>44</v>
+      </c>
+      <c r="I4" s="5">
+        <v>45487</v>
+      </c>
+      <c r="J4" s="5"/>
+      <c r="K4" s="4"/>
+    </row>
+    <row r="5" spans="1:11" ht="30" customHeight="1">
+      <c r="A5" s="4">
+        <v>117</v>
+      </c>
+      <c r="B5" s="4" t="s">
+        <v>121</v>
+      </c>
+      <c r="C5" s="10" t="s">
+        <v>122</v>
+      </c>
+      <c r="D5" s="4" t="s">
+        <v>49</v>
+      </c>
+      <c r="E5" s="6" t="s">
+        <v>124</v>
+      </c>
+      <c r="F5" s="4" t="s">
+        <v>123</v>
+      </c>
+      <c r="G5" s="4" t="s">
+        <v>44</v>
+      </c>
+      <c r="H5" s="4" t="s">
+        <v>44</v>
+      </c>
+      <c r="I5" s="5">
+        <v>45489</v>
+      </c>
+      <c r="J5" s="5"/>
+      <c r="K5" s="4"/>
+    </row>
   </sheetData>
   <phoneticPr fontId="1" type="noConversion"/>
-  <conditionalFormatting sqref="D2:D3">
+  <conditionalFormatting sqref="D2:D5">
     <cfRule type="expression" dxfId="2" priority="1">
       <formula>D2="Easy"</formula>
     </cfRule>
@@ -3004,11 +3082,13 @@
     </cfRule>
   </conditionalFormatting>
   <hyperlinks>
-    <hyperlink ref="C2" r:id="rId1" xr:uid="{13210F83-F6EB-B544-ABBA-8F955E2F9194}"/>
-    <hyperlink ref="C3" r:id="rId2" xr:uid="{8BC7B711-ADEB-4546-905F-7D690999B5BB}"/>
+    <hyperlink ref="C4" r:id="rId1" xr:uid="{13210F83-F6EB-B544-ABBA-8F955E2F9194}"/>
+    <hyperlink ref="C5" r:id="rId2" xr:uid="{8BC7B711-ADEB-4546-905F-7D690999B5BB}"/>
+    <hyperlink ref="C2" r:id="rId3" xr:uid="{C2B4A6B6-B0D8-4F31-9802-387F04CC45FB}"/>
+    <hyperlink ref="C3" r:id="rId4" xr:uid="{5615EAD9-62C1-4780-AE19-6BFAC2939521}"/>
   </hyperlinks>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
-  <pageSetup paperSize="9" orientation="portrait" verticalDpi="0" r:id="rId3"/>
+  <pageSetup paperSize="9" orientation="portrait" verticalDpi="0" r:id="rId5"/>
   <headerFooter>
     <oddFooter>&amp;L_x000D_&amp;1#&amp;"Calibri"&amp;10&amp;K000000 General</oddFooter>
   </headerFooter>

</xml_diff>

<commit_message>
Completed some DFS & BFS practices.
</commit_message>
<xml_diff>
--- a/LeetCode Techniques.xlsx
+++ b/LeetCode Techniques.xlsx
@@ -8,9 +8,9 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\jack.yao\Desktop\LeetCode\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{35CC21E4-04BF-413C-8152-F663C1057A0F}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{B44FC48D-9B2B-4385-8134-5E6946714FFA}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="-120" yWindow="-120" windowWidth="20640" windowHeight="11040" firstSheet="1" activeTab="6" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
+    <workbookView xWindow="-120" yWindow="-120" windowWidth="20640" windowHeight="11040" firstSheet="1" activeTab="5" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
   <sheets>
     <sheet name="Binary Search" sheetId="1" r:id="rId1"/>
@@ -39,7 +39,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="334" uniqueCount="130">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="348" uniqueCount="137">
   <si>
     <t>Name</t>
   </si>
@@ -525,6 +525,28 @@
   </si>
   <si>
     <t>https://leetcode.com/problems/binary-tree-level-order-traversal-ii/description/</t>
+  </si>
+  <si>
+    <t>Maximum Width of Binary Tree</t>
+  </si>
+  <si>
+    <t>https://leetcode.com/problems/maximum-width-of-binary-tree/</t>
+  </si>
+  <si>
+    <t>Use parent &amp; children indices
+relationship to efficiently compute width.</t>
+  </si>
+  <si>
+    <t>Evaluate Division</t>
+  </si>
+  <si>
+    <t>https://leetcode.com/problems/evaluate-division/description/</t>
+  </si>
+  <si>
+    <t>Use dict to build graph and trace nodes.</t>
+  </si>
+  <si>
+    <t>Graph</t>
   </si>
 </sst>
 </file>
@@ -534,7 +556,7 @@
   <numFmts count="1">
     <numFmt numFmtId="164" formatCode="yyyy&quot;年&quot;m&quot;月&quot;d&quot;日&quot;;@"/>
   </numFmts>
-  <fonts count="8">
+  <fonts count="11">
     <font>
       <sz val="11"/>
       <color theme="1"/>
@@ -593,6 +615,23 @@
       <family val="2"/>
       <charset val="134"/>
     </font>
+    <font>
+      <b/>
+      <sz val="10"/>
+      <color theme="1"/>
+      <name val="Microsoft YaHei"/>
+    </font>
+    <font>
+      <u/>
+      <sz val="10"/>
+      <color theme="10"/>
+      <name val="Microsoft YaHei"/>
+    </font>
+    <font>
+      <sz val="10"/>
+      <color theme="1"/>
+      <name val="Microsoft YaHei"/>
+    </font>
   </fonts>
   <fills count="2">
     <fill>
@@ -630,7 +669,7 @@
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
     <xf numFmtId="0" fontId="4" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
   </cellStyleXfs>
-  <cellXfs count="11">
+  <cellXfs count="13">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="164" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1"/>
     <xf numFmtId="0" fontId="2" fillId="0" borderId="1" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
@@ -655,9 +694,13 @@
       <alignment horizontal="center" vertical="center"/>
     </xf>
     <xf numFmtId="0" fontId="7" fillId="0" borderId="0" xfId="0" applyFont="1"/>
-    <xf numFmtId="0" fontId="4" fillId="0" borderId="1" xfId="1" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="8" fillId="0" borderId="1" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
     </xf>
+    <xf numFmtId="0" fontId="9" fillId="0" borderId="1" xfId="1" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="10" fillId="0" borderId="0" xfId="0" applyFont="1"/>
   </cellXfs>
   <cellStyles count="2">
     <cellStyle name="Hyperlink" xfId="1" builtinId="8"/>
@@ -2483,15 +2526,15 @@
 
 <file path=xl/worksheets/sheet6.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{C287181F-E765-1C4E-B964-9C9FDBE62A17}">
-  <dimension ref="A1:K12"/>
+  <dimension ref="A1:K13"/>
   <sheetViews>
-    <sheetView zoomScaleNormal="100" workbookViewId="0"/>
+    <sheetView tabSelected="1" zoomScaleNormal="100" workbookViewId="0"/>
   </sheetViews>
   <sheetFormatPr defaultColWidth="9" defaultRowHeight="16.5"/>
   <cols>
     <col min="1" max="1" width="11" customWidth="1"/>
     <col min="2" max="2" width="36" customWidth="1"/>
-    <col min="3" max="3" width="35.85546875" style="9" customWidth="1"/>
+    <col min="3" max="3" width="35.85546875" style="12" customWidth="1"/>
     <col min="4" max="4" width="16" customWidth="1"/>
     <col min="5" max="5" width="36" customWidth="1"/>
     <col min="6" max="8" width="21" customWidth="1"/>
@@ -2506,7 +2549,7 @@
       <c r="B1" s="2" t="s">
         <v>0</v>
       </c>
-      <c r="C1" s="2" t="s">
+      <c r="C1" s="10" t="s">
         <v>1</v>
       </c>
       <c r="D1" s="2" t="s">
@@ -2541,7 +2584,7 @@
       <c r="B2" s="4" t="s">
         <v>92</v>
       </c>
-      <c r="C2" s="8" t="s">
+      <c r="C2" s="11" t="s">
         <v>94</v>
       </c>
       <c r="D2" s="4" t="s">
@@ -2570,7 +2613,7 @@
       <c r="B3" s="4" t="s">
         <v>93</v>
       </c>
-      <c r="C3" s="8" t="s">
+      <c r="C3" s="11" t="s">
         <v>95</v>
       </c>
       <c r="D3" s="4" t="s">
@@ -2599,7 +2642,7 @@
       <c r="B4" s="4" t="s">
         <v>99</v>
       </c>
-      <c r="C4" s="8" t="s">
+      <c r="C4" s="11" t="s">
         <v>100</v>
       </c>
       <c r="D4" s="4" t="s">
@@ -2628,7 +2671,7 @@
       <c r="B5" s="4" t="s">
         <v>101</v>
       </c>
-      <c r="C5" s="8" t="s">
+      <c r="C5" s="11" t="s">
         <v>102</v>
       </c>
       <c r="D5" s="4" t="s">
@@ -2652,20 +2695,22 @@
     </row>
     <row r="6" spans="1:11" ht="20.100000000000001" customHeight="1">
       <c r="A6" s="4">
-        <v>437</v>
+        <v>399</v>
       </c>
       <c r="B6" s="4" t="s">
-        <v>107</v>
-      </c>
-      <c r="C6" s="8" t="s">
-        <v>108</v>
+        <v>133</v>
+      </c>
+      <c r="C6" s="11" t="s">
+        <v>134</v>
       </c>
       <c r="D6" s="4" t="s">
         <v>49</v>
       </c>
-      <c r="E6" s="4"/>
+      <c r="E6" s="4" t="s">
+        <v>135</v>
+      </c>
       <c r="F6" s="4" t="s">
-        <v>106</v>
+        <v>136</v>
       </c>
       <c r="G6" s="4" t="s">
         <v>44</v>
@@ -2674,20 +2719,20 @@
         <v>44</v>
       </c>
       <c r="I6" s="5">
-        <v>45487</v>
+        <v>45490</v>
       </c>
       <c r="J6" s="5"/>
       <c r="K6" s="4"/>
     </row>
     <row r="7" spans="1:11" ht="20.100000000000001" customHeight="1">
       <c r="A7" s="4">
-        <v>508</v>
+        <v>437</v>
       </c>
       <c r="B7" s="4" t="s">
-        <v>109</v>
-      </c>
-      <c r="C7" s="8" t="s">
-        <v>110</v>
+        <v>107</v>
+      </c>
+      <c r="C7" s="11" t="s">
+        <v>108</v>
       </c>
       <c r="D7" s="4" t="s">
         <v>49</v>
@@ -2710,13 +2755,13 @@
     </row>
     <row r="8" spans="1:11" ht="20.100000000000001" customHeight="1">
       <c r="A8" s="4">
-        <v>513</v>
+        <v>508</v>
       </c>
       <c r="B8" s="4" t="s">
-        <v>104</v>
-      </c>
-      <c r="C8" s="8" t="s">
-        <v>105</v>
+        <v>109</v>
+      </c>
+      <c r="C8" s="11" t="s">
+        <v>110</v>
       </c>
       <c r="D8" s="4" t="s">
         <v>49</v>
@@ -2729,7 +2774,7 @@
         <v>44</v>
       </c>
       <c r="H8" s="4" t="s">
-        <v>29</v>
+        <v>44</v>
       </c>
       <c r="I8" s="5">
         <v>45487</v>
@@ -2739,13 +2784,13 @@
     </row>
     <row r="9" spans="1:11" ht="20.100000000000001" customHeight="1">
       <c r="A9" s="4">
-        <v>515</v>
+        <v>513</v>
       </c>
       <c r="B9" s="4" t="s">
-        <v>111</v>
-      </c>
-      <c r="C9" s="8" t="s">
-        <v>112</v>
+        <v>104</v>
+      </c>
+      <c r="C9" s="11" t="s">
+        <v>105</v>
       </c>
       <c r="D9" s="4" t="s">
         <v>49</v>
@@ -2758,23 +2803,23 @@
         <v>44</v>
       </c>
       <c r="H9" s="4" t="s">
-        <v>14</v>
+        <v>29</v>
       </c>
       <c r="I9" s="5">
-        <v>45488</v>
+        <v>45487</v>
       </c>
       <c r="J9" s="5"/>
       <c r="K9" s="4"/>
     </row>
     <row r="10" spans="1:11" ht="20.100000000000001" customHeight="1">
       <c r="A10" s="4">
-        <v>623</v>
+        <v>515</v>
       </c>
       <c r="B10" s="4" t="s">
-        <v>113</v>
-      </c>
-      <c r="C10" s="8" t="s">
-        <v>114</v>
+        <v>111</v>
+      </c>
+      <c r="C10" s="11" t="s">
+        <v>112</v>
       </c>
       <c r="D10" s="4" t="s">
         <v>49</v>
@@ -2787,7 +2832,7 @@
         <v>44</v>
       </c>
       <c r="H10" s="4" t="s">
-        <v>29</v>
+        <v>14</v>
       </c>
       <c r="I10" s="5">
         <v>45488</v>
@@ -2795,22 +2840,20 @@
       <c r="J10" s="5"/>
       <c r="K10" s="4"/>
     </row>
-    <row r="11" spans="1:11" ht="30" customHeight="1">
+    <row r="11" spans="1:11" ht="20.100000000000001" customHeight="1">
       <c r="A11" s="4">
-        <v>652</v>
+        <v>623</v>
       </c>
       <c r="B11" s="4" t="s">
-        <v>115</v>
-      </c>
-      <c r="C11" s="8" t="s">
-        <v>116</v>
+        <v>113</v>
+      </c>
+      <c r="C11" s="11" t="s">
+        <v>114</v>
       </c>
       <c r="D11" s="4" t="s">
         <v>49</v>
       </c>
-      <c r="E11" s="6" t="s">
-        <v>117</v>
-      </c>
+      <c r="E11" s="4"/>
       <c r="F11" s="4" t="s">
         <v>106</v>
       </c>
@@ -2818,7 +2861,7 @@
         <v>44</v>
       </c>
       <c r="H11" s="4" t="s">
-        <v>44</v>
+        <v>29</v>
       </c>
       <c r="I11" s="5">
         <v>45488</v>
@@ -2828,19 +2871,19 @@
     </row>
     <row r="12" spans="1:11" ht="30" customHeight="1">
       <c r="A12" s="4">
-        <v>687</v>
+        <v>652</v>
       </c>
       <c r="B12" s="4" t="s">
-        <v>118</v>
-      </c>
-      <c r="C12" s="8" t="s">
-        <v>119</v>
+        <v>115</v>
+      </c>
+      <c r="C12" s="11" t="s">
+        <v>116</v>
       </c>
       <c r="D12" s="4" t="s">
         <v>49</v>
       </c>
       <c r="E12" s="6" t="s">
-        <v>120</v>
+        <v>117</v>
       </c>
       <c r="F12" s="4" t="s">
         <v>106</v>
@@ -2849,7 +2892,7 @@
         <v>44</v>
       </c>
       <c r="H12" s="4" t="s">
-        <v>29</v>
+        <v>44</v>
       </c>
       <c r="I12" s="5">
         <v>45488</v>
@@ -2857,9 +2900,40 @@
       <c r="J12" s="5"/>
       <c r="K12" s="4"/>
     </row>
+    <row r="13" spans="1:11" ht="30" customHeight="1">
+      <c r="A13" s="4">
+        <v>687</v>
+      </c>
+      <c r="B13" s="4" t="s">
+        <v>118</v>
+      </c>
+      <c r="C13" s="11" t="s">
+        <v>119</v>
+      </c>
+      <c r="D13" s="4" t="s">
+        <v>49</v>
+      </c>
+      <c r="E13" s="6" t="s">
+        <v>120</v>
+      </c>
+      <c r="F13" s="4" t="s">
+        <v>106</v>
+      </c>
+      <c r="G13" s="4" t="s">
+        <v>44</v>
+      </c>
+      <c r="H13" s="4" t="s">
+        <v>29</v>
+      </c>
+      <c r="I13" s="5">
+        <v>45488</v>
+      </c>
+      <c r="J13" s="5"/>
+      <c r="K13" s="4"/>
+    </row>
   </sheetData>
   <phoneticPr fontId="1" type="noConversion"/>
-  <conditionalFormatting sqref="D2:D12">
+  <conditionalFormatting sqref="D2:D13">
     <cfRule type="expression" dxfId="5" priority="1">
       <formula>D2="Easy"</formula>
     </cfRule>
@@ -2875,16 +2949,17 @@
     <hyperlink ref="C3" r:id="rId2" xr:uid="{75408504-4022-5F46-87C2-C45DD0C84D7E}"/>
     <hyperlink ref="C4" r:id="rId3" xr:uid="{58EBA3C8-38C3-AD4D-86B6-2BD56DBBCDCD}"/>
     <hyperlink ref="C5" r:id="rId4" xr:uid="{63AC3368-EC03-1949-9ACD-8B642757EADB}"/>
-    <hyperlink ref="C8" r:id="rId5" xr:uid="{2E17F9D2-5401-784D-B0AE-3D6983893C12}"/>
-    <hyperlink ref="C6" r:id="rId6" xr:uid="{5CC483BA-CBD2-634B-808B-DA60BB15872A}"/>
-    <hyperlink ref="C7" r:id="rId7" xr:uid="{3C24C6AF-34E6-D142-95AA-D541F8679AD8}"/>
-    <hyperlink ref="C9" r:id="rId8" xr:uid="{8EE9509C-DFBF-7B45-85D3-B7096029C524}"/>
-    <hyperlink ref="C10" r:id="rId9" xr:uid="{DC0AB236-A846-624D-8598-9984C67224C0}"/>
-    <hyperlink ref="C11" r:id="rId10" xr:uid="{92D47051-6BA8-D549-944F-00B0154554E6}"/>
-    <hyperlink ref="C12" r:id="rId11" xr:uid="{CBAD603C-7336-874C-B3F7-58227D327CE0}"/>
+    <hyperlink ref="C9" r:id="rId5" xr:uid="{2E17F9D2-5401-784D-B0AE-3D6983893C12}"/>
+    <hyperlink ref="C7" r:id="rId6" xr:uid="{5CC483BA-CBD2-634B-808B-DA60BB15872A}"/>
+    <hyperlink ref="C8" r:id="rId7" xr:uid="{3C24C6AF-34E6-D142-95AA-D541F8679AD8}"/>
+    <hyperlink ref="C10" r:id="rId8" xr:uid="{8EE9509C-DFBF-7B45-85D3-B7096029C524}"/>
+    <hyperlink ref="C11" r:id="rId9" xr:uid="{DC0AB236-A846-624D-8598-9984C67224C0}"/>
+    <hyperlink ref="C12" r:id="rId10" xr:uid="{92D47051-6BA8-D549-944F-00B0154554E6}"/>
+    <hyperlink ref="C13" r:id="rId11" xr:uid="{CBAD603C-7336-874C-B3F7-58227D327CE0}"/>
+    <hyperlink ref="C6" r:id="rId12" xr:uid="{98CD3759-6763-4A59-8FC7-20CD817AC0B4}"/>
   </hyperlinks>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
-  <pageSetup paperSize="9" orientation="portrait" verticalDpi="0" r:id="rId12"/>
+  <pageSetup paperSize="9" orientation="portrait" verticalDpi="0" r:id="rId13"/>
   <headerFooter>
     <oddFooter>&amp;L_x000D_&amp;1#&amp;"Calibri"&amp;10&amp;K000000 General</oddFooter>
   </headerFooter>
@@ -2893,9 +2968,9 @@
 
 <file path=xl/worksheets/sheet7.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{75AC292A-7720-E145-9563-F6FD48AA33E3}">
-  <dimension ref="A1:K5"/>
+  <dimension ref="A1:K6"/>
   <sheetViews>
-    <sheetView tabSelected="1" zoomScaleNormal="100" workbookViewId="0"/>
+    <sheetView zoomScaleNormal="100" workbookViewId="0"/>
   </sheetViews>
   <sheetFormatPr defaultColWidth="9" defaultRowHeight="16.5"/>
   <cols>
@@ -2916,7 +2991,7 @@
       <c r="B1" s="2" t="s">
         <v>0</v>
       </c>
-      <c r="C1" s="2" t="s">
+      <c r="C1" s="10" t="s">
         <v>1</v>
       </c>
       <c r="D1" s="2" t="s">
@@ -2951,7 +3026,7 @@
       <c r="B2" s="4" t="s">
         <v>126</v>
       </c>
-      <c r="C2" s="10" t="s">
+      <c r="C2" s="11" t="s">
         <v>127</v>
       </c>
       <c r="D2" s="4" t="s">
@@ -2982,7 +3057,7 @@
       <c r="B3" s="6" t="s">
         <v>128</v>
       </c>
-      <c r="C3" s="10" t="s">
+      <c r="C3" s="11" t="s">
         <v>129</v>
       </c>
       <c r="D3" s="4" t="s">
@@ -3013,7 +3088,7 @@
       <c r="B4" s="4" t="s">
         <v>98</v>
       </c>
-      <c r="C4" s="8" t="s">
+      <c r="C4" s="11" t="s">
         <v>97</v>
       </c>
       <c r="D4" s="4" t="s">
@@ -3044,7 +3119,7 @@
       <c r="B5" s="4" t="s">
         <v>121</v>
       </c>
-      <c r="C5" s="10" t="s">
+      <c r="C5" s="11" t="s">
         <v>122</v>
       </c>
       <c r="D5" s="4" t="s">
@@ -3068,9 +3143,40 @@
       <c r="J5" s="5"/>
       <c r="K5" s="4"/>
     </row>
+    <row r="6" spans="1:11" ht="30" customHeight="1">
+      <c r="A6" s="4">
+        <v>662</v>
+      </c>
+      <c r="B6" s="4" t="s">
+        <v>130</v>
+      </c>
+      <c r="C6" s="11" t="s">
+        <v>131</v>
+      </c>
+      <c r="D6" s="4" t="s">
+        <v>49</v>
+      </c>
+      <c r="E6" s="6" t="s">
+        <v>132</v>
+      </c>
+      <c r="F6" s="4" t="s">
+        <v>123</v>
+      </c>
+      <c r="G6" s="4" t="s">
+        <v>44</v>
+      </c>
+      <c r="H6" s="4" t="s">
+        <v>44</v>
+      </c>
+      <c r="I6" s="5">
+        <v>45490</v>
+      </c>
+      <c r="J6" s="5"/>
+      <c r="K6" s="4"/>
+    </row>
   </sheetData>
   <phoneticPr fontId="1" type="noConversion"/>
-  <conditionalFormatting sqref="D2:D5">
+  <conditionalFormatting sqref="D2:D6">
     <cfRule type="expression" dxfId="2" priority="1">
       <formula>D2="Easy"</formula>
     </cfRule>
@@ -3086,9 +3192,10 @@
     <hyperlink ref="C5" r:id="rId2" xr:uid="{8BC7B711-ADEB-4546-905F-7D690999B5BB}"/>
     <hyperlink ref="C2" r:id="rId3" xr:uid="{C2B4A6B6-B0D8-4F31-9802-387F04CC45FB}"/>
     <hyperlink ref="C3" r:id="rId4" xr:uid="{5615EAD9-62C1-4780-AE19-6BFAC2939521}"/>
+    <hyperlink ref="C6" r:id="rId5" xr:uid="{6D55272D-BA36-4797-A7CF-581EE973B392}"/>
   </hyperlinks>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
-  <pageSetup paperSize="9" orientation="portrait" verticalDpi="0" r:id="rId5"/>
+  <pageSetup paperSize="9" orientation="portrait" verticalDpi="0" r:id="rId6"/>
   <headerFooter>
     <oddFooter>&amp;L_x000D_&amp;1#&amp;"Calibri"&amp;10&amp;K000000 General</oddFooter>
   </headerFooter>

</xml_diff>

<commit_message>
Completed two more BFS practices.
</commit_message>
<xml_diff>
--- a/LeetCode Techniques.xlsx
+++ b/LeetCode Techniques.xlsx
@@ -8,9 +8,9 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\jack.yao\Desktop\LeetCode\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{B44FC48D-9B2B-4385-8134-5E6946714FFA}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{A18B67DE-D201-4A4D-B4FC-DC6EDA79DF77}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="-120" yWindow="-120" windowWidth="20640" windowHeight="11040" firstSheet="1" activeTab="5" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
+    <workbookView xWindow="-120" yWindow="-120" windowWidth="20640" windowHeight="11040" firstSheet="1" activeTab="6" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
   <sheets>
     <sheet name="Binary Search" sheetId="1" r:id="rId1"/>
@@ -39,7 +39,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="348" uniqueCount="137">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="360" uniqueCount="141">
   <si>
     <t>Name</t>
   </si>
@@ -533,20 +533,32 @@
     <t>https://leetcode.com/problems/maximum-width-of-binary-tree/</t>
   </si>
   <si>
+    <t>Evaluate Division</t>
+  </si>
+  <si>
+    <t>https://leetcode.com/problems/evaluate-division/description/</t>
+  </si>
+  <si>
+    <t>Use dict to build graph and trace nodes.</t>
+  </si>
+  <si>
+    <t>Graph</t>
+  </si>
+  <si>
+    <t>Check Completeness of a Binary Tree</t>
+  </si>
+  <si>
+    <t>https://leetcode.com/problems/check-completeness-of-a-binary-tree/description/</t>
+  </si>
+  <si>
     <t>Use parent &amp; children indices
-relationship to efficiently compute width.</t>
-  </si>
-  <si>
-    <t>Evaluate Division</t>
-  </si>
-  <si>
-    <t>https://leetcode.com/problems/evaluate-division/description/</t>
-  </si>
-  <si>
-    <t>Use dict to build graph and trace nodes.</t>
-  </si>
-  <si>
-    <t>Graph</t>
+relationship to swiftly compute width.</t>
+  </si>
+  <si>
+    <t>Maximum Level Sum of a Binary Tree</t>
+  </si>
+  <si>
+    <t>https://leetcode.com/problems/maximum-level-sum-of-a-binary-tree/</t>
   </si>
 </sst>
 </file>
@@ -2528,7 +2540,7 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{C287181F-E765-1C4E-B964-9C9FDBE62A17}">
   <dimension ref="A1:K13"/>
   <sheetViews>
-    <sheetView tabSelected="1" zoomScaleNormal="100" workbookViewId="0"/>
+    <sheetView zoomScaleNormal="100" workbookViewId="0"/>
   </sheetViews>
   <sheetFormatPr defaultColWidth="9" defaultRowHeight="16.5"/>
   <cols>
@@ -2698,19 +2710,19 @@
         <v>399</v>
       </c>
       <c r="B6" s="4" t="s">
+        <v>132</v>
+      </c>
+      <c r="C6" s="11" t="s">
         <v>133</v>
-      </c>
-      <c r="C6" s="11" t="s">
-        <v>134</v>
       </c>
       <c r="D6" s="4" t="s">
         <v>49</v>
       </c>
       <c r="E6" s="4" t="s">
+        <v>134</v>
+      </c>
+      <c r="F6" s="4" t="s">
         <v>135</v>
-      </c>
-      <c r="F6" s="4" t="s">
-        <v>136</v>
       </c>
       <c r="G6" s="4" t="s">
         <v>44</v>
@@ -2968,15 +2980,15 @@
 
 <file path=xl/worksheets/sheet7.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{75AC292A-7720-E145-9563-F6FD48AA33E3}">
-  <dimension ref="A1:K6"/>
+  <dimension ref="A1:K8"/>
   <sheetViews>
-    <sheetView zoomScaleNormal="100" workbookViewId="0"/>
+    <sheetView tabSelected="1" zoomScaleNormal="100" workbookViewId="0"/>
   </sheetViews>
   <sheetFormatPr defaultColWidth="9" defaultRowHeight="16.5"/>
   <cols>
     <col min="1" max="1" width="11" customWidth="1"/>
     <col min="2" max="2" width="43.28515625" customWidth="1"/>
-    <col min="3" max="3" width="35.85546875" style="9" customWidth="1"/>
+    <col min="3" max="3" width="35.85546875" style="12" customWidth="1"/>
     <col min="4" max="4" width="16" customWidth="1"/>
     <col min="5" max="5" width="36" customWidth="1"/>
     <col min="6" max="8" width="21" customWidth="1"/>
@@ -3157,7 +3169,7 @@
         <v>49</v>
       </c>
       <c r="E6" s="6" t="s">
-        <v>132</v>
+        <v>138</v>
       </c>
       <c r="F6" s="4" t="s">
         <v>123</v>
@@ -3174,9 +3186,67 @@
       <c r="J6" s="5"/>
       <c r="K6" s="4"/>
     </row>
+    <row r="7" spans="1:11" ht="20.100000000000001" customHeight="1">
+      <c r="A7" s="4">
+        <v>958</v>
+      </c>
+      <c r="B7" s="4" t="s">
+        <v>136</v>
+      </c>
+      <c r="C7" s="11" t="s">
+        <v>137</v>
+      </c>
+      <c r="D7" s="4" t="s">
+        <v>49</v>
+      </c>
+      <c r="E7" s="6"/>
+      <c r="F7" s="4" t="s">
+        <v>123</v>
+      </c>
+      <c r="G7" s="4" t="s">
+        <v>44</v>
+      </c>
+      <c r="H7" s="4" t="s">
+        <v>44</v>
+      </c>
+      <c r="I7" s="5">
+        <v>45491</v>
+      </c>
+      <c r="J7" s="5"/>
+      <c r="K7" s="4"/>
+    </row>
+    <row r="8" spans="1:11" ht="20.100000000000001" customHeight="1">
+      <c r="A8" s="4">
+        <v>1161</v>
+      </c>
+      <c r="B8" s="4" t="s">
+        <v>139</v>
+      </c>
+      <c r="C8" s="11" t="s">
+        <v>140</v>
+      </c>
+      <c r="D8" s="4" t="s">
+        <v>49</v>
+      </c>
+      <c r="E8" s="6"/>
+      <c r="F8" s="4" t="s">
+        <v>123</v>
+      </c>
+      <c r="G8" s="4" t="s">
+        <v>44</v>
+      </c>
+      <c r="H8" s="4" t="s">
+        <v>44</v>
+      </c>
+      <c r="I8" s="5">
+        <v>45491</v>
+      </c>
+      <c r="J8" s="5"/>
+      <c r="K8" s="4"/>
+    </row>
   </sheetData>
   <phoneticPr fontId="1" type="noConversion"/>
-  <conditionalFormatting sqref="D2:D6">
+  <conditionalFormatting sqref="D2:D8">
     <cfRule type="expression" dxfId="2" priority="1">
       <formula>D2="Easy"</formula>
     </cfRule>
@@ -3193,9 +3263,11 @@
     <hyperlink ref="C2" r:id="rId3" xr:uid="{C2B4A6B6-B0D8-4F31-9802-387F04CC45FB}"/>
     <hyperlink ref="C3" r:id="rId4" xr:uid="{5615EAD9-62C1-4780-AE19-6BFAC2939521}"/>
     <hyperlink ref="C6" r:id="rId5" xr:uid="{6D55272D-BA36-4797-A7CF-581EE973B392}"/>
+    <hyperlink ref="C7" r:id="rId6" xr:uid="{A382170A-F086-4927-B656-868CCD453ABF}"/>
+    <hyperlink ref="C8" r:id="rId7" xr:uid="{25BA1857-5CC6-4D6B-94BB-2E650759A139}"/>
   </hyperlinks>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
-  <pageSetup paperSize="9" orientation="portrait" verticalDpi="0" r:id="rId6"/>
+  <pageSetup paperSize="9" orientation="portrait" verticalDpi="0" r:id="rId8"/>
   <headerFooter>
     <oddFooter>&amp;L_x000D_&amp;1#&amp;"Calibri"&amp;10&amp;K000000 General</oddFooter>
   </headerFooter>

</xml_diff>

<commit_message>
Completed several DP practices.
</commit_message>
<xml_diff>
--- a/LeetCode Techniques.xlsx
+++ b/LeetCode Techniques.xlsx
@@ -1,25 +1,26 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
-  <fileVersion appName="xl" lastEdited="7" lowestEdited="4" rupBuild="26731"/>
+  <fileVersion appName="xl" lastEdited="7" lowestEdited="4" rupBuild="10714"/>
   <workbookPr defaultThemeVersion="124226"/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\jack.yao\Desktop\LeetCode\"/>
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="/Users/blackjack625/Desktop/LeetCode/"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{A18B67DE-D201-4A4D-B4FC-DC6EDA79DF77}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{7944EEAC-C002-FC47-9553-D61AFE66D2F0}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="-120" yWindow="-120" windowWidth="20640" windowHeight="11040" firstSheet="1" activeTab="6" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
+    <workbookView xWindow="0" yWindow="500" windowWidth="20640" windowHeight="11040" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
   <sheets>
-    <sheet name="Binary Search" sheetId="1" r:id="rId1"/>
-    <sheet name="Sliding Window" sheetId="2" r:id="rId2"/>
-    <sheet name="Set Maneuver" sheetId="3" r:id="rId3"/>
-    <sheet name="Recursion" sheetId="5" r:id="rId4"/>
-    <sheet name="Trie" sheetId="4" r:id="rId5"/>
-    <sheet name="Depth First Search" sheetId="6" r:id="rId6"/>
-    <sheet name="Breadth First Search" sheetId="7" r:id="rId7"/>
+    <sheet name="Dynamic Programming" sheetId="8" r:id="rId1"/>
+    <sheet name="Binary Search" sheetId="1" r:id="rId2"/>
+    <sheet name="Sliding Window" sheetId="2" r:id="rId3"/>
+    <sheet name="Set Maneuver" sheetId="3" r:id="rId4"/>
+    <sheet name="Recursion" sheetId="5" r:id="rId5"/>
+    <sheet name="Trie" sheetId="4" r:id="rId6"/>
+    <sheet name="Depth First Search" sheetId="6" r:id="rId7"/>
+    <sheet name="Breadth First Search" sheetId="7" r:id="rId8"/>
   </sheets>
   <calcPr calcId="191029"/>
   <extLst>
@@ -39,7 +40,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="360" uniqueCount="141">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="423" uniqueCount="164">
   <si>
     <t>Name</t>
   </si>
@@ -559,6 +560,101 @@
   </si>
   <si>
     <t>https://leetcode.com/problems/maximum-level-sum-of-a-binary-tree/</t>
+  </si>
+  <si>
+    <t>Binary Tree Maximum Path Sum</t>
+    <phoneticPr fontId="1" type="noConversion"/>
+  </si>
+  <si>
+    <t>https://leetcode.com/problems/binary-tree-maximum-path-sum/description/</t>
+    <phoneticPr fontId="1" type="noConversion"/>
+  </si>
+  <si>
+    <t>When returning path to parent,
+can't take both left &amp; right paths.</t>
+    <phoneticPr fontId="1" type="noConversion"/>
+  </si>
+  <si>
+    <t>Unique Paths</t>
+    <phoneticPr fontId="1" type="noConversion"/>
+  </si>
+  <si>
+    <t>Unique Paths II</t>
+    <phoneticPr fontId="1" type="noConversion"/>
+  </si>
+  <si>
+    <t>https://leetcode.com/problems/unique-paths/description/</t>
+    <phoneticPr fontId="1" type="noConversion"/>
+  </si>
+  <si>
+    <t>https://leetcode.com/problems/unique-paths-ii/description/</t>
+    <phoneticPr fontId="1" type="noConversion"/>
+  </si>
+  <si>
+    <t>Minimum Path Sum</t>
+    <phoneticPr fontId="1" type="noConversion"/>
+  </si>
+  <si>
+    <t>https://leetcode.com/problems/minimum-path-sum/</t>
+    <phoneticPr fontId="1" type="noConversion"/>
+  </si>
+  <si>
+    <t>Obstacles will block entire
+righter row &amp; lower column entries.</t>
+    <phoneticPr fontId="1" type="noConversion"/>
+  </si>
+  <si>
+    <t>House Robber</t>
+    <phoneticPr fontId="1" type="noConversion"/>
+  </si>
+  <si>
+    <t>House Robber II</t>
+    <phoneticPr fontId="1" type="noConversion"/>
+  </si>
+  <si>
+    <t>https://leetcode.com/problems/house-robber/submissions/1250506908/</t>
+    <phoneticPr fontId="1" type="noConversion"/>
+  </si>
+  <si>
+    <t>https://leetcode.com/problems/house-robber-ii/submissions/1250688145/</t>
+    <phoneticPr fontId="1" type="noConversion"/>
+  </si>
+  <si>
+    <t xml:space="preserve">Do two iterations in circular cases:
+one excluding 1st item, and the other excluding last item. </t>
+    <phoneticPr fontId="1" type="noConversion"/>
+  </si>
+  <si>
+    <t>Triangle</t>
+    <phoneticPr fontId="1" type="noConversion"/>
+  </si>
+  <si>
+    <t>https://leetcode.com/problems/triangle/description/</t>
+    <phoneticPr fontId="1" type="noConversion"/>
+  </si>
+  <si>
+    <t>MWIS</t>
+    <phoneticPr fontId="1" type="noConversion"/>
+  </si>
+  <si>
+    <t>Maximum Subarray</t>
+    <phoneticPr fontId="1" type="noConversion"/>
+  </si>
+  <si>
+    <t>https://leetcode.com/problems/maximum-subarray/description/</t>
+    <phoneticPr fontId="1" type="noConversion"/>
+  </si>
+  <si>
+    <t>Maximum Product Subarray</t>
+    <phoneticPr fontId="1" type="noConversion"/>
+  </si>
+  <si>
+    <t>https://leetcode.com/problems/maximum-product-subarray/</t>
+    <phoneticPr fontId="1" type="noConversion"/>
+  </si>
+  <si>
+    <t>Prepare positive &amp; negative subarrays in case they switch roles due to incoming negative number.</t>
+    <phoneticPr fontId="1" type="noConversion"/>
   </si>
 </sst>
 </file>
@@ -566,19 +662,19 @@
 <file path=xl/styles.xml><?xml version="1.0" encoding="utf-8"?>
 <styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:x16r2="http://schemas.microsoft.com/office/spreadsheetml/2015/02/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" mc:Ignorable="x14ac x16r2 xr">
   <numFmts count="1">
-    <numFmt numFmtId="164" formatCode="yyyy&quot;年&quot;m&quot;月&quot;d&quot;日&quot;;@"/>
+    <numFmt numFmtId="176" formatCode="yyyy&quot;年&quot;m&quot;月&quot;d&quot;日&quot;;@"/>
   </numFmts>
   <fonts count="11">
     <font>
       <sz val="11"/>
       <color theme="1"/>
-      <name val="Calibri"/>
+      <name val="新細明體"/>
       <family val="2"/>
       <scheme val="minor"/>
     </font>
     <font>
       <sz val="9"/>
-      <name val="Calibri"/>
+      <name val="新細明體"/>
       <family val="2"/>
       <charset val="136"/>
       <scheme val="minor"/>
@@ -602,7 +698,7 @@
       <u/>
       <sz val="11"/>
       <color theme="10"/>
-      <name val="Calibri"/>
+      <name val="新細明體"/>
       <family val="2"/>
       <scheme val="minor"/>
     </font>
@@ -632,17 +728,20 @@
       <sz val="10"/>
       <color theme="1"/>
       <name val="Microsoft YaHei"/>
+      <charset val="134"/>
     </font>
     <font>
       <u/>
       <sz val="10"/>
       <color theme="10"/>
       <name val="Microsoft YaHei"/>
+      <charset val="134"/>
     </font>
     <font>
       <sz val="10"/>
       <color theme="1"/>
       <name val="Microsoft YaHei"/>
+      <charset val="134"/>
     </font>
   </fonts>
   <fills count="2">
@@ -681,19 +780,19 @@
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
     <xf numFmtId="0" fontId="4" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
   </cellStyleXfs>
-  <cellXfs count="13">
+  <cellXfs count="14">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
-    <xf numFmtId="164" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1"/>
+    <xf numFmtId="176" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1"/>
     <xf numFmtId="0" fontId="2" fillId="0" borderId="1" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
     </xf>
-    <xf numFmtId="164" fontId="2" fillId="0" borderId="1" xfId="0" applyNumberFormat="1" applyFont="1" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="176" fontId="2" fillId="0" borderId="1" xfId="0" applyNumberFormat="1" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
     </xf>
     <xf numFmtId="0" fontId="3" fillId="0" borderId="1" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
     </xf>
-    <xf numFmtId="164" fontId="3" fillId="0" borderId="1" xfId="0" applyNumberFormat="1" applyFont="1" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="176" fontId="3" fillId="0" borderId="1" xfId="0" applyNumberFormat="1" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
     </xf>
     <xf numFmtId="0" fontId="3" fillId="0" borderId="1" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
@@ -713,12 +812,73 @@
       <alignment horizontal="center" vertical="center"/>
     </xf>
     <xf numFmtId="0" fontId="10" fillId="0" borderId="0" xfId="0" applyFont="1"/>
+    <xf numFmtId="0" fontId="3" fillId="0" borderId="0" xfId="0" applyFont="1"/>
   </cellXfs>
   <cellStyles count="2">
-    <cellStyle name="Hyperlink" xfId="1" builtinId="8"/>
-    <cellStyle name="Normal" xfId="0" builtinId="0"/>
+    <cellStyle name="一般" xfId="0" builtinId="0"/>
+    <cellStyle name="超連結" xfId="1" builtinId="8"/>
   </cellStyles>
-  <dxfs count="27">
+  <dxfs count="33">
+    <dxf>
+      <font>
+        <color rgb="FFFFFF00"/>
+      </font>
+      <fill>
+        <patternFill>
+          <bgColor rgb="FFFF0000"/>
+        </patternFill>
+      </fill>
+    </dxf>
+    <dxf>
+      <font>
+        <color theme="1"/>
+      </font>
+      <fill>
+        <patternFill>
+          <bgColor rgb="FFFFFF00"/>
+        </patternFill>
+      </fill>
+    </dxf>
+    <dxf>
+      <font>
+        <color theme="0"/>
+      </font>
+      <fill>
+        <patternFill>
+          <bgColor rgb="FF00B050"/>
+        </patternFill>
+      </fill>
+    </dxf>
+    <dxf>
+      <font>
+        <color rgb="FFFFFF00"/>
+      </font>
+      <fill>
+        <patternFill>
+          <bgColor rgb="FFFF0000"/>
+        </patternFill>
+      </fill>
+    </dxf>
+    <dxf>
+      <font>
+        <color theme="1"/>
+      </font>
+      <fill>
+        <patternFill>
+          <bgColor rgb="FFFFFF00"/>
+        </patternFill>
+      </fill>
+    </dxf>
+    <dxf>
+      <font>
+        <color theme="0"/>
+      </font>
+      <fill>
+        <patternFill>
+          <bgColor rgb="FF00B050"/>
+        </patternFill>
+      </fill>
+    </dxf>
     <dxf>
       <font>
         <color rgb="FFFFFF00"/>
@@ -1288,15 +1448,357 @@
 </file>
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{23E6E9DF-BEE0-B544-8910-7DDC3380F4B7}">
+  <dimension ref="A1:K10"/>
+  <sheetViews>
+    <sheetView tabSelected="1" zoomScaleNormal="100" workbookViewId="0"/>
+  </sheetViews>
+  <sheetFormatPr baseColWidth="10" defaultColWidth="9" defaultRowHeight="16"/>
+  <cols>
+    <col min="1" max="1" width="11" customWidth="1"/>
+    <col min="2" max="2" width="46" customWidth="1"/>
+    <col min="3" max="3" width="65.796875" style="13" customWidth="1"/>
+    <col min="4" max="4" width="16" customWidth="1"/>
+    <col min="5" max="5" width="36" customWidth="1"/>
+    <col min="6" max="8" width="21" customWidth="1"/>
+    <col min="9" max="10" width="16" style="1" customWidth="1"/>
+    <col min="11" max="11" width="16" customWidth="1"/>
+  </cols>
+  <sheetData>
+    <row r="1" spans="1:11" ht="20" customHeight="1">
+      <c r="A1" s="2" t="s">
+        <v>4</v>
+      </c>
+      <c r="B1" s="2" t="s">
+        <v>0</v>
+      </c>
+      <c r="C1" s="2" t="s">
+        <v>1</v>
+      </c>
+      <c r="D1" s="2" t="s">
+        <v>2</v>
+      </c>
+      <c r="E1" s="2" t="s">
+        <v>30</v>
+      </c>
+      <c r="F1" s="2" t="s">
+        <v>22</v>
+      </c>
+      <c r="G1" s="2" t="s">
+        <v>5</v>
+      </c>
+      <c r="H1" s="2" t="s">
+        <v>6</v>
+      </c>
+      <c r="I1" s="3" t="s">
+        <v>8</v>
+      </c>
+      <c r="J1" s="3" t="s">
+        <v>7</v>
+      </c>
+      <c r="K1" s="2" t="s">
+        <v>3</v>
+      </c>
+    </row>
+    <row r="2" spans="1:11" ht="20" customHeight="1">
+      <c r="A2" s="4">
+        <v>53</v>
+      </c>
+      <c r="B2" s="4" t="s">
+        <v>159</v>
+      </c>
+      <c r="C2" s="8" t="s">
+        <v>160</v>
+      </c>
+      <c r="D2" s="4" t="s">
+        <v>49</v>
+      </c>
+      <c r="E2" s="4"/>
+      <c r="F2" s="4"/>
+      <c r="G2" s="4" t="s">
+        <v>11</v>
+      </c>
+      <c r="H2" s="4" t="s">
+        <v>29</v>
+      </c>
+      <c r="I2" s="5">
+        <v>45404</v>
+      </c>
+      <c r="J2" s="5"/>
+      <c r="K2" s="4"/>
+    </row>
+    <row r="3" spans="1:11" ht="20" customHeight="1">
+      <c r="A3" s="4">
+        <v>62</v>
+      </c>
+      <c r="B3" s="4" t="s">
+        <v>144</v>
+      </c>
+      <c r="C3" s="8" t="s">
+        <v>146</v>
+      </c>
+      <c r="D3" s="4" t="s">
+        <v>49</v>
+      </c>
+      <c r="E3" s="4"/>
+      <c r="F3" s="4"/>
+      <c r="G3" s="4" t="s">
+        <v>75</v>
+      </c>
+      <c r="H3" s="4" t="s">
+        <v>71</v>
+      </c>
+      <c r="I3" s="5">
+        <v>45493</v>
+      </c>
+      <c r="J3" s="5"/>
+      <c r="K3" s="4"/>
+    </row>
+    <row r="4" spans="1:11" ht="30" customHeight="1">
+      <c r="A4" s="4">
+        <v>63</v>
+      </c>
+      <c r="B4" s="4" t="s">
+        <v>145</v>
+      </c>
+      <c r="C4" s="8" t="s">
+        <v>147</v>
+      </c>
+      <c r="D4" s="4" t="s">
+        <v>49</v>
+      </c>
+      <c r="E4" s="6" t="s">
+        <v>150</v>
+      </c>
+      <c r="F4" s="4"/>
+      <c r="G4" s="4" t="s">
+        <v>75</v>
+      </c>
+      <c r="H4" s="4" t="s">
+        <v>75</v>
+      </c>
+      <c r="I4" s="5">
+        <v>45493</v>
+      </c>
+      <c r="J4" s="5"/>
+      <c r="K4" s="4"/>
+    </row>
+    <row r="5" spans="1:11" ht="20" customHeight="1">
+      <c r="A5" s="4">
+        <v>64</v>
+      </c>
+      <c r="B5" s="4" t="s">
+        <v>148</v>
+      </c>
+      <c r="C5" s="8" t="s">
+        <v>149</v>
+      </c>
+      <c r="D5" s="4" t="s">
+        <v>49</v>
+      </c>
+      <c r="E5" s="4"/>
+      <c r="F5" s="4"/>
+      <c r="G5" s="4" t="s">
+        <v>75</v>
+      </c>
+      <c r="H5" s="4" t="s">
+        <v>71</v>
+      </c>
+      <c r="I5" s="5">
+        <v>45493</v>
+      </c>
+      <c r="J5" s="5"/>
+      <c r="K5" s="4"/>
+    </row>
+    <row r="6" spans="1:11" ht="20" customHeight="1">
+      <c r="A6" s="4">
+        <v>120</v>
+      </c>
+      <c r="B6" s="4" t="s">
+        <v>156</v>
+      </c>
+      <c r="C6" s="8" t="s">
+        <v>157</v>
+      </c>
+      <c r="D6" s="4" t="s">
+        <v>10</v>
+      </c>
+      <c r="E6" s="4"/>
+      <c r="F6" s="4"/>
+      <c r="G6" s="4" t="s">
+        <v>11</v>
+      </c>
+      <c r="H6" s="4" t="s">
+        <v>11</v>
+      </c>
+      <c r="I6" s="5">
+        <v>45494</v>
+      </c>
+      <c r="J6" s="5"/>
+      <c r="K6" s="4"/>
+    </row>
+    <row r="7" spans="1:11" ht="30" customHeight="1">
+      <c r="A7" s="4">
+        <v>124</v>
+      </c>
+      <c r="B7" s="4" t="s">
+        <v>141</v>
+      </c>
+      <c r="C7" s="8" t="s">
+        <v>142</v>
+      </c>
+      <c r="D7" s="4" t="s">
+        <v>16</v>
+      </c>
+      <c r="E7" s="6" t="s">
+        <v>143</v>
+      </c>
+      <c r="F7" s="4" t="s">
+        <v>72</v>
+      </c>
+      <c r="G7" s="4" t="s">
+        <v>11</v>
+      </c>
+      <c r="H7" s="4" t="s">
+        <v>11</v>
+      </c>
+      <c r="I7" s="5">
+        <v>45493</v>
+      </c>
+      <c r="J7" s="5"/>
+      <c r="K7" s="4"/>
+    </row>
+    <row r="8" spans="1:11" ht="45" customHeight="1">
+      <c r="A8" s="4">
+        <v>152</v>
+      </c>
+      <c r="B8" s="4" t="s">
+        <v>161</v>
+      </c>
+      <c r="C8" s="8" t="s">
+        <v>162</v>
+      </c>
+      <c r="D8" s="4" t="s">
+        <v>49</v>
+      </c>
+      <c r="E8" s="6" t="s">
+        <v>163</v>
+      </c>
+      <c r="F8" s="4"/>
+      <c r="G8" s="4" t="s">
+        <v>11</v>
+      </c>
+      <c r="H8" s="4" t="s">
+        <v>29</v>
+      </c>
+      <c r="I8" s="5">
+        <v>45405</v>
+      </c>
+      <c r="J8" s="5"/>
+      <c r="K8" s="4"/>
+    </row>
+    <row r="9" spans="1:11" ht="20" customHeight="1">
+      <c r="A9" s="4">
+        <v>198</v>
+      </c>
+      <c r="B9" s="4" t="s">
+        <v>151</v>
+      </c>
+      <c r="C9" s="8" t="s">
+        <v>153</v>
+      </c>
+      <c r="D9" s="4" t="s">
+        <v>49</v>
+      </c>
+      <c r="E9" s="4"/>
+      <c r="F9" s="4" t="s">
+        <v>158</v>
+      </c>
+      <c r="G9" s="4" t="s">
+        <v>11</v>
+      </c>
+      <c r="H9" s="4" t="s">
+        <v>29</v>
+      </c>
+      <c r="I9" s="5">
+        <v>45418</v>
+      </c>
+      <c r="J9" s="5"/>
+      <c r="K9" s="4"/>
+    </row>
+    <row r="10" spans="1:11" ht="45" customHeight="1">
+      <c r="A10" s="4">
+        <v>213</v>
+      </c>
+      <c r="B10" s="4" t="s">
+        <v>152</v>
+      </c>
+      <c r="C10" s="8" t="s">
+        <v>154</v>
+      </c>
+      <c r="D10" s="4" t="s">
+        <v>49</v>
+      </c>
+      <c r="E10" s="6" t="s">
+        <v>155</v>
+      </c>
+      <c r="F10" s="4" t="s">
+        <v>158</v>
+      </c>
+      <c r="G10" s="4" t="s">
+        <v>44</v>
+      </c>
+      <c r="H10" s="4" t="s">
+        <v>29</v>
+      </c>
+      <c r="I10" s="5">
+        <v>45418</v>
+      </c>
+      <c r="J10" s="5"/>
+      <c r="K10" s="4"/>
+    </row>
+  </sheetData>
+  <phoneticPr fontId="1" type="noConversion"/>
+  <conditionalFormatting sqref="D2:D10">
+    <cfRule type="expression" dxfId="32" priority="1">
+      <formula>D2="Easy"</formula>
+    </cfRule>
+    <cfRule type="expression" dxfId="31" priority="2">
+      <formula>D2="Medium"</formula>
+    </cfRule>
+    <cfRule type="expression" dxfId="30" priority="3">
+      <formula>D2="Hard"</formula>
+    </cfRule>
+  </conditionalFormatting>
+  <hyperlinks>
+    <hyperlink ref="C3" r:id="rId1" xr:uid="{7E21394E-57A4-E54A-9299-637EDCA54312}"/>
+    <hyperlink ref="C10" r:id="rId2" xr:uid="{296D78C9-0683-A64E-B81F-7705D07A2653}"/>
+    <hyperlink ref="C4" r:id="rId3" xr:uid="{43DDB127-5D11-D54D-BBEF-BA3EAAF66580}"/>
+    <hyperlink ref="C5" r:id="rId4" xr:uid="{437899AB-6D74-0947-B37F-B30C732DC535}"/>
+    <hyperlink ref="C9" r:id="rId5" xr:uid="{2C34938E-0988-9A47-85E4-F3B76883B44D}"/>
+    <hyperlink ref="C7" r:id="rId6" xr:uid="{C4D656BA-A6C7-544D-8F38-EB79AFC85969}"/>
+    <hyperlink ref="C6" r:id="rId7" xr:uid="{2022A0AD-F338-4B4A-8571-BB4A95D7EE00}"/>
+    <hyperlink ref="C2" r:id="rId8" xr:uid="{11FB62CE-95A4-8149-A0D0-EC80907AD300}"/>
+    <hyperlink ref="C8" r:id="rId9" xr:uid="{D0C86F76-90D0-4847-AD9B-8F8B4200A39D}"/>
+  </hyperlinks>
+  <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
+  <pageSetup paperSize="9" orientation="portrait" verticalDpi="0" r:id="rId10"/>
+  <headerFooter>
+    <oddFooter>&amp;L_x000D_&amp;1#&amp;"Calibri"&amp;10&amp;K000000 General</oddFooter>
+  </headerFooter>
+</worksheet>
+</file>
+
+<file path=xl/worksheets/sheet2.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0000-000000000000}">
   <dimension ref="A1:K15"/>
   <sheetViews>
     <sheetView zoomScaleNormal="100" workbookViewId="0"/>
   </sheetViews>
-  <sheetFormatPr defaultColWidth="9" defaultRowHeight="16.5"/>
+  <sheetFormatPr baseColWidth="10" defaultColWidth="9" defaultRowHeight="17"/>
   <cols>
     <col min="1" max="1" width="11" customWidth="1"/>
-    <col min="2" max="2" width="38.140625" customWidth="1"/>
+    <col min="2" max="2" width="38.19921875" customWidth="1"/>
     <col min="3" max="3" width="71" style="9" customWidth="1"/>
     <col min="4" max="4" width="16" customWidth="1"/>
     <col min="5" max="5" width="36" customWidth="1"/>
@@ -1305,7 +1807,7 @@
     <col min="11" max="11" width="16" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:11" ht="20.100000000000001" customHeight="1">
+    <row r="1" spans="1:11" ht="20" customHeight="1">
       <c r="A1" s="2" t="s">
         <v>4</v>
       </c>
@@ -1340,7 +1842,7 @@
         <v>3</v>
       </c>
     </row>
-    <row r="2" spans="1:11" ht="20.100000000000001" customHeight="1">
+    <row r="2" spans="1:11" ht="20" customHeight="1">
       <c r="A2" s="4">
         <v>74</v>
       </c>
@@ -1367,7 +1869,7 @@
       <c r="J2" s="3"/>
       <c r="K2" s="2"/>
     </row>
-    <row r="3" spans="1:11" ht="20.100000000000001" customHeight="1">
+    <row r="3" spans="1:11" ht="20" customHeight="1">
       <c r="A3" s="4">
         <v>220</v>
       </c>
@@ -1423,7 +1925,7 @@
       <c r="J4" s="5"/>
       <c r="K4" s="4"/>
     </row>
-    <row r="5" spans="1:11" ht="20.100000000000001" customHeight="1">
+    <row r="5" spans="1:11" ht="20" customHeight="1">
       <c r="A5" s="4">
         <v>315</v>
       </c>
@@ -1450,7 +1952,7 @@
       <c r="J5" s="5"/>
       <c r="K5" s="4"/>
     </row>
-    <row r="6" spans="1:11" ht="20.100000000000001" customHeight="1">
+    <row r="6" spans="1:11" ht="20" customHeight="1">
       <c r="A6" s="4">
         <v>352</v>
       </c>
@@ -1479,7 +1981,7 @@
       <c r="J6" s="5"/>
       <c r="K6" s="4"/>
     </row>
-    <row r="7" spans="1:11" ht="20.100000000000001" customHeight="1">
+    <row r="7" spans="1:11" ht="20" customHeight="1">
       <c r="A7" s="4">
         <v>480</v>
       </c>
@@ -1506,7 +2008,7 @@
       <c r="J7" s="5"/>
       <c r="K7" s="4"/>
     </row>
-    <row r="8" spans="1:11" ht="20.100000000000001" customHeight="1">
+    <row r="8" spans="1:11" ht="20" customHeight="1">
       <c r="A8" s="4">
         <v>493</v>
       </c>
@@ -1533,7 +2035,7 @@
       <c r="J8" s="5"/>
       <c r="K8" s="4"/>
     </row>
-    <row r="9" spans="1:11" ht="20.100000000000001" customHeight="1">
+    <row r="9" spans="1:11" ht="20" customHeight="1">
       <c r="A9" s="4">
         <v>611</v>
       </c>
@@ -1562,7 +2064,7 @@
       <c r="J9" s="5"/>
       <c r="K9" s="4"/>
     </row>
-    <row r="10" spans="1:11" ht="20.100000000000001" customHeight="1">
+    <row r="10" spans="1:11" ht="20" customHeight="1">
       <c r="A10" s="4">
         <v>729</v>
       </c>
@@ -1589,7 +2091,7 @@
       <c r="J10" s="5"/>
       <c r="K10" s="4"/>
     </row>
-    <row r="11" spans="1:11" ht="20.100000000000001" customHeight="1">
+    <row r="11" spans="1:11" ht="20" customHeight="1">
       <c r="A11" s="4">
         <v>1095</v>
       </c>
@@ -1647,7 +2149,7 @@
       <c r="J12" s="5"/>
       <c r="K12" s="4"/>
     </row>
-    <row r="13" spans="1:11" ht="20.100000000000001" customHeight="1">
+    <row r="13" spans="1:11" ht="20" customHeight="1">
       <c r="A13" s="4">
         <v>1825</v>
       </c>
@@ -1676,7 +2178,7 @@
       <c r="J13" s="5"/>
       <c r="K13" s="4"/>
     </row>
-    <row r="14" spans="1:11" ht="20.100000000000001" customHeight="1">
+    <row r="14" spans="1:11" ht="20" customHeight="1">
       <c r="A14" s="4">
         <v>2034</v>
       </c>
@@ -1705,7 +2207,7 @@
       <c r="J14" s="5"/>
       <c r="K14" s="4"/>
     </row>
-    <row r="15" spans="1:11" ht="20.100000000000001" customHeight="1">
+    <row r="15" spans="1:11" ht="20" customHeight="1">
       <c r="A15" s="4">
         <v>2102</v>
       </c>
@@ -1740,24 +2242,24 @@
   </sortState>
   <phoneticPr fontId="1" type="noConversion"/>
   <conditionalFormatting sqref="D2:D3">
-    <cfRule type="expression" dxfId="26" priority="1">
+    <cfRule type="expression" dxfId="29" priority="1">
       <formula>D2="Easy"</formula>
     </cfRule>
-    <cfRule type="expression" dxfId="25" priority="2">
+    <cfRule type="expression" dxfId="28" priority="2">
       <formula>D2="Medium"</formula>
     </cfRule>
-    <cfRule type="expression" dxfId="24" priority="3">
+    <cfRule type="expression" dxfId="27" priority="3">
       <formula>D2="Hard"</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="D4:E15">
-    <cfRule type="expression" dxfId="23" priority="4">
+    <cfRule type="expression" dxfId="26" priority="4">
       <formula>D4="Easy"</formula>
     </cfRule>
-    <cfRule type="expression" dxfId="22" priority="5">
+    <cfRule type="expression" dxfId="25" priority="5">
       <formula>D4="Medium"</formula>
     </cfRule>
-    <cfRule type="expression" dxfId="21" priority="6">
+    <cfRule type="expression" dxfId="24" priority="6">
       <formula>D4="Hard"</formula>
     </cfRule>
   </conditionalFormatting>
@@ -1784,16 +2286,16 @@
 </worksheet>
 </file>
 
-<file path=xl/worksheets/sheet2.xml><?xml version="1.0" encoding="utf-8"?>
+<file path=xl/worksheets/sheet3.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{96F16DFC-20ED-4148-9FB8-AA8D12910A09}">
   <dimension ref="A1:K3"/>
   <sheetViews>
     <sheetView zoomScaleNormal="100" workbookViewId="0"/>
   </sheetViews>
-  <sheetFormatPr defaultColWidth="9" defaultRowHeight="16.5"/>
+  <sheetFormatPr baseColWidth="10" defaultColWidth="9" defaultRowHeight="17"/>
   <cols>
     <col min="1" max="1" width="11" customWidth="1"/>
-    <col min="2" max="2" width="45.85546875" customWidth="1"/>
+    <col min="2" max="2" width="45.796875" customWidth="1"/>
     <col min="3" max="3" width="71" style="9" customWidth="1"/>
     <col min="4" max="4" width="16" customWidth="1"/>
     <col min="5" max="5" width="36" customWidth="1"/>
@@ -1802,7 +2304,7 @@
     <col min="11" max="11" width="16" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:11" ht="20.100000000000001" customHeight="1">
+    <row r="1" spans="1:11" ht="20" customHeight="1">
       <c r="A1" s="2" t="s">
         <v>4</v>
       </c>
@@ -1837,7 +2339,7 @@
         <v>3</v>
       </c>
     </row>
-    <row r="2" spans="1:11" ht="20.100000000000001" customHeight="1">
+    <row r="2" spans="1:11" ht="20" customHeight="1">
       <c r="A2" s="4">
         <v>3</v>
       </c>
@@ -1864,7 +2366,7 @@
       <c r="J2" s="5"/>
       <c r="K2" s="4"/>
     </row>
-    <row r="3" spans="1:11" ht="20.100000000000001" customHeight="1">
+    <row r="3" spans="1:11" ht="20" customHeight="1">
       <c r="A3" s="4">
         <v>1695</v>
       </c>
@@ -1894,13 +2396,13 @@
   </sheetData>
   <phoneticPr fontId="1" type="noConversion"/>
   <conditionalFormatting sqref="D2:E3">
-    <cfRule type="expression" dxfId="20" priority="4">
+    <cfRule type="expression" dxfId="23" priority="4">
       <formula>D2="Easy"</formula>
     </cfRule>
-    <cfRule type="expression" dxfId="19" priority="5">
+    <cfRule type="expression" dxfId="22" priority="5">
       <formula>D2="Medium"</formula>
     </cfRule>
-    <cfRule type="expression" dxfId="18" priority="6">
+    <cfRule type="expression" dxfId="21" priority="6">
       <formula>D2="Hard"</formula>
     </cfRule>
   </conditionalFormatting>
@@ -1915,17 +2417,17 @@
 </worksheet>
 </file>
 
-<file path=xl/worksheets/sheet3.xml><?xml version="1.0" encoding="utf-8"?>
+<file path=xl/worksheets/sheet4.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{4F94156D-DED3-4FD7-B619-DDD9FD49102F}">
   <dimension ref="A1:K4"/>
   <sheetViews>
     <sheetView zoomScaleNormal="100" workbookViewId="0"/>
   </sheetViews>
-  <sheetFormatPr defaultColWidth="9" defaultRowHeight="16.5"/>
+  <sheetFormatPr baseColWidth="10" defaultColWidth="9" defaultRowHeight="17"/>
   <cols>
     <col min="1" max="1" width="11" customWidth="1"/>
-    <col min="2" max="2" width="25.85546875" customWidth="1"/>
-    <col min="3" max="3" width="65.85546875" style="9" customWidth="1"/>
+    <col min="2" max="2" width="25.796875" customWidth="1"/>
+    <col min="3" max="3" width="65.796875" style="9" customWidth="1"/>
     <col min="4" max="4" width="16" customWidth="1"/>
     <col min="5" max="5" width="36" customWidth="1"/>
     <col min="6" max="8" width="21" customWidth="1"/>
@@ -1933,7 +2435,7 @@
     <col min="11" max="11" width="16" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:11" ht="20.100000000000001" customHeight="1">
+    <row r="1" spans="1:11" ht="20" customHeight="1">
       <c r="A1" s="2" t="s">
         <v>4</v>
       </c>
@@ -1968,7 +2470,7 @@
         <v>3</v>
       </c>
     </row>
-    <row r="2" spans="1:11" ht="20.100000000000001" customHeight="1">
+    <row r="2" spans="1:11" ht="20" customHeight="1">
       <c r="A2" s="4">
         <v>41</v>
       </c>
@@ -1999,7 +2501,7 @@
       </c>
       <c r="K2" s="4"/>
     </row>
-    <row r="3" spans="1:11" ht="20.100000000000001" customHeight="1">
+    <row r="3" spans="1:11" ht="20" customHeight="1">
       <c r="A3" s="4">
         <v>287</v>
       </c>
@@ -2026,7 +2528,7 @@
       <c r="J3" s="5"/>
       <c r="K3" s="4"/>
     </row>
-    <row r="4" spans="1:11" ht="20.100000000000001" customHeight="1">
+    <row r="4" spans="1:11" ht="20" customHeight="1">
       <c r="A4" s="4">
         <v>645</v>
       </c>
@@ -2056,24 +2558,24 @@
   </sheetData>
   <phoneticPr fontId="1" type="noConversion"/>
   <conditionalFormatting sqref="D2">
-    <cfRule type="expression" dxfId="17" priority="1">
+    <cfRule type="expression" dxfId="20" priority="1">
       <formula>D2="Easy"</formula>
     </cfRule>
-    <cfRule type="expression" dxfId="16" priority="2">
+    <cfRule type="expression" dxfId="19" priority="2">
       <formula>D2="Medium"</formula>
     </cfRule>
-    <cfRule type="expression" dxfId="15" priority="3">
+    <cfRule type="expression" dxfId="18" priority="3">
       <formula>D2="Hard"</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="D3:E4">
-    <cfRule type="expression" dxfId="14" priority="4">
+    <cfRule type="expression" dxfId="17" priority="4">
       <formula>D3="Easy"</formula>
     </cfRule>
-    <cfRule type="expression" dxfId="13" priority="5">
+    <cfRule type="expression" dxfId="16" priority="5">
       <formula>D3="Medium"</formula>
     </cfRule>
-    <cfRule type="expression" dxfId="12" priority="6">
+    <cfRule type="expression" dxfId="15" priority="6">
       <formula>D3="Hard"</formula>
     </cfRule>
   </conditionalFormatting>
@@ -2090,17 +2592,17 @@
 </worksheet>
 </file>
 
-<file path=xl/worksheets/sheet4.xml><?xml version="1.0" encoding="utf-8"?>
+<file path=xl/worksheets/sheet5.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{69159F7B-7780-4FD1-9225-126219315A4A}">
   <dimension ref="A1:K2"/>
   <sheetViews>
     <sheetView zoomScaleNormal="100" workbookViewId="0"/>
   </sheetViews>
-  <sheetFormatPr defaultColWidth="9" defaultRowHeight="16.5"/>
+  <sheetFormatPr baseColWidth="10" defaultColWidth="9" defaultRowHeight="17"/>
   <cols>
     <col min="1" max="1" width="11" customWidth="1"/>
     <col min="2" max="2" width="16" customWidth="1"/>
-    <col min="3" max="3" width="35.85546875" style="9" customWidth="1"/>
+    <col min="3" max="3" width="35.796875" style="9" customWidth="1"/>
     <col min="4" max="4" width="16" customWidth="1"/>
     <col min="5" max="5" width="36" customWidth="1"/>
     <col min="6" max="8" width="21" customWidth="1"/>
@@ -2108,7 +2610,7 @@
     <col min="11" max="11" width="16" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:11" ht="20.100000000000001" customHeight="1">
+    <row r="1" spans="1:11" ht="20" customHeight="1">
       <c r="A1" s="2" t="s">
         <v>4</v>
       </c>
@@ -2143,7 +2645,7 @@
         <v>3</v>
       </c>
     </row>
-    <row r="2" spans="1:11" ht="20.100000000000001" customHeight="1">
+    <row r="2" spans="1:11" ht="20" customHeight="1">
       <c r="A2" s="4">
         <v>394</v>
       </c>
@@ -2173,13 +2675,13 @@
   </sheetData>
   <phoneticPr fontId="1" type="noConversion"/>
   <conditionalFormatting sqref="D2">
-    <cfRule type="expression" dxfId="11" priority="1">
+    <cfRule type="expression" dxfId="14" priority="1">
       <formula>D2="Easy"</formula>
     </cfRule>
-    <cfRule type="expression" dxfId="10" priority="2">
+    <cfRule type="expression" dxfId="13" priority="2">
       <formula>D2="Medium"</formula>
     </cfRule>
-    <cfRule type="expression" dxfId="9" priority="3">
+    <cfRule type="expression" dxfId="12" priority="3">
       <formula>D2="Hard"</formula>
     </cfRule>
   </conditionalFormatting>
@@ -2194,17 +2696,17 @@
 </worksheet>
 </file>
 
-<file path=xl/worksheets/sheet5.xml><?xml version="1.0" encoding="utf-8"?>
+<file path=xl/worksheets/sheet6.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{52261E16-6011-467F-965D-8624702367C9}">
   <dimension ref="A1:K10"/>
   <sheetViews>
     <sheetView zoomScaleNormal="100" workbookViewId="0"/>
   </sheetViews>
-  <sheetFormatPr defaultColWidth="9" defaultRowHeight="16.5"/>
+  <sheetFormatPr baseColWidth="10" defaultColWidth="9" defaultRowHeight="17"/>
   <cols>
     <col min="1" max="1" width="11" customWidth="1"/>
     <col min="2" max="2" width="46" customWidth="1"/>
-    <col min="3" max="3" width="65.85546875" style="9" customWidth="1"/>
+    <col min="3" max="3" width="65.796875" style="9" customWidth="1"/>
     <col min="4" max="4" width="16" customWidth="1"/>
     <col min="5" max="5" width="36" customWidth="1"/>
     <col min="6" max="8" width="21" customWidth="1"/>
@@ -2212,7 +2714,7 @@
     <col min="11" max="11" width="16" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:11" ht="20.100000000000001" customHeight="1">
+    <row r="1" spans="1:11" ht="20" customHeight="1">
       <c r="A1" s="2" t="s">
         <v>4</v>
       </c>
@@ -2247,7 +2749,7 @@
         <v>3</v>
       </c>
     </row>
-    <row r="2" spans="1:11" ht="20.100000000000001" customHeight="1">
+    <row r="2" spans="1:11" ht="20" customHeight="1">
       <c r="A2" s="4">
         <v>208</v>
       </c>
@@ -2274,7 +2776,7 @@
       <c r="J2" s="5"/>
       <c r="K2" s="4"/>
     </row>
-    <row r="3" spans="1:11" ht="20.100000000000001" customHeight="1">
+    <row r="3" spans="1:11" ht="20" customHeight="1">
       <c r="A3" s="4">
         <v>211</v>
       </c>
@@ -2303,7 +2805,7 @@
       <c r="J3" s="5"/>
       <c r="K3" s="4"/>
     </row>
-    <row r="4" spans="1:11" ht="20.100000000000001" customHeight="1">
+    <row r="4" spans="1:11" ht="20" customHeight="1">
       <c r="A4" s="4">
         <v>386</v>
       </c>
@@ -2332,7 +2834,7 @@
       <c r="J4" s="5"/>
       <c r="K4" s="4"/>
     </row>
-    <row r="5" spans="1:11" ht="20.100000000000001" customHeight="1">
+    <row r="5" spans="1:11" ht="20" customHeight="1">
       <c r="A5" s="4">
         <v>648</v>
       </c>
@@ -2359,7 +2861,7 @@
       <c r="J5" s="5"/>
       <c r="K5" s="4"/>
     </row>
-    <row r="6" spans="1:11" ht="20.100000000000001" customHeight="1">
+    <row r="6" spans="1:11" ht="20" customHeight="1">
       <c r="A6" s="4">
         <v>677</v>
       </c>
@@ -2388,7 +2890,7 @@
       <c r="J6" s="5"/>
       <c r="K6" s="4"/>
     </row>
-    <row r="7" spans="1:11" ht="20.100000000000001" customHeight="1">
+    <row r="7" spans="1:11" ht="20" customHeight="1">
       <c r="A7" s="4">
         <v>720</v>
       </c>
@@ -2446,7 +2948,7 @@
       <c r="J8" s="5"/>
       <c r="K8" s="4"/>
     </row>
-    <row r="9" spans="1:11" ht="20.100000000000001" customHeight="1">
+    <row r="9" spans="1:11" ht="20" customHeight="1">
       <c r="A9" s="4">
         <v>1268</v>
       </c>
@@ -2507,13 +3009,13 @@
   </sheetData>
   <phoneticPr fontId="1" type="noConversion"/>
   <conditionalFormatting sqref="D2:D10">
-    <cfRule type="expression" dxfId="8" priority="1">
+    <cfRule type="expression" dxfId="11" priority="1">
       <formula>D2="Easy"</formula>
     </cfRule>
-    <cfRule type="expression" dxfId="7" priority="2">
+    <cfRule type="expression" dxfId="10" priority="2">
       <formula>D2="Medium"</formula>
     </cfRule>
-    <cfRule type="expression" dxfId="6" priority="3">
+    <cfRule type="expression" dxfId="9" priority="3">
       <formula>D2="Hard"</formula>
     </cfRule>
   </conditionalFormatting>
@@ -2536,17 +3038,17 @@
 </worksheet>
 </file>
 
-<file path=xl/worksheets/sheet6.xml><?xml version="1.0" encoding="utf-8"?>
+<file path=xl/worksheets/sheet7.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{C287181F-E765-1C4E-B964-9C9FDBE62A17}">
-  <dimension ref="A1:K13"/>
+  <dimension ref="A1:K11"/>
   <sheetViews>
     <sheetView zoomScaleNormal="100" workbookViewId="0"/>
   </sheetViews>
-  <sheetFormatPr defaultColWidth="9" defaultRowHeight="16.5"/>
+  <sheetFormatPr baseColWidth="10" defaultColWidth="9" defaultRowHeight="16"/>
   <cols>
     <col min="1" max="1" width="11" customWidth="1"/>
     <col min="2" max="2" width="36" customWidth="1"/>
-    <col min="3" max="3" width="35.85546875" style="12" customWidth="1"/>
+    <col min="3" max="3" width="35.796875" style="12" customWidth="1"/>
     <col min="4" max="4" width="16" customWidth="1"/>
     <col min="5" max="5" width="36" customWidth="1"/>
     <col min="6" max="8" width="21" customWidth="1"/>
@@ -2554,7 +3056,7 @@
     <col min="11" max="11" width="16" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:11" ht="20.100000000000001" customHeight="1">
+    <row r="1" spans="1:11" ht="20" customHeight="1">
       <c r="A1" s="2" t="s">
         <v>4</v>
       </c>
@@ -2589,7 +3091,7 @@
         <v>3</v>
       </c>
     </row>
-    <row r="2" spans="1:11" ht="20.100000000000001" customHeight="1">
+    <row r="2" spans="1:11" ht="20" customHeight="1">
       <c r="A2" s="4">
         <v>113</v>
       </c>
@@ -2618,7 +3120,7 @@
       <c r="J2" s="5"/>
       <c r="K2" s="4"/>
     </row>
-    <row r="3" spans="1:11" ht="20.100000000000001" customHeight="1">
+    <row r="3" spans="1:11" ht="20" customHeight="1">
       <c r="A3" s="4">
         <v>114</v>
       </c>
@@ -2647,7 +3149,7 @@
       <c r="J3" s="5"/>
       <c r="K3" s="4"/>
     </row>
-    <row r="4" spans="1:11" ht="20.100000000000001" customHeight="1">
+    <row r="4" spans="1:11" ht="20" customHeight="1">
       <c r="A4" s="4">
         <v>129</v>
       </c>
@@ -2676,7 +3178,7 @@
       <c r="J4" s="5"/>
       <c r="K4" s="4"/>
     </row>
-    <row r="5" spans="1:11" ht="20.100000000000001" customHeight="1">
+    <row r="5" spans="1:11" ht="20" customHeight="1">
       <c r="A5" s="4">
         <v>341</v>
       </c>
@@ -2705,7 +3207,7 @@
       <c r="J5" s="5"/>
       <c r="K5" s="4"/>
     </row>
-    <row r="6" spans="1:11" ht="20.100000000000001" customHeight="1">
+    <row r="6" spans="1:11" ht="20" customHeight="1">
       <c r="A6" s="4">
         <v>399</v>
       </c>
@@ -2736,7 +3238,7 @@
       <c r="J6" s="5"/>
       <c r="K6" s="4"/>
     </row>
-    <row r="7" spans="1:11" ht="20.100000000000001" customHeight="1">
+    <row r="7" spans="1:11" ht="20" customHeight="1">
       <c r="A7" s="4">
         <v>437</v>
       </c>
@@ -2765,7 +3267,7 @@
       <c r="J7" s="5"/>
       <c r="K7" s="4"/>
     </row>
-    <row r="8" spans="1:11" ht="20.100000000000001" customHeight="1">
+    <row r="8" spans="1:11" ht="20" customHeight="1">
       <c r="A8" s="4">
         <v>508</v>
       </c>
@@ -2794,15 +3296,15 @@
       <c r="J8" s="5"/>
       <c r="K8" s="4"/>
     </row>
-    <row r="9" spans="1:11" ht="20.100000000000001" customHeight="1">
+    <row r="9" spans="1:11" ht="20" customHeight="1">
       <c r="A9" s="4">
-        <v>513</v>
+        <v>623</v>
       </c>
       <c r="B9" s="4" t="s">
-        <v>104</v>
+        <v>113</v>
       </c>
       <c r="C9" s="11" t="s">
-        <v>105</v>
+        <v>114</v>
       </c>
       <c r="D9" s="4" t="s">
         <v>49</v>
@@ -2818,25 +3320,27 @@
         <v>29</v>
       </c>
       <c r="I9" s="5">
-        <v>45487</v>
+        <v>45488</v>
       </c>
       <c r="J9" s="5"/>
       <c r="K9" s="4"/>
     </row>
-    <row r="10" spans="1:11" ht="20.100000000000001" customHeight="1">
+    <row r="10" spans="1:11" ht="30" customHeight="1">
       <c r="A10" s="4">
-        <v>515</v>
+        <v>652</v>
       </c>
       <c r="B10" s="4" t="s">
-        <v>111</v>
+        <v>115</v>
       </c>
       <c r="C10" s="11" t="s">
-        <v>112</v>
+        <v>116</v>
       </c>
       <c r="D10" s="4" t="s">
         <v>49</v>
       </c>
-      <c r="E10" s="4"/>
+      <c r="E10" s="6" t="s">
+        <v>117</v>
+      </c>
       <c r="F10" s="4" t="s">
         <v>106</v>
       </c>
@@ -2844,7 +3348,7 @@
         <v>44</v>
       </c>
       <c r="H10" s="4" t="s">
-        <v>14</v>
+        <v>44</v>
       </c>
       <c r="I10" s="5">
         <v>45488</v>
@@ -2852,20 +3356,22 @@
       <c r="J10" s="5"/>
       <c r="K10" s="4"/>
     </row>
-    <row r="11" spans="1:11" ht="20.100000000000001" customHeight="1">
+    <row r="11" spans="1:11" ht="30" customHeight="1">
       <c r="A11" s="4">
-        <v>623</v>
+        <v>687</v>
       </c>
       <c r="B11" s="4" t="s">
-        <v>113</v>
+        <v>118</v>
       </c>
       <c r="C11" s="11" t="s">
-        <v>114</v>
+        <v>119</v>
       </c>
       <c r="D11" s="4" t="s">
         <v>49</v>
       </c>
-      <c r="E11" s="4"/>
+      <c r="E11" s="6" t="s">
+        <v>120</v>
+      </c>
       <c r="F11" s="4" t="s">
         <v>106</v>
       </c>
@@ -2881,78 +3387,16 @@
       <c r="J11" s="5"/>
       <c r="K11" s="4"/>
     </row>
-    <row r="12" spans="1:11" ht="30" customHeight="1">
-      <c r="A12" s="4">
-        <v>652</v>
-      </c>
-      <c r="B12" s="4" t="s">
-        <v>115</v>
-      </c>
-      <c r="C12" s="11" t="s">
-        <v>116</v>
-      </c>
-      <c r="D12" s="4" t="s">
-        <v>49</v>
-      </c>
-      <c r="E12" s="6" t="s">
-        <v>117</v>
-      </c>
-      <c r="F12" s="4" t="s">
-        <v>106</v>
-      </c>
-      <c r="G12" s="4" t="s">
-        <v>44</v>
-      </c>
-      <c r="H12" s="4" t="s">
-        <v>44</v>
-      </c>
-      <c r="I12" s="5">
-        <v>45488</v>
-      </c>
-      <c r="J12" s="5"/>
-      <c r="K12" s="4"/>
-    </row>
-    <row r="13" spans="1:11" ht="30" customHeight="1">
-      <c r="A13" s="4">
-        <v>687</v>
-      </c>
-      <c r="B13" s="4" t="s">
-        <v>118</v>
-      </c>
-      <c r="C13" s="11" t="s">
-        <v>119</v>
-      </c>
-      <c r="D13" s="4" t="s">
-        <v>49</v>
-      </c>
-      <c r="E13" s="6" t="s">
-        <v>120</v>
-      </c>
-      <c r="F13" s="4" t="s">
-        <v>106</v>
-      </c>
-      <c r="G13" s="4" t="s">
-        <v>44</v>
-      </c>
-      <c r="H13" s="4" t="s">
-        <v>29</v>
-      </c>
-      <c r="I13" s="5">
-        <v>45488</v>
-      </c>
-      <c r="J13" s="5"/>
-      <c r="K13" s="4"/>
-    </row>
   </sheetData>
   <phoneticPr fontId="1" type="noConversion"/>
-  <conditionalFormatting sqref="D2:D13">
-    <cfRule type="expression" dxfId="5" priority="1">
+  <conditionalFormatting sqref="D2:D11">
+    <cfRule type="expression" dxfId="8" priority="1">
       <formula>D2="Easy"</formula>
     </cfRule>
-    <cfRule type="expression" dxfId="4" priority="2">
+    <cfRule type="expression" dxfId="7" priority="2">
       <formula>D2="Medium"</formula>
     </cfRule>
-    <cfRule type="expression" dxfId="3" priority="3">
+    <cfRule type="expression" dxfId="6" priority="3">
       <formula>D2="Hard"</formula>
     </cfRule>
   </conditionalFormatting>
@@ -2961,34 +3405,32 @@
     <hyperlink ref="C3" r:id="rId2" xr:uid="{75408504-4022-5F46-87C2-C45DD0C84D7E}"/>
     <hyperlink ref="C4" r:id="rId3" xr:uid="{58EBA3C8-38C3-AD4D-86B6-2BD56DBBCDCD}"/>
     <hyperlink ref="C5" r:id="rId4" xr:uid="{63AC3368-EC03-1949-9ACD-8B642757EADB}"/>
-    <hyperlink ref="C9" r:id="rId5" xr:uid="{2E17F9D2-5401-784D-B0AE-3D6983893C12}"/>
-    <hyperlink ref="C7" r:id="rId6" xr:uid="{5CC483BA-CBD2-634B-808B-DA60BB15872A}"/>
-    <hyperlink ref="C8" r:id="rId7" xr:uid="{3C24C6AF-34E6-D142-95AA-D541F8679AD8}"/>
-    <hyperlink ref="C10" r:id="rId8" xr:uid="{8EE9509C-DFBF-7B45-85D3-B7096029C524}"/>
-    <hyperlink ref="C11" r:id="rId9" xr:uid="{DC0AB236-A846-624D-8598-9984C67224C0}"/>
-    <hyperlink ref="C12" r:id="rId10" xr:uid="{92D47051-6BA8-D549-944F-00B0154554E6}"/>
-    <hyperlink ref="C13" r:id="rId11" xr:uid="{CBAD603C-7336-874C-B3F7-58227D327CE0}"/>
-    <hyperlink ref="C6" r:id="rId12" xr:uid="{98CD3759-6763-4A59-8FC7-20CD817AC0B4}"/>
+    <hyperlink ref="C7" r:id="rId5" xr:uid="{5CC483BA-CBD2-634B-808B-DA60BB15872A}"/>
+    <hyperlink ref="C8" r:id="rId6" xr:uid="{3C24C6AF-34E6-D142-95AA-D541F8679AD8}"/>
+    <hyperlink ref="C9" r:id="rId7" xr:uid="{DC0AB236-A846-624D-8598-9984C67224C0}"/>
+    <hyperlink ref="C10" r:id="rId8" xr:uid="{92D47051-6BA8-D549-944F-00B0154554E6}"/>
+    <hyperlink ref="C11" r:id="rId9" xr:uid="{CBAD603C-7336-874C-B3F7-58227D327CE0}"/>
+    <hyperlink ref="C6" r:id="rId10" xr:uid="{98CD3759-6763-4A59-8FC7-20CD817AC0B4}"/>
   </hyperlinks>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
-  <pageSetup paperSize="9" orientation="portrait" verticalDpi="0" r:id="rId13"/>
+  <pageSetup paperSize="9" orientation="portrait" verticalDpi="0" r:id="rId11"/>
   <headerFooter>
     <oddFooter>&amp;L_x000D_&amp;1#&amp;"Calibri"&amp;10&amp;K000000 General</oddFooter>
   </headerFooter>
 </worksheet>
 </file>
 
-<file path=xl/worksheets/sheet7.xml><?xml version="1.0" encoding="utf-8"?>
+<file path=xl/worksheets/sheet8.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{75AC292A-7720-E145-9563-F6FD48AA33E3}">
-  <dimension ref="A1:K8"/>
+  <dimension ref="A1:K10"/>
   <sheetViews>
-    <sheetView tabSelected="1" zoomScaleNormal="100" workbookViewId="0"/>
+    <sheetView zoomScaleNormal="100" workbookViewId="0"/>
   </sheetViews>
-  <sheetFormatPr defaultColWidth="9" defaultRowHeight="16.5"/>
+  <sheetFormatPr baseColWidth="10" defaultColWidth="9" defaultRowHeight="16"/>
   <cols>
     <col min="1" max="1" width="11" customWidth="1"/>
-    <col min="2" max="2" width="43.28515625" customWidth="1"/>
-    <col min="3" max="3" width="35.85546875" style="12" customWidth="1"/>
+    <col min="2" max="2" width="43.19921875" customWidth="1"/>
+    <col min="3" max="3" width="35.796875" style="12" customWidth="1"/>
     <col min="4" max="4" width="16" customWidth="1"/>
     <col min="5" max="5" width="36" customWidth="1"/>
     <col min="6" max="8" width="21" customWidth="1"/>
@@ -2996,7 +3438,7 @@
     <col min="11" max="11" width="16" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:11" ht="20.100000000000001" customHeight="1">
+    <row r="1" spans="1:11" ht="20" customHeight="1">
       <c r="A1" s="2" t="s">
         <v>4</v>
       </c>
@@ -3155,80 +3597,80 @@
       <c r="J5" s="5"/>
       <c r="K5" s="4"/>
     </row>
-    <row r="6" spans="1:11" ht="30" customHeight="1">
+    <row r="6" spans="1:11" ht="20" customHeight="1">
       <c r="A6" s="4">
-        <v>662</v>
+        <v>513</v>
       </c>
       <c r="B6" s="4" t="s">
-        <v>130</v>
+        <v>104</v>
       </c>
       <c r="C6" s="11" t="s">
-        <v>131</v>
+        <v>105</v>
       </c>
       <c r="D6" s="4" t="s">
         <v>49</v>
       </c>
-      <c r="E6" s="6" t="s">
-        <v>138</v>
-      </c>
+      <c r="E6" s="4"/>
       <c r="F6" s="4" t="s">
-        <v>123</v>
+        <v>106</v>
       </c>
       <c r="G6" s="4" t="s">
         <v>44</v>
       </c>
       <c r="H6" s="4" t="s">
-        <v>44</v>
+        <v>29</v>
       </c>
       <c r="I6" s="5">
-        <v>45490</v>
+        <v>45487</v>
       </c>
       <c r="J6" s="5"/>
       <c r="K6" s="4"/>
     </row>
-    <row r="7" spans="1:11" ht="20.100000000000001" customHeight="1">
+    <row r="7" spans="1:11" ht="20" customHeight="1">
       <c r="A7" s="4">
-        <v>958</v>
+        <v>515</v>
       </c>
       <c r="B7" s="4" t="s">
-        <v>136</v>
+        <v>111</v>
       </c>
       <c r="C7" s="11" t="s">
-        <v>137</v>
+        <v>112</v>
       </c>
       <c r="D7" s="4" t="s">
         <v>49</v>
       </c>
-      <c r="E7" s="6"/>
+      <c r="E7" s="4"/>
       <c r="F7" s="4" t="s">
-        <v>123</v>
+        <v>106</v>
       </c>
       <c r="G7" s="4" t="s">
         <v>44</v>
       </c>
       <c r="H7" s="4" t="s">
-        <v>44</v>
+        <v>11</v>
       </c>
       <c r="I7" s="5">
-        <v>45491</v>
+        <v>45488</v>
       </c>
       <c r="J7" s="5"/>
       <c r="K7" s="4"/>
     </row>
-    <row r="8" spans="1:11" ht="20.100000000000001" customHeight="1">
+    <row r="8" spans="1:11" ht="30" customHeight="1">
       <c r="A8" s="4">
-        <v>1161</v>
+        <v>662</v>
       </c>
       <c r="B8" s="4" t="s">
-        <v>139</v>
+        <v>130</v>
       </c>
       <c r="C8" s="11" t="s">
-        <v>140</v>
+        <v>131</v>
       </c>
       <c r="D8" s="4" t="s">
         <v>49</v>
       </c>
-      <c r="E8" s="6"/>
+      <c r="E8" s="6" t="s">
+        <v>138</v>
+      </c>
       <c r="F8" s="4" t="s">
         <v>123</v>
       </c>
@@ -3239,22 +3681,91 @@
         <v>44</v>
       </c>
       <c r="I8" s="5">
-        <v>45491</v>
+        <v>45490</v>
       </c>
       <c r="J8" s="5"/>
       <c r="K8" s="4"/>
     </row>
+    <row r="9" spans="1:11" ht="20" customHeight="1">
+      <c r="A9" s="4">
+        <v>958</v>
+      </c>
+      <c r="B9" s="4" t="s">
+        <v>136</v>
+      </c>
+      <c r="C9" s="11" t="s">
+        <v>137</v>
+      </c>
+      <c r="D9" s="4" t="s">
+        <v>49</v>
+      </c>
+      <c r="E9" s="6"/>
+      <c r="F9" s="4" t="s">
+        <v>123</v>
+      </c>
+      <c r="G9" s="4" t="s">
+        <v>44</v>
+      </c>
+      <c r="H9" s="4" t="s">
+        <v>44</v>
+      </c>
+      <c r="I9" s="5">
+        <v>45491</v>
+      </c>
+      <c r="J9" s="5"/>
+      <c r="K9" s="4"/>
+    </row>
+    <row r="10" spans="1:11" ht="20" customHeight="1">
+      <c r="A10" s="4">
+        <v>1161</v>
+      </c>
+      <c r="B10" s="4" t="s">
+        <v>139</v>
+      </c>
+      <c r="C10" s="11" t="s">
+        <v>140</v>
+      </c>
+      <c r="D10" s="4" t="s">
+        <v>49</v>
+      </c>
+      <c r="E10" s="6"/>
+      <c r="F10" s="4" t="s">
+        <v>123</v>
+      </c>
+      <c r="G10" s="4" t="s">
+        <v>44</v>
+      </c>
+      <c r="H10" s="4" t="s">
+        <v>44</v>
+      </c>
+      <c r="I10" s="5">
+        <v>45491</v>
+      </c>
+      <c r="J10" s="5"/>
+      <c r="K10" s="4"/>
+    </row>
   </sheetData>
   <phoneticPr fontId="1" type="noConversion"/>
-  <conditionalFormatting sqref="D2:D8">
-    <cfRule type="expression" dxfId="2" priority="1">
+  <conditionalFormatting sqref="D2:D5 D8:D10">
+    <cfRule type="expression" dxfId="5" priority="4">
       <formula>D2="Easy"</formula>
     </cfRule>
-    <cfRule type="expression" dxfId="1" priority="2">
+    <cfRule type="expression" dxfId="4" priority="5">
       <formula>D2="Medium"</formula>
     </cfRule>
+    <cfRule type="expression" dxfId="3" priority="6">
+      <formula>D2="Hard"</formula>
+    </cfRule>
+  </conditionalFormatting>
+  <conditionalFormatting sqref="D6:D7">
+    <cfRule type="expression" dxfId="2" priority="1">
+      <formula>D6="Easy"</formula>
+    </cfRule>
+    <cfRule type="expression" dxfId="1" priority="2">
+      <formula>D6="Medium"</formula>
+    </cfRule>
     <cfRule type="expression" dxfId="0" priority="3">
-      <formula>D2="Hard"</formula>
+      <formula>D6="Hard"</formula>
     </cfRule>
   </conditionalFormatting>
   <hyperlinks>
@@ -3262,12 +3773,14 @@
     <hyperlink ref="C5" r:id="rId2" xr:uid="{8BC7B711-ADEB-4546-905F-7D690999B5BB}"/>
     <hyperlink ref="C2" r:id="rId3" xr:uid="{C2B4A6B6-B0D8-4F31-9802-387F04CC45FB}"/>
     <hyperlink ref="C3" r:id="rId4" xr:uid="{5615EAD9-62C1-4780-AE19-6BFAC2939521}"/>
-    <hyperlink ref="C6" r:id="rId5" xr:uid="{6D55272D-BA36-4797-A7CF-581EE973B392}"/>
-    <hyperlink ref="C7" r:id="rId6" xr:uid="{A382170A-F086-4927-B656-868CCD453ABF}"/>
-    <hyperlink ref="C8" r:id="rId7" xr:uid="{25BA1857-5CC6-4D6B-94BB-2E650759A139}"/>
+    <hyperlink ref="C8" r:id="rId5" xr:uid="{6D55272D-BA36-4797-A7CF-581EE973B392}"/>
+    <hyperlink ref="C9" r:id="rId6" xr:uid="{A382170A-F086-4927-B656-868CCD453ABF}"/>
+    <hyperlink ref="C10" r:id="rId7" xr:uid="{25BA1857-5CC6-4D6B-94BB-2E650759A139}"/>
+    <hyperlink ref="C6" r:id="rId8" xr:uid="{2E17F9D2-5401-784D-B0AE-3D6983893C12}"/>
+    <hyperlink ref="C7" r:id="rId9" xr:uid="{8EE9509C-DFBF-7B45-85D3-B7096029C524}"/>
   </hyperlinks>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
-  <pageSetup paperSize="9" orientation="portrait" verticalDpi="0" r:id="rId8"/>
+  <pageSetup paperSize="9" orientation="portrait" verticalDpi="0" r:id="rId10"/>
   <headerFooter>
     <oddFooter>&amp;L_x000D_&amp;1#&amp;"Calibri"&amp;10&amp;K000000 General</oddFooter>
   </headerFooter>

</xml_diff>

<commit_message>
Completed several hard practices.
</commit_message>
<xml_diff>
--- a/LeetCode Techniques.xlsx
+++ b/LeetCode Techniques.xlsx
@@ -1,16 +1,16 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
-  <fileVersion appName="xl" lastEdited="7" lowestEdited="4" rupBuild="27328"/>
+  <fileVersion appName="xl" lastEdited="7" lowestEdited="4" rupBuild="10714"/>
   <workbookPr defaultThemeVersion="124226"/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\jack.yao\Desktop\LeetCode\"/>
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="/Users/blackjack625/Desktop/LeetCode/"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{6D82DA80-7DD6-455C-899F-64FB20D4CE3C}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{D2E7134D-1C74-634B-B161-D5D0EEF4D56F}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="-120" yWindow="-120" windowWidth="20640" windowHeight="11040" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
+    <workbookView xWindow="0" yWindow="0" windowWidth="28800" windowHeight="18000" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
   <sheets>
     <sheet name="Dynamic Programming" sheetId="8" r:id="rId1"/>
@@ -658,6 +658,7 @@
         <sz val="10"/>
         <color theme="1"/>
         <rFont val="Microsoft YaHei"/>
+        <charset val="134"/>
       </rPr>
       <t>2</t>
     </r>
@@ -780,6 +781,7 @@
         <sz val="10"/>
         <color theme="1"/>
         <rFont val="Microsoft YaHei"/>
+        <charset val="134"/>
       </rPr>
       <t>querying target - num permutation</t>
     </r>
@@ -799,6 +801,7 @@
         <sz val="10"/>
         <color theme="1"/>
         <rFont val="Microsoft YaHei"/>
+        <charset val="134"/>
       </rPr>
       <t>just sum up to record permutations</t>
     </r>
@@ -822,19 +825,19 @@
 <file path=xl/styles.xml><?xml version="1.0" encoding="utf-8"?>
 <styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:x16r2="http://schemas.microsoft.com/office/spreadsheetml/2015/02/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" mc:Ignorable="x14ac x16r2 xr">
   <numFmts count="1">
-    <numFmt numFmtId="164" formatCode="yyyy&quot;年&quot;m&quot;月&quot;d&quot;日&quot;;@"/>
+    <numFmt numFmtId="176" formatCode="yyyy&quot;年&quot;m&quot;月&quot;d&quot;日&quot;;@"/>
   </numFmts>
   <fonts count="14">
     <font>
       <sz val="11"/>
       <color theme="1"/>
-      <name val="Calibri"/>
+      <name val="新細明體"/>
       <family val="2"/>
       <scheme val="minor"/>
     </font>
     <font>
       <sz val="9"/>
-      <name val="Calibri"/>
+      <name val="新細明體"/>
       <family val="2"/>
       <charset val="136"/>
       <scheme val="minor"/>
@@ -858,7 +861,7 @@
       <u/>
       <sz val="11"/>
       <color theme="10"/>
-      <name val="Calibri"/>
+      <name val="新細明體"/>
       <family val="2"/>
       <scheme val="minor"/>
     </font>
@@ -907,18 +910,21 @@
       <sz val="10"/>
       <color theme="1"/>
       <name val="Microsoft YaHei"/>
+      <charset val="134"/>
     </font>
     <font>
       <b/>
       <sz val="10"/>
       <color theme="1"/>
       <name val="Microsoft YaHei"/>
+      <charset val="134"/>
     </font>
     <font>
       <u/>
       <sz val="10"/>
       <color theme="10"/>
       <name val="Microsoft YaHei"/>
+      <charset val="134"/>
     </font>
   </fonts>
   <fills count="2">
@@ -959,17 +965,17 @@
   </cellStyleXfs>
   <cellXfs count="17">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
-    <xf numFmtId="164" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1"/>
+    <xf numFmtId="176" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1"/>
     <xf numFmtId="0" fontId="2" fillId="0" borderId="1" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
     </xf>
-    <xf numFmtId="164" fontId="2" fillId="0" borderId="1" xfId="0" applyNumberFormat="1" applyFont="1" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="176" fontId="2" fillId="0" borderId="1" xfId="0" applyNumberFormat="1" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
     </xf>
     <xf numFmtId="0" fontId="3" fillId="0" borderId="1" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
     </xf>
-    <xf numFmtId="164" fontId="3" fillId="0" borderId="1" xfId="0" applyNumberFormat="1" applyFont="1" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="176" fontId="3" fillId="0" borderId="1" xfId="0" applyNumberFormat="1" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
     </xf>
     <xf numFmtId="0" fontId="3" fillId="0" borderId="1" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
@@ -1001,40 +1007,10 @@
     </xf>
   </cellXfs>
   <cellStyles count="2">
-    <cellStyle name="Hyperlink" xfId="1" builtinId="8"/>
-    <cellStyle name="Normal" xfId="0" builtinId="0"/>
+    <cellStyle name="一般" xfId="0" builtinId="0"/>
+    <cellStyle name="超連結" xfId="1" builtinId="8"/>
   </cellStyles>
-  <dxfs count="33">
-    <dxf>
-      <font>
-        <color rgb="FFFFFF00"/>
-      </font>
-      <fill>
-        <patternFill>
-          <bgColor rgb="FFFF0000"/>
-        </patternFill>
-      </fill>
-    </dxf>
-    <dxf>
-      <font>
-        <color theme="1"/>
-      </font>
-      <fill>
-        <patternFill>
-          <bgColor rgb="FFFFFF00"/>
-        </patternFill>
-      </fill>
-    </dxf>
-    <dxf>
-      <font>
-        <color theme="0"/>
-      </font>
-      <fill>
-        <patternFill>
-          <bgColor rgb="FF00B050"/>
-        </patternFill>
-      </fill>
-    </dxf>
+  <dxfs count="30">
     <dxf>
       <font>
         <color rgb="FFFFFF00"/>
@@ -1639,11 +1615,11 @@
   <sheetViews>
     <sheetView tabSelected="1" zoomScaleNormal="100" workbookViewId="0"/>
   </sheetViews>
-  <sheetFormatPr defaultColWidth="9" defaultRowHeight="16.5"/>
+  <sheetFormatPr baseColWidth="10" defaultColWidth="9" defaultRowHeight="16"/>
   <cols>
     <col min="1" max="1" width="11" customWidth="1"/>
-    <col min="2" max="2" width="30.7109375" customWidth="1"/>
-    <col min="3" max="3" width="40.7109375" style="15" customWidth="1"/>
+    <col min="2" max="2" width="36" customWidth="1"/>
+    <col min="3" max="3" width="40.796875" style="15" customWidth="1"/>
     <col min="4" max="4" width="16" customWidth="1"/>
     <col min="5" max="5" width="36" customWidth="1"/>
     <col min="6" max="8" width="21" customWidth="1"/>
@@ -1651,7 +1627,7 @@
     <col min="11" max="11" width="16" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:11" ht="20.100000000000001" customHeight="1">
+    <row r="1" spans="1:11" ht="20" customHeight="1">
       <c r="A1" s="2" t="s">
         <v>4</v>
       </c>
@@ -1686,7 +1662,7 @@
         <v>3</v>
       </c>
     </row>
-    <row r="2" spans="1:11" ht="20.100000000000001" customHeight="1">
+    <row r="2" spans="1:11" ht="20" customHeight="1">
       <c r="A2" s="4">
         <v>53</v>
       </c>
@@ -1713,7 +1689,7 @@
       <c r="J2" s="5"/>
       <c r="K2" s="4"/>
     </row>
-    <row r="3" spans="1:11" ht="20.100000000000001" customHeight="1">
+    <row r="3" spans="1:11" ht="20" customHeight="1">
       <c r="A3" s="4">
         <v>62</v>
       </c>
@@ -1769,7 +1745,7 @@
       <c r="J4" s="5"/>
       <c r="K4" s="4"/>
     </row>
-    <row r="5" spans="1:11" ht="20.100000000000001" customHeight="1">
+    <row r="5" spans="1:11" ht="20" customHeight="1">
       <c r="A5" s="4">
         <v>64</v>
       </c>
@@ -1796,7 +1772,7 @@
       <c r="J5" s="5"/>
       <c r="K5" s="4"/>
     </row>
-    <row r="6" spans="1:11" ht="20.100000000000001" customHeight="1">
+    <row r="6" spans="1:11" ht="20" customHeight="1">
       <c r="A6" s="4">
         <v>120</v>
       </c>
@@ -1883,7 +1859,7 @@
       <c r="J8" s="5"/>
       <c r="K8" s="4"/>
     </row>
-    <row r="9" spans="1:11" ht="20.100000000000001" customHeight="1">
+    <row r="9" spans="1:11" ht="20" customHeight="1">
       <c r="A9" s="4">
         <v>198</v>
       </c>
@@ -1943,7 +1919,7 @@
       <c r="J10" s="5"/>
       <c r="K10" s="4"/>
     </row>
-    <row r="11" spans="1:11" ht="20.100000000000001" customHeight="1">
+    <row r="11" spans="1:11" ht="20" customHeight="1">
       <c r="A11" s="4">
         <v>279</v>
       </c>
@@ -2032,7 +2008,7 @@
       <c r="J13" s="5"/>
       <c r="K13" s="4"/>
     </row>
-    <row r="14" spans="1:11" ht="20.100000000000001" customHeight="1">
+    <row r="14" spans="1:11" ht="20" customHeight="1">
       <c r="A14" s="4">
         <v>343</v>
       </c>
@@ -2119,7 +2095,7 @@
       <c r="J16" s="5"/>
       <c r="K16" s="4"/>
     </row>
-    <row r="17" spans="1:11" ht="20.100000000000001" customHeight="1">
+    <row r="17" spans="1:11" ht="20" customHeight="1">
       <c r="A17" s="4">
         <v>931</v>
       </c>
@@ -2180,13 +2156,13 @@
   </sheetData>
   <phoneticPr fontId="1" type="noConversion"/>
   <conditionalFormatting sqref="D2:D18">
-    <cfRule type="expression" dxfId="32" priority="1">
+    <cfRule type="expression" dxfId="29" priority="1">
       <formula>D2="Easy"</formula>
     </cfRule>
-    <cfRule type="expression" dxfId="31" priority="2">
+    <cfRule type="expression" dxfId="28" priority="2">
       <formula>D2="Medium"</formula>
     </cfRule>
-    <cfRule type="expression" dxfId="30" priority="3">
+    <cfRule type="expression" dxfId="27" priority="3">
       <formula>D2="Hard"</formula>
     </cfRule>
   </conditionalFormatting>
@@ -2223,10 +2199,10 @@
   <sheetViews>
     <sheetView zoomScaleNormal="100" workbookViewId="0"/>
   </sheetViews>
-  <sheetFormatPr defaultColWidth="9" defaultRowHeight="16.5"/>
+  <sheetFormatPr baseColWidth="10" defaultColWidth="9" defaultRowHeight="17"/>
   <cols>
     <col min="1" max="1" width="11" customWidth="1"/>
-    <col min="2" max="2" width="38.140625" customWidth="1"/>
+    <col min="2" max="2" width="38.19921875" customWidth="1"/>
     <col min="3" max="3" width="71" style="9" customWidth="1"/>
     <col min="4" max="4" width="16" customWidth="1"/>
     <col min="5" max="5" width="36" customWidth="1"/>
@@ -2235,7 +2211,7 @@
     <col min="11" max="11" width="16" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:11" ht="20.100000000000001" customHeight="1">
+    <row r="1" spans="1:11" ht="20" customHeight="1">
       <c r="A1" s="2" t="s">
         <v>4</v>
       </c>
@@ -2270,7 +2246,7 @@
         <v>3</v>
       </c>
     </row>
-    <row r="2" spans="1:11" ht="20.100000000000001" customHeight="1">
+    <row r="2" spans="1:11" ht="20" customHeight="1">
       <c r="A2" s="4">
         <v>74</v>
       </c>
@@ -2297,7 +2273,7 @@
       <c r="J2" s="3"/>
       <c r="K2" s="2"/>
     </row>
-    <row r="3" spans="1:11" ht="20.100000000000001" customHeight="1">
+    <row r="3" spans="1:11" ht="20" customHeight="1">
       <c r="A3" s="4">
         <v>220</v>
       </c>
@@ -2353,7 +2329,7 @@
       <c r="J4" s="5"/>
       <c r="K4" s="4"/>
     </row>
-    <row r="5" spans="1:11" ht="20.100000000000001" customHeight="1">
+    <row r="5" spans="1:11" ht="20" customHeight="1">
       <c r="A5" s="4">
         <v>315</v>
       </c>
@@ -2380,7 +2356,7 @@
       <c r="J5" s="5"/>
       <c r="K5" s="4"/>
     </row>
-    <row r="6" spans="1:11" ht="20.100000000000001" customHeight="1">
+    <row r="6" spans="1:11" ht="20" customHeight="1">
       <c r="A6" s="4">
         <v>352</v>
       </c>
@@ -2409,7 +2385,7 @@
       <c r="J6" s="5"/>
       <c r="K6" s="4"/>
     </row>
-    <row r="7" spans="1:11" ht="20.100000000000001" customHeight="1">
+    <row r="7" spans="1:11" ht="20" customHeight="1">
       <c r="A7" s="4">
         <v>480</v>
       </c>
@@ -2436,7 +2412,7 @@
       <c r="J7" s="5"/>
       <c r="K7" s="4"/>
     </row>
-    <row r="8" spans="1:11" ht="20.100000000000001" customHeight="1">
+    <row r="8" spans="1:11" ht="20" customHeight="1">
       <c r="A8" s="4">
         <v>493</v>
       </c>
@@ -2463,7 +2439,7 @@
       <c r="J8" s="5"/>
       <c r="K8" s="4"/>
     </row>
-    <row r="9" spans="1:11" ht="20.100000000000001" customHeight="1">
+    <row r="9" spans="1:11" ht="20" customHeight="1">
       <c r="A9" s="4">
         <v>611</v>
       </c>
@@ -2492,7 +2468,7 @@
       <c r="J9" s="5"/>
       <c r="K9" s="4"/>
     </row>
-    <row r="10" spans="1:11" ht="20.100000000000001" customHeight="1">
+    <row r="10" spans="1:11" ht="20" customHeight="1">
       <c r="A10" s="4">
         <v>729</v>
       </c>
@@ -2519,7 +2495,7 @@
       <c r="J10" s="5"/>
       <c r="K10" s="4"/>
     </row>
-    <row r="11" spans="1:11" ht="20.100000000000001" customHeight="1">
+    <row r="11" spans="1:11" ht="20" customHeight="1">
       <c r="A11" s="4">
         <v>1095</v>
       </c>
@@ -2577,7 +2553,7 @@
       <c r="J12" s="5"/>
       <c r="K12" s="4"/>
     </row>
-    <row r="13" spans="1:11" ht="20.100000000000001" customHeight="1">
+    <row r="13" spans="1:11" ht="20" customHeight="1">
       <c r="A13" s="4">
         <v>1825</v>
       </c>
@@ -2606,7 +2582,7 @@
       <c r="J13" s="5"/>
       <c r="K13" s="4"/>
     </row>
-    <row r="14" spans="1:11" ht="20.100000000000001" customHeight="1">
+    <row r="14" spans="1:11" ht="20" customHeight="1">
       <c r="A14" s="4">
         <v>2034</v>
       </c>
@@ -2635,7 +2611,7 @@
       <c r="J14" s="5"/>
       <c r="K14" s="4"/>
     </row>
-    <row r="15" spans="1:11" ht="20.100000000000001" customHeight="1">
+    <row r="15" spans="1:11" ht="20" customHeight="1">
       <c r="A15" s="4">
         <v>2102</v>
       </c>
@@ -2670,24 +2646,24 @@
   </sortState>
   <phoneticPr fontId="1" type="noConversion"/>
   <conditionalFormatting sqref="D2:D3">
-    <cfRule type="expression" dxfId="29" priority="1">
+    <cfRule type="expression" dxfId="26" priority="1">
       <formula>D2="Easy"</formula>
     </cfRule>
-    <cfRule type="expression" dxfId="28" priority="2">
+    <cfRule type="expression" dxfId="25" priority="2">
       <formula>D2="Medium"</formula>
     </cfRule>
-    <cfRule type="expression" dxfId="27" priority="3">
+    <cfRule type="expression" dxfId="24" priority="3">
       <formula>D2="Hard"</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="D4:E15">
-    <cfRule type="expression" dxfId="26" priority="4">
+    <cfRule type="expression" dxfId="23" priority="4">
       <formula>D4="Easy"</formula>
     </cfRule>
-    <cfRule type="expression" dxfId="25" priority="5">
+    <cfRule type="expression" dxfId="22" priority="5">
       <formula>D4="Medium"</formula>
     </cfRule>
-    <cfRule type="expression" dxfId="24" priority="6">
+    <cfRule type="expression" dxfId="21" priority="6">
       <formula>D4="Hard"</formula>
     </cfRule>
   </conditionalFormatting>
@@ -2720,10 +2696,10 @@
   <sheetViews>
     <sheetView zoomScaleNormal="100" workbookViewId="0"/>
   </sheetViews>
-  <sheetFormatPr defaultColWidth="9" defaultRowHeight="16.5"/>
+  <sheetFormatPr baseColWidth="10" defaultColWidth="9" defaultRowHeight="17"/>
   <cols>
     <col min="1" max="1" width="11" customWidth="1"/>
-    <col min="2" max="2" width="45.85546875" customWidth="1"/>
+    <col min="2" max="2" width="45.796875" customWidth="1"/>
     <col min="3" max="3" width="71" style="9" customWidth="1"/>
     <col min="4" max="4" width="16" customWidth="1"/>
     <col min="5" max="5" width="36" customWidth="1"/>
@@ -2732,7 +2708,7 @@
     <col min="11" max="11" width="16" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:11" ht="20.100000000000001" customHeight="1">
+    <row r="1" spans="1:11" ht="20" customHeight="1">
       <c r="A1" s="2" t="s">
         <v>4</v>
       </c>
@@ -2767,7 +2743,7 @@
         <v>3</v>
       </c>
     </row>
-    <row r="2" spans="1:11" ht="20.100000000000001" customHeight="1">
+    <row r="2" spans="1:11" ht="20" customHeight="1">
       <c r="A2" s="4">
         <v>3</v>
       </c>
@@ -2794,7 +2770,7 @@
       <c r="J2" s="5"/>
       <c r="K2" s="4"/>
     </row>
-    <row r="3" spans="1:11" ht="20.100000000000001" customHeight="1">
+    <row r="3" spans="1:11" ht="20" customHeight="1">
       <c r="A3" s="4">
         <v>1695</v>
       </c>
@@ -2824,13 +2800,13 @@
   </sheetData>
   <phoneticPr fontId="1" type="noConversion"/>
   <conditionalFormatting sqref="D2:E3">
-    <cfRule type="expression" dxfId="23" priority="4">
+    <cfRule type="expression" dxfId="20" priority="4">
       <formula>D2="Easy"</formula>
     </cfRule>
-    <cfRule type="expression" dxfId="22" priority="5">
+    <cfRule type="expression" dxfId="19" priority="5">
       <formula>D2="Medium"</formula>
     </cfRule>
-    <cfRule type="expression" dxfId="21" priority="6">
+    <cfRule type="expression" dxfId="18" priority="6">
       <formula>D2="Hard"</formula>
     </cfRule>
   </conditionalFormatting>
@@ -2851,11 +2827,11 @@
   <sheetViews>
     <sheetView zoomScaleNormal="100" workbookViewId="0"/>
   </sheetViews>
-  <sheetFormatPr defaultColWidth="9" defaultRowHeight="16.5"/>
+  <sheetFormatPr baseColWidth="10" defaultColWidth="9" defaultRowHeight="17"/>
   <cols>
     <col min="1" max="1" width="11" customWidth="1"/>
-    <col min="2" max="2" width="25.85546875" customWidth="1"/>
-    <col min="3" max="3" width="65.85546875" style="9" customWidth="1"/>
+    <col min="2" max="2" width="25.796875" customWidth="1"/>
+    <col min="3" max="3" width="65.796875" style="9" customWidth="1"/>
     <col min="4" max="4" width="16" customWidth="1"/>
     <col min="5" max="5" width="36" customWidth="1"/>
     <col min="6" max="8" width="21" customWidth="1"/>
@@ -2863,7 +2839,7 @@
     <col min="11" max="11" width="16" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:11" ht="20.100000000000001" customHeight="1">
+    <row r="1" spans="1:11" ht="20" customHeight="1">
       <c r="A1" s="2" t="s">
         <v>4</v>
       </c>
@@ -2898,7 +2874,7 @@
         <v>3</v>
       </c>
     </row>
-    <row r="2" spans="1:11" ht="20.100000000000001" customHeight="1">
+    <row r="2" spans="1:11" ht="20" customHeight="1">
       <c r="A2" s="4">
         <v>41</v>
       </c>
@@ -2929,7 +2905,7 @@
       </c>
       <c r="K2" s="4"/>
     </row>
-    <row r="3" spans="1:11" ht="20.100000000000001" customHeight="1">
+    <row r="3" spans="1:11" ht="20" customHeight="1">
       <c r="A3" s="4">
         <v>287</v>
       </c>
@@ -2956,7 +2932,7 @@
       <c r="J3" s="5"/>
       <c r="K3" s="4"/>
     </row>
-    <row r="4" spans="1:11" ht="20.100000000000001" customHeight="1">
+    <row r="4" spans="1:11" ht="20" customHeight="1">
       <c r="A4" s="4">
         <v>645</v>
       </c>
@@ -2986,24 +2962,24 @@
   </sheetData>
   <phoneticPr fontId="1" type="noConversion"/>
   <conditionalFormatting sqref="D2">
-    <cfRule type="expression" dxfId="20" priority="1">
+    <cfRule type="expression" dxfId="17" priority="1">
       <formula>D2="Easy"</formula>
     </cfRule>
-    <cfRule type="expression" dxfId="19" priority="2">
+    <cfRule type="expression" dxfId="16" priority="2">
       <formula>D2="Medium"</formula>
     </cfRule>
-    <cfRule type="expression" dxfId="18" priority="3">
+    <cfRule type="expression" dxfId="15" priority="3">
       <formula>D2="Hard"</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="D3:E4">
-    <cfRule type="expression" dxfId="17" priority="4">
+    <cfRule type="expression" dxfId="14" priority="4">
       <formula>D3="Easy"</formula>
     </cfRule>
-    <cfRule type="expression" dxfId="16" priority="5">
+    <cfRule type="expression" dxfId="13" priority="5">
       <formula>D3="Medium"</formula>
     </cfRule>
-    <cfRule type="expression" dxfId="15" priority="6">
+    <cfRule type="expression" dxfId="12" priority="6">
       <formula>D3="Hard"</formula>
     </cfRule>
   </conditionalFormatting>
@@ -3026,11 +3002,11 @@
   <sheetViews>
     <sheetView zoomScaleNormal="100" workbookViewId="0"/>
   </sheetViews>
-  <sheetFormatPr defaultColWidth="9" defaultRowHeight="16.5"/>
+  <sheetFormatPr baseColWidth="10" defaultColWidth="9" defaultRowHeight="17"/>
   <cols>
     <col min="1" max="1" width="11" customWidth="1"/>
     <col min="2" max="2" width="16" customWidth="1"/>
-    <col min="3" max="3" width="35.85546875" style="9" customWidth="1"/>
+    <col min="3" max="3" width="35.796875" style="9" customWidth="1"/>
     <col min="4" max="4" width="16" customWidth="1"/>
     <col min="5" max="5" width="36" customWidth="1"/>
     <col min="6" max="8" width="21" customWidth="1"/>
@@ -3038,7 +3014,7 @@
     <col min="11" max="11" width="16" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:11" ht="20.100000000000001" customHeight="1">
+    <row r="1" spans="1:11" ht="20" customHeight="1">
       <c r="A1" s="2" t="s">
         <v>4</v>
       </c>
@@ -3073,7 +3049,7 @@
         <v>3</v>
       </c>
     </row>
-    <row r="2" spans="1:11" ht="20.100000000000001" customHeight="1">
+    <row r="2" spans="1:11" ht="20" customHeight="1">
       <c r="A2" s="4">
         <v>394</v>
       </c>
@@ -3103,13 +3079,13 @@
   </sheetData>
   <phoneticPr fontId="1" type="noConversion"/>
   <conditionalFormatting sqref="D2">
-    <cfRule type="expression" dxfId="14" priority="1">
+    <cfRule type="expression" dxfId="11" priority="1">
       <formula>D2="Easy"</formula>
     </cfRule>
-    <cfRule type="expression" dxfId="13" priority="2">
+    <cfRule type="expression" dxfId="10" priority="2">
       <formula>D2="Medium"</formula>
     </cfRule>
-    <cfRule type="expression" dxfId="12" priority="3">
+    <cfRule type="expression" dxfId="9" priority="3">
       <formula>D2="Hard"</formula>
     </cfRule>
   </conditionalFormatting>
@@ -3130,11 +3106,11 @@
   <sheetViews>
     <sheetView zoomScaleNormal="100" workbookViewId="0"/>
   </sheetViews>
-  <sheetFormatPr defaultColWidth="9" defaultRowHeight="16.5"/>
+  <sheetFormatPr baseColWidth="10" defaultColWidth="9" defaultRowHeight="17"/>
   <cols>
     <col min="1" max="1" width="11" customWidth="1"/>
     <col min="2" max="2" width="46" customWidth="1"/>
-    <col min="3" max="3" width="65.85546875" style="9" customWidth="1"/>
+    <col min="3" max="3" width="65.796875" style="9" customWidth="1"/>
     <col min="4" max="4" width="16" customWidth="1"/>
     <col min="5" max="5" width="36" customWidth="1"/>
     <col min="6" max="8" width="21" customWidth="1"/>
@@ -3142,7 +3118,7 @@
     <col min="11" max="11" width="16" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:11" ht="20.100000000000001" customHeight="1">
+    <row r="1" spans="1:11" ht="20" customHeight="1">
       <c r="A1" s="2" t="s">
         <v>4</v>
       </c>
@@ -3177,7 +3153,7 @@
         <v>3</v>
       </c>
     </row>
-    <row r="2" spans="1:11" ht="20.100000000000001" customHeight="1">
+    <row r="2" spans="1:11" ht="20" customHeight="1">
       <c r="A2" s="4">
         <v>208</v>
       </c>
@@ -3204,7 +3180,7 @@
       <c r="J2" s="5"/>
       <c r="K2" s="4"/>
     </row>
-    <row r="3" spans="1:11" ht="20.100000000000001" customHeight="1">
+    <row r="3" spans="1:11" ht="20" customHeight="1">
       <c r="A3" s="4">
         <v>211</v>
       </c>
@@ -3233,7 +3209,7 @@
       <c r="J3" s="5"/>
       <c r="K3" s="4"/>
     </row>
-    <row r="4" spans="1:11" ht="20.100000000000001" customHeight="1">
+    <row r="4" spans="1:11" ht="20" customHeight="1">
       <c r="A4" s="4">
         <v>386</v>
       </c>
@@ -3262,7 +3238,7 @@
       <c r="J4" s="5"/>
       <c r="K4" s="4"/>
     </row>
-    <row r="5" spans="1:11" ht="20.100000000000001" customHeight="1">
+    <row r="5" spans="1:11" ht="20" customHeight="1">
       <c r="A5" s="4">
         <v>648</v>
       </c>
@@ -3289,7 +3265,7 @@
       <c r="J5" s="5"/>
       <c r="K5" s="4"/>
     </row>
-    <row r="6" spans="1:11" ht="20.100000000000001" customHeight="1">
+    <row r="6" spans="1:11" ht="20" customHeight="1">
       <c r="A6" s="4">
         <v>677</v>
       </c>
@@ -3318,7 +3294,7 @@
       <c r="J6" s="5"/>
       <c r="K6" s="4"/>
     </row>
-    <row r="7" spans="1:11" ht="20.100000000000001" customHeight="1">
+    <row r="7" spans="1:11" ht="20" customHeight="1">
       <c r="A7" s="4">
         <v>720</v>
       </c>
@@ -3376,7 +3352,7 @@
       <c r="J8" s="5"/>
       <c r="K8" s="4"/>
     </row>
-    <row r="9" spans="1:11" ht="20.100000000000001" customHeight="1">
+    <row r="9" spans="1:11" ht="20" customHeight="1">
       <c r="A9" s="4">
         <v>1268</v>
       </c>
@@ -3437,13 +3413,13 @@
   </sheetData>
   <phoneticPr fontId="1" type="noConversion"/>
   <conditionalFormatting sqref="D2:D10">
-    <cfRule type="expression" dxfId="11" priority="1">
+    <cfRule type="expression" dxfId="8" priority="1">
       <formula>D2="Easy"</formula>
     </cfRule>
-    <cfRule type="expression" dxfId="10" priority="2">
+    <cfRule type="expression" dxfId="7" priority="2">
       <formula>D2="Medium"</formula>
     </cfRule>
-    <cfRule type="expression" dxfId="9" priority="3">
+    <cfRule type="expression" dxfId="6" priority="3">
       <formula>D2="Hard"</formula>
     </cfRule>
   </conditionalFormatting>
@@ -3472,11 +3448,11 @@
   <sheetViews>
     <sheetView zoomScaleNormal="100" workbookViewId="0"/>
   </sheetViews>
-  <sheetFormatPr defaultColWidth="9" defaultRowHeight="16.5"/>
+  <sheetFormatPr baseColWidth="10" defaultColWidth="9" defaultRowHeight="16"/>
   <cols>
     <col min="1" max="1" width="11" customWidth="1"/>
     <col min="2" max="2" width="36" customWidth="1"/>
-    <col min="3" max="3" width="35.85546875" style="12" customWidth="1"/>
+    <col min="3" max="3" width="35.796875" style="12" customWidth="1"/>
     <col min="4" max="4" width="16" customWidth="1"/>
     <col min="5" max="5" width="36" customWidth="1"/>
     <col min="6" max="8" width="21" customWidth="1"/>
@@ -3484,7 +3460,7 @@
     <col min="11" max="11" width="16" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:11" ht="20.100000000000001" customHeight="1">
+    <row r="1" spans="1:11" ht="20" customHeight="1">
       <c r="A1" s="2" t="s">
         <v>4</v>
       </c>
@@ -3519,7 +3495,7 @@
         <v>3</v>
       </c>
     </row>
-    <row r="2" spans="1:11" ht="20.100000000000001" customHeight="1">
+    <row r="2" spans="1:11" ht="20" customHeight="1">
       <c r="A2" s="4">
         <v>113</v>
       </c>
@@ -3548,7 +3524,7 @@
       <c r="J2" s="5"/>
       <c r="K2" s="4"/>
     </row>
-    <row r="3" spans="1:11" ht="20.100000000000001" customHeight="1">
+    <row r="3" spans="1:11" ht="20" customHeight="1">
       <c r="A3" s="4">
         <v>114</v>
       </c>
@@ -3577,7 +3553,7 @@
       <c r="J3" s="5"/>
       <c r="K3" s="4"/>
     </row>
-    <row r="4" spans="1:11" ht="20.100000000000001" customHeight="1">
+    <row r="4" spans="1:11" ht="20" customHeight="1">
       <c r="A4" s="4">
         <v>129</v>
       </c>
@@ -3606,7 +3582,7 @@
       <c r="J4" s="5"/>
       <c r="K4" s="4"/>
     </row>
-    <row r="5" spans="1:11" ht="20.100000000000001" customHeight="1">
+    <row r="5" spans="1:11" ht="20" customHeight="1">
       <c r="A5" s="4">
         <v>341</v>
       </c>
@@ -3635,7 +3611,7 @@
       <c r="J5" s="5"/>
       <c r="K5" s="4"/>
     </row>
-    <row r="6" spans="1:11" ht="20.100000000000001" customHeight="1">
+    <row r="6" spans="1:11" ht="20" customHeight="1">
       <c r="A6" s="4">
         <v>399</v>
       </c>
@@ -3666,7 +3642,7 @@
       <c r="J6" s="5"/>
       <c r="K6" s="4"/>
     </row>
-    <row r="7" spans="1:11" ht="20.100000000000001" customHeight="1">
+    <row r="7" spans="1:11" ht="20" customHeight="1">
       <c r="A7" s="4">
         <v>437</v>
       </c>
@@ -3695,7 +3671,7 @@
       <c r="J7" s="5"/>
       <c r="K7" s="4"/>
     </row>
-    <row r="8" spans="1:11" ht="20.100000000000001" customHeight="1">
+    <row r="8" spans="1:11" ht="20" customHeight="1">
       <c r="A8" s="4">
         <v>508</v>
       </c>
@@ -3724,7 +3700,7 @@
       <c r="J8" s="5"/>
       <c r="K8" s="4"/>
     </row>
-    <row r="9" spans="1:11" ht="20.100000000000001" customHeight="1">
+    <row r="9" spans="1:11" ht="20" customHeight="1">
       <c r="A9" s="4">
         <v>623</v>
       </c>
@@ -3818,13 +3794,13 @@
   </sheetData>
   <phoneticPr fontId="1" type="noConversion"/>
   <conditionalFormatting sqref="D2:D11">
-    <cfRule type="expression" dxfId="8" priority="1">
+    <cfRule type="expression" dxfId="5" priority="1">
       <formula>D2="Easy"</formula>
     </cfRule>
-    <cfRule type="expression" dxfId="7" priority="2">
+    <cfRule type="expression" dxfId="4" priority="2">
       <formula>D2="Medium"</formula>
     </cfRule>
-    <cfRule type="expression" dxfId="6" priority="3">
+    <cfRule type="expression" dxfId="3" priority="3">
       <formula>D2="Hard"</formula>
     </cfRule>
   </conditionalFormatting>
@@ -3854,11 +3830,11 @@
   <sheetViews>
     <sheetView zoomScaleNormal="100" workbookViewId="0"/>
   </sheetViews>
-  <sheetFormatPr defaultColWidth="9" defaultRowHeight="16.5"/>
+  <sheetFormatPr baseColWidth="10" defaultColWidth="9" defaultRowHeight="16"/>
   <cols>
     <col min="1" max="1" width="11" customWidth="1"/>
-    <col min="2" max="2" width="43.140625" customWidth="1"/>
-    <col min="3" max="3" width="35.85546875" style="12" customWidth="1"/>
+    <col min="2" max="2" width="43.19921875" customWidth="1"/>
+    <col min="3" max="3" width="35.796875" style="12" customWidth="1"/>
     <col min="4" max="4" width="16" customWidth="1"/>
     <col min="5" max="5" width="36" customWidth="1"/>
     <col min="6" max="8" width="21" customWidth="1"/>
@@ -3866,7 +3842,7 @@
     <col min="11" max="11" width="16" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:11" ht="20.100000000000001" customHeight="1">
+    <row r="1" spans="1:11" ht="20" customHeight="1">
       <c r="A1" s="2" t="s">
         <v>4</v>
       </c>
@@ -4025,7 +4001,7 @@
       <c r="J5" s="5"/>
       <c r="K5" s="4"/>
     </row>
-    <row r="6" spans="1:11" ht="20.100000000000001" customHeight="1">
+    <row r="6" spans="1:11" ht="20" customHeight="1">
       <c r="A6" s="4">
         <v>513</v>
       </c>
@@ -4054,7 +4030,7 @@
       <c r="J6" s="5"/>
       <c r="K6" s="4"/>
     </row>
-    <row r="7" spans="1:11" ht="20.100000000000001" customHeight="1">
+    <row r="7" spans="1:11" ht="20" customHeight="1">
       <c r="A7" s="4">
         <v>515</v>
       </c>
@@ -4114,7 +4090,7 @@
       <c r="J8" s="5"/>
       <c r="K8" s="4"/>
     </row>
-    <row r="9" spans="1:11" ht="20.100000000000001" customHeight="1">
+    <row r="9" spans="1:11" ht="20" customHeight="1">
       <c r="A9" s="4">
         <v>958</v>
       </c>
@@ -4143,7 +4119,7 @@
       <c r="J9" s="5"/>
       <c r="K9" s="4"/>
     </row>
-    <row r="10" spans="1:11" ht="20.100000000000001" customHeight="1">
+    <row r="10" spans="1:11" ht="20" customHeight="1">
       <c r="A10" s="4">
         <v>1161</v>
       </c>
@@ -4174,26 +4150,15 @@
     </row>
   </sheetData>
   <phoneticPr fontId="1" type="noConversion"/>
-  <conditionalFormatting sqref="D2:D5 D8:D10">
-    <cfRule type="expression" dxfId="5" priority="4">
+  <conditionalFormatting sqref="D2:D10">
+    <cfRule type="expression" dxfId="2" priority="1">
       <formula>D2="Easy"</formula>
     </cfRule>
-    <cfRule type="expression" dxfId="4" priority="5">
+    <cfRule type="expression" dxfId="1" priority="2">
       <formula>D2="Medium"</formula>
     </cfRule>
-    <cfRule type="expression" dxfId="3" priority="6">
+    <cfRule type="expression" dxfId="0" priority="3">
       <formula>D2="Hard"</formula>
-    </cfRule>
-  </conditionalFormatting>
-  <conditionalFormatting sqref="D6:D7">
-    <cfRule type="expression" dxfId="2" priority="1">
-      <formula>D6="Easy"</formula>
-    </cfRule>
-    <cfRule type="expression" dxfId="1" priority="2">
-      <formula>D6="Medium"</formula>
-    </cfRule>
-    <cfRule type="expression" dxfId="0" priority="3">
-      <formula>D6="Hard"</formula>
     </cfRule>
   </conditionalFormatting>
   <hyperlinks>

</xml_diff>

<commit_message>
Completed two more hard practices.
</commit_message>
<xml_diff>
--- a/LeetCode Techniques.xlsx
+++ b/LeetCode Techniques.xlsx
@@ -1,16 +1,16 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
-  <fileVersion appName="xl" lastEdited="7" lowestEdited="4" rupBuild="10714"/>
+  <fileVersion appName="xl" lastEdited="7" lowestEdited="4" rupBuild="27328"/>
   <workbookPr defaultThemeVersion="124226"/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="/Users/blackjack625/Desktop/LeetCode/"/>
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\jack.yao\Desktop\LeetCode\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{81BC5399-56B0-9B4D-A15A-F945C85CDAF8}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{D495B4CE-CF63-49A9-976A-7BF267B2D07C}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="0" yWindow="500" windowWidth="28800" windowHeight="16480" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
+    <workbookView xWindow="-120" yWindow="-120" windowWidth="20640" windowHeight="11040" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
   <sheets>
     <sheet name="DP" sheetId="8" r:id="rId1"/>
@@ -42,7 +42,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="547" uniqueCount="229">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="553" uniqueCount="232">
   <si>
     <t>Name</t>
   </si>
@@ -934,25 +934,34 @@
 index to pick from list.</t>
     <phoneticPr fontId="1" type="noConversion"/>
   </si>
+  <si>
+    <t>Maximum Frequency Stack</t>
+  </si>
+  <si>
+    <t>https://leetcode.com/problems/maximum-frequency-stack/description/</t>
+  </si>
+  <si>
+    <t>Binary Search, Hash</t>
+  </si>
 </sst>
 </file>
 
 <file path=xl/styles.xml><?xml version="1.0" encoding="utf-8"?>
 <styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:x16r2="http://schemas.microsoft.com/office/spreadsheetml/2015/02/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" mc:Ignorable="x14ac x16r2 xr">
   <numFmts count="1">
-    <numFmt numFmtId="176" formatCode="yyyy&quot;年&quot;m&quot;月&quot;d&quot;日&quot;;@"/>
+    <numFmt numFmtId="164" formatCode="yyyy&quot;年&quot;m&quot;月&quot;d&quot;日&quot;;@"/>
   </numFmts>
   <fonts count="16">
     <font>
       <sz val="11"/>
       <color theme="1"/>
-      <name val="新細明體"/>
+      <name val="Calibri"/>
       <family val="2"/>
       <scheme val="minor"/>
     </font>
     <font>
       <sz val="9"/>
-      <name val="新細明體"/>
+      <name val="Calibri"/>
       <family val="2"/>
       <charset val="136"/>
       <scheme val="minor"/>
@@ -976,7 +985,7 @@
       <u/>
       <sz val="11"/>
       <color theme="10"/>
-      <name val="新細明體"/>
+      <name val="Calibri"/>
       <family val="2"/>
       <scheme val="minor"/>
     </font>
@@ -1040,20 +1049,17 @@
       <sz val="10"/>
       <color theme="1"/>
       <name val="Microsoft YaHei"/>
-      <charset val="134"/>
     </font>
     <font>
       <u/>
       <sz val="10"/>
       <color theme="10"/>
       <name val="Microsoft YaHei"/>
-      <charset val="134"/>
     </font>
     <font>
       <sz val="10"/>
       <color theme="1"/>
       <name val="Microsoft YaHei"/>
-      <charset val="134"/>
     </font>
   </fonts>
   <fills count="2">
@@ -1094,17 +1100,17 @@
   </cellStyleXfs>
   <cellXfs count="21">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
-    <xf numFmtId="176" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1"/>
+    <xf numFmtId="164" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1"/>
     <xf numFmtId="0" fontId="2" fillId="0" borderId="1" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
     </xf>
-    <xf numFmtId="176" fontId="2" fillId="0" borderId="1" xfId="0" applyNumberFormat="1" applyFont="1" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="164" fontId="2" fillId="0" borderId="1" xfId="0" applyNumberFormat="1" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
     </xf>
     <xf numFmtId="0" fontId="3" fillId="0" borderId="1" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
     </xf>
-    <xf numFmtId="176" fontId="3" fillId="0" borderId="1" xfId="0" applyNumberFormat="1" applyFont="1" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="164" fontId="3" fillId="0" borderId="1" xfId="0" applyNumberFormat="1" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
     </xf>
     <xf numFmtId="0" fontId="3" fillId="0" borderId="1" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
@@ -1146,8 +1152,8 @@
     <xf numFmtId="0" fontId="15" fillId="0" borderId="0" xfId="0" applyFont="1"/>
   </cellXfs>
   <cellStyles count="2">
-    <cellStyle name="一般" xfId="0" builtinId="0"/>
-    <cellStyle name="超連結" xfId="1" builtinId="8"/>
+    <cellStyle name="Hyperlink" xfId="1" builtinId="8"/>
+    <cellStyle name="Normal" xfId="0" builtinId="0"/>
   </cellStyles>
   <dxfs count="36">
     <dxf>
@@ -1814,11 +1820,11 @@
   <sheetViews>
     <sheetView tabSelected="1" zoomScaleNormal="100" workbookViewId="0"/>
   </sheetViews>
-  <sheetFormatPr baseColWidth="10" defaultColWidth="9" defaultRowHeight="16"/>
+  <sheetFormatPr defaultColWidth="9" defaultRowHeight="16.5"/>
   <cols>
     <col min="1" max="1" width="11" customWidth="1"/>
     <col min="2" max="2" width="46" customWidth="1"/>
-    <col min="3" max="3" width="40.796875" style="14" customWidth="1"/>
+    <col min="3" max="3" width="40.85546875" style="14" customWidth="1"/>
     <col min="4" max="4" width="16" customWidth="1"/>
     <col min="5" max="5" width="36" customWidth="1"/>
     <col min="6" max="8" width="21" customWidth="1"/>
@@ -1826,7 +1832,7 @@
     <col min="11" max="11" width="16" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:11" ht="20" customHeight="1">
+    <row r="1" spans="1:11" ht="20.100000000000001" customHeight="1">
       <c r="A1" s="2" t="s">
         <v>4</v>
       </c>
@@ -1861,7 +1867,7 @@
         <v>3</v>
       </c>
     </row>
-    <row r="2" spans="1:11" ht="20" customHeight="1">
+    <row r="2" spans="1:11" ht="20.100000000000001" customHeight="1">
       <c r="A2" s="4">
         <v>53</v>
       </c>
@@ -1888,7 +1894,7 @@
       <c r="J2" s="5"/>
       <c r="K2" s="4"/>
     </row>
-    <row r="3" spans="1:11" ht="20" customHeight="1">
+    <row r="3" spans="1:11" ht="20.100000000000001" customHeight="1">
       <c r="A3" s="4">
         <v>62</v>
       </c>
@@ -1944,7 +1950,7 @@
       <c r="J4" s="5"/>
       <c r="K4" s="4"/>
     </row>
-    <row r="5" spans="1:11" ht="20" customHeight="1">
+    <row r="5" spans="1:11" ht="20.100000000000001" customHeight="1">
       <c r="A5" s="4">
         <v>64</v>
       </c>
@@ -1971,7 +1977,7 @@
       <c r="J5" s="5"/>
       <c r="K5" s="4"/>
     </row>
-    <row r="6" spans="1:11" ht="20" customHeight="1">
+    <row r="6" spans="1:11" ht="20.100000000000001" customHeight="1">
       <c r="A6" s="4">
         <v>120</v>
       </c>
@@ -2058,7 +2064,7 @@
       <c r="J8" s="5"/>
       <c r="K8" s="4"/>
     </row>
-    <row r="9" spans="1:11" ht="20" customHeight="1">
+    <row r="9" spans="1:11" ht="20.100000000000001" customHeight="1">
       <c r="A9" s="4">
         <v>198</v>
       </c>
@@ -2118,7 +2124,7 @@
       <c r="J10" s="5"/>
       <c r="K10" s="4"/>
     </row>
-    <row r="11" spans="1:11" ht="20" customHeight="1">
+    <row r="11" spans="1:11" ht="20.100000000000001" customHeight="1">
       <c r="A11" s="4">
         <v>279</v>
       </c>
@@ -2207,7 +2213,7 @@
       <c r="J13" s="5"/>
       <c r="K13" s="4"/>
     </row>
-    <row r="14" spans="1:11" ht="20" customHeight="1">
+    <row r="14" spans="1:11" ht="20.100000000000001" customHeight="1">
       <c r="A14" s="4">
         <v>343</v>
       </c>
@@ -2294,7 +2300,7 @@
       <c r="J16" s="5"/>
       <c r="K16" s="4"/>
     </row>
-    <row r="17" spans="1:11" ht="20" customHeight="1">
+    <row r="17" spans="1:11" ht="20.100000000000001" customHeight="1">
       <c r="A17" s="4">
         <v>907</v>
       </c>
@@ -2325,7 +2331,7 @@
       <c r="J17" s="5"/>
       <c r="K17" s="4"/>
     </row>
-    <row r="18" spans="1:11" ht="20" customHeight="1">
+    <row r="18" spans="1:11" ht="20.100000000000001" customHeight="1">
       <c r="A18" s="4">
         <v>931</v>
       </c>
@@ -2352,7 +2358,7 @@
       <c r="J18" s="5"/>
       <c r="K18" s="4"/>
     </row>
-    <row r="19" spans="1:11" ht="20" customHeight="1">
+    <row r="19" spans="1:11" ht="20.100000000000001" customHeight="1">
       <c r="A19" s="4">
         <v>1220</v>
       </c>
@@ -2410,7 +2416,7 @@
       <c r="J20" s="5"/>
       <c r="K20" s="4"/>
     </row>
-    <row r="21" spans="1:11" ht="20" customHeight="1">
+    <row r="21" spans="1:11" ht="20.100000000000001" customHeight="1">
       <c r="A21" s="4">
         <v>1301</v>
       </c>
@@ -2437,7 +2443,7 @@
       <c r="J21" s="5"/>
       <c r="K21" s="4"/>
     </row>
-    <row r="22" spans="1:11" ht="20" customHeight="1">
+    <row r="22" spans="1:11" ht="20.100000000000001" customHeight="1">
       <c r="A22" s="4">
         <v>1359</v>
       </c>
@@ -2495,7 +2501,7 @@
       <c r="J23" s="5"/>
       <c r="K23" s="4"/>
     </row>
-    <row r="24" spans="1:11" ht="20" customHeight="1">
+    <row r="24" spans="1:11" ht="20.100000000000001" customHeight="1">
       <c r="A24" s="4">
         <v>1449</v>
       </c>
@@ -2575,11 +2581,11 @@
   <sheetViews>
     <sheetView zoomScaleNormal="100" workbookViewId="0"/>
   </sheetViews>
-  <sheetFormatPr baseColWidth="10" defaultColWidth="9" defaultRowHeight="17"/>
+  <sheetFormatPr defaultColWidth="9" defaultRowHeight="16.5"/>
   <cols>
     <col min="1" max="1" width="11" customWidth="1"/>
     <col min="2" max="2" width="16" customWidth="1"/>
-    <col min="3" max="3" width="35.796875" style="9" customWidth="1"/>
+    <col min="3" max="3" width="35.85546875" style="9" customWidth="1"/>
     <col min="4" max="4" width="16" customWidth="1"/>
     <col min="5" max="5" width="36" customWidth="1"/>
     <col min="6" max="8" width="21" customWidth="1"/>
@@ -2587,7 +2593,7 @@
     <col min="11" max="11" width="16" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:11" ht="20" customHeight="1">
+    <row r="1" spans="1:11" ht="20.100000000000001" customHeight="1">
       <c r="A1" s="2" t="s">
         <v>4</v>
       </c>
@@ -2622,7 +2628,7 @@
         <v>3</v>
       </c>
     </row>
-    <row r="2" spans="1:11" ht="20" customHeight="1">
+    <row r="2" spans="1:11" ht="20.100000000000001" customHeight="1">
       <c r="A2" s="4">
         <v>394</v>
       </c>
@@ -2679,10 +2685,10 @@
   <sheetViews>
     <sheetView zoomScaleNormal="100" workbookViewId="0"/>
   </sheetViews>
-  <sheetFormatPr baseColWidth="10" defaultColWidth="9" defaultRowHeight="17"/>
+  <sheetFormatPr defaultColWidth="9" defaultRowHeight="16.5"/>
   <cols>
     <col min="1" max="1" width="11" customWidth="1"/>
-    <col min="2" max="2" width="38.19921875" customWidth="1"/>
+    <col min="2" max="2" width="38.140625" customWidth="1"/>
     <col min="3" max="3" width="71" style="9" customWidth="1"/>
     <col min="4" max="4" width="16" customWidth="1"/>
     <col min="5" max="5" width="36" customWidth="1"/>
@@ -2691,7 +2697,7 @@
     <col min="11" max="11" width="16" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:11" ht="20" customHeight="1">
+    <row r="1" spans="1:11" ht="20.100000000000001" customHeight="1">
       <c r="A1" s="2" t="s">
         <v>4</v>
       </c>
@@ -2726,7 +2732,7 @@
         <v>3</v>
       </c>
     </row>
-    <row r="2" spans="1:11" ht="20" customHeight="1">
+    <row r="2" spans="1:11" ht="20.100000000000001" customHeight="1">
       <c r="A2" s="4">
         <v>74</v>
       </c>
@@ -2753,7 +2759,7 @@
       <c r="J2" s="3"/>
       <c r="K2" s="2"/>
     </row>
-    <row r="3" spans="1:11" ht="20" customHeight="1">
+    <row r="3" spans="1:11" ht="20.100000000000001" customHeight="1">
       <c r="A3" s="4">
         <v>220</v>
       </c>
@@ -2809,7 +2815,7 @@
       <c r="J4" s="5"/>
       <c r="K4" s="4"/>
     </row>
-    <row r="5" spans="1:11" ht="20" customHeight="1">
+    <row r="5" spans="1:11" ht="20.100000000000001" customHeight="1">
       <c r="A5" s="4">
         <v>315</v>
       </c>
@@ -2836,7 +2842,7 @@
       <c r="J5" s="5"/>
       <c r="K5" s="4"/>
     </row>
-    <row r="6" spans="1:11" ht="20" customHeight="1">
+    <row r="6" spans="1:11" ht="20.100000000000001" customHeight="1">
       <c r="A6" s="4">
         <v>352</v>
       </c>
@@ -2865,7 +2871,7 @@
       <c r="J6" s="5"/>
       <c r="K6" s="4"/>
     </row>
-    <row r="7" spans="1:11" ht="20" customHeight="1">
+    <row r="7" spans="1:11" ht="20.100000000000001" customHeight="1">
       <c r="A7" s="4">
         <v>480</v>
       </c>
@@ -2892,7 +2898,7 @@
       <c r="J7" s="5"/>
       <c r="K7" s="4"/>
     </row>
-    <row r="8" spans="1:11" ht="20" customHeight="1">
+    <row r="8" spans="1:11" ht="20.100000000000001" customHeight="1">
       <c r="A8" s="4">
         <v>493</v>
       </c>
@@ -2919,7 +2925,7 @@
       <c r="J8" s="5"/>
       <c r="K8" s="4"/>
     </row>
-    <row r="9" spans="1:11" ht="20" customHeight="1">
+    <row r="9" spans="1:11" ht="20.100000000000001" customHeight="1">
       <c r="A9" s="4">
         <v>611</v>
       </c>
@@ -2948,7 +2954,7 @@
       <c r="J9" s="5"/>
       <c r="K9" s="4"/>
     </row>
-    <row r="10" spans="1:11" ht="20" customHeight="1">
+    <row r="10" spans="1:11" ht="20.100000000000001" customHeight="1">
       <c r="A10" s="4">
         <v>729</v>
       </c>
@@ -2975,7 +2981,7 @@
       <c r="J10" s="5"/>
       <c r="K10" s="4"/>
     </row>
-    <row r="11" spans="1:11" ht="20" customHeight="1">
+    <row r="11" spans="1:11" ht="20.100000000000001" customHeight="1">
       <c r="A11" s="4">
         <v>1095</v>
       </c>
@@ -3033,7 +3039,7 @@
       <c r="J12" s="5"/>
       <c r="K12" s="4"/>
     </row>
-    <row r="13" spans="1:11" ht="20" customHeight="1">
+    <row r="13" spans="1:11" ht="20.100000000000001" customHeight="1">
       <c r="A13" s="4">
         <v>1825</v>
       </c>
@@ -3062,7 +3068,7 @@
       <c r="J13" s="5"/>
       <c r="K13" s="4"/>
     </row>
-    <row r="14" spans="1:11" ht="20" customHeight="1">
+    <row r="14" spans="1:11" ht="20.100000000000001" customHeight="1">
       <c r="A14" s="4">
         <v>2034</v>
       </c>
@@ -3091,7 +3097,7 @@
       <c r="J14" s="5"/>
       <c r="K14" s="4"/>
     </row>
-    <row r="15" spans="1:11" ht="20" customHeight="1">
+    <row r="15" spans="1:11" ht="20.100000000000001" customHeight="1">
       <c r="A15" s="4">
         <v>2102</v>
       </c>
@@ -3176,11 +3182,11 @@
   <sheetViews>
     <sheetView zoomScaleNormal="100" workbookViewId="0"/>
   </sheetViews>
-  <sheetFormatPr baseColWidth="10" defaultColWidth="9" defaultRowHeight="16"/>
+  <sheetFormatPr defaultColWidth="9" defaultRowHeight="16.5"/>
   <cols>
     <col min="1" max="1" width="11" customWidth="1"/>
     <col min="2" max="2" width="36" customWidth="1"/>
-    <col min="3" max="3" width="35.796875" style="14" customWidth="1"/>
+    <col min="3" max="3" width="35.85546875" style="14" customWidth="1"/>
     <col min="4" max="4" width="16" customWidth="1"/>
     <col min="5" max="5" width="36" customWidth="1"/>
     <col min="6" max="8" width="21" customWidth="1"/>
@@ -3188,7 +3194,7 @@
     <col min="11" max="11" width="16" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:11" ht="20" customHeight="1">
+    <row r="1" spans="1:11" ht="20.100000000000001" customHeight="1">
       <c r="A1" s="2" t="s">
         <v>4</v>
       </c>
@@ -3223,7 +3229,7 @@
         <v>3</v>
       </c>
     </row>
-    <row r="2" spans="1:11" ht="20" customHeight="1">
+    <row r="2" spans="1:11" ht="20.100000000000001" customHeight="1">
       <c r="A2" s="4">
         <v>113</v>
       </c>
@@ -3250,7 +3256,7 @@
       <c r="J2" s="5"/>
       <c r="K2" s="4"/>
     </row>
-    <row r="3" spans="1:11" ht="20" customHeight="1">
+    <row r="3" spans="1:11" ht="20.100000000000001" customHeight="1">
       <c r="A3" s="4">
         <v>114</v>
       </c>
@@ -3277,7 +3283,7 @@
       <c r="J3" s="5"/>
       <c r="K3" s="4"/>
     </row>
-    <row r="4" spans="1:11" ht="20" customHeight="1">
+    <row r="4" spans="1:11" ht="20.100000000000001" customHeight="1">
       <c r="A4" s="4">
         <v>129</v>
       </c>
@@ -3333,7 +3339,7 @@
       <c r="J5" s="5"/>
       <c r="K5" s="4"/>
     </row>
-    <row r="6" spans="1:11" ht="20" customHeight="1">
+    <row r="6" spans="1:11" ht="20.100000000000001" customHeight="1">
       <c r="A6" s="4">
         <v>341</v>
       </c>
@@ -3360,7 +3366,7 @@
       <c r="J6" s="5"/>
       <c r="K6" s="4"/>
     </row>
-    <row r="7" spans="1:11" ht="20" customHeight="1">
+    <row r="7" spans="1:11" ht="20.100000000000001" customHeight="1">
       <c r="A7" s="4">
         <v>399</v>
       </c>
@@ -3391,7 +3397,7 @@
       <c r="J7" s="5"/>
       <c r="K7" s="4"/>
     </row>
-    <row r="8" spans="1:11" ht="20" customHeight="1">
+    <row r="8" spans="1:11" ht="20.100000000000001" customHeight="1">
       <c r="A8" s="4">
         <v>437</v>
       </c>
@@ -3418,7 +3424,7 @@
       <c r="J8" s="5"/>
       <c r="K8" s="4"/>
     </row>
-    <row r="9" spans="1:11" ht="20" customHeight="1">
+    <row r="9" spans="1:11" ht="20.100000000000001" customHeight="1">
       <c r="A9" s="4">
         <v>508</v>
       </c>
@@ -3445,7 +3451,7 @@
       <c r="J9" s="5"/>
       <c r="K9" s="4"/>
     </row>
-    <row r="10" spans="1:11" ht="20" customHeight="1">
+    <row r="10" spans="1:11" ht="20.100000000000001" customHeight="1">
       <c r="A10" s="4">
         <v>623</v>
       </c>
@@ -3600,11 +3606,11 @@
   <sheetViews>
     <sheetView zoomScaleNormal="100" workbookViewId="0"/>
   </sheetViews>
-  <sheetFormatPr baseColWidth="10" defaultColWidth="9" defaultRowHeight="16"/>
+  <sheetFormatPr defaultColWidth="9" defaultRowHeight="16.5"/>
   <cols>
     <col min="1" max="1" width="11" customWidth="1"/>
-    <col min="2" max="2" width="43.19921875" customWidth="1"/>
-    <col min="3" max="3" width="35.796875" style="11" customWidth="1"/>
+    <col min="2" max="2" width="43.140625" customWidth="1"/>
+    <col min="3" max="3" width="35.85546875" style="11" customWidth="1"/>
     <col min="4" max="4" width="16" customWidth="1"/>
     <col min="5" max="5" width="36" customWidth="1"/>
     <col min="6" max="8" width="21" customWidth="1"/>
@@ -3612,7 +3618,7 @@
     <col min="11" max="11" width="16" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:11" ht="20" customHeight="1">
+    <row r="1" spans="1:11" ht="20.100000000000001" customHeight="1">
       <c r="A1" s="2" t="s">
         <v>4</v>
       </c>
@@ -3763,7 +3769,7 @@
       <c r="J5" s="5"/>
       <c r="K5" s="4"/>
     </row>
-    <row r="6" spans="1:11" ht="20" customHeight="1">
+    <row r="6" spans="1:11" ht="20.100000000000001" customHeight="1">
       <c r="A6" s="4">
         <v>513</v>
       </c>
@@ -3790,7 +3796,7 @@
       <c r="J6" s="5"/>
       <c r="K6" s="4"/>
     </row>
-    <row r="7" spans="1:11" ht="20" customHeight="1">
+    <row r="7" spans="1:11" ht="20.100000000000001" customHeight="1">
       <c r="A7" s="4">
         <v>515</v>
       </c>
@@ -3846,7 +3852,7 @@
       <c r="J8" s="5"/>
       <c r="K8" s="4"/>
     </row>
-    <row r="9" spans="1:11" ht="20" customHeight="1">
+    <row r="9" spans="1:11" ht="20.100000000000001" customHeight="1">
       <c r="A9" s="4">
         <v>958</v>
       </c>
@@ -3873,7 +3879,7 @@
       <c r="J9" s="5"/>
       <c r="K9" s="4"/>
     </row>
-    <row r="10" spans="1:11" ht="20" customHeight="1">
+    <row r="10" spans="1:11" ht="20.100000000000001" customHeight="1">
       <c r="A10" s="4">
         <v>987</v>
       </c>
@@ -3900,7 +3906,7 @@
       <c r="J10" s="5"/>
       <c r="K10" s="4"/>
     </row>
-    <row r="11" spans="1:11" ht="20" customHeight="1">
+    <row r="11" spans="1:11" ht="20.100000000000001" customHeight="1">
       <c r="A11" s="4">
         <v>1161</v>
       </c>
@@ -3966,11 +3972,11 @@
   <sheetViews>
     <sheetView zoomScaleNormal="100" workbookViewId="0"/>
   </sheetViews>
-  <sheetFormatPr baseColWidth="10" defaultColWidth="9" defaultRowHeight="16"/>
+  <sheetFormatPr defaultColWidth="9" defaultRowHeight="16.5"/>
   <cols>
     <col min="1" max="1" width="11" customWidth="1"/>
-    <col min="2" max="2" width="43.19921875" customWidth="1"/>
-    <col min="3" max="3" width="35.796875" style="11" customWidth="1"/>
+    <col min="2" max="2" width="43.140625" customWidth="1"/>
+    <col min="3" max="3" width="35.85546875" style="11" customWidth="1"/>
     <col min="4" max="4" width="16" customWidth="1"/>
     <col min="5" max="5" width="36" customWidth="1"/>
     <col min="6" max="8" width="21" customWidth="1"/>
@@ -3978,7 +3984,7 @@
     <col min="11" max="11" width="16" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:11" ht="20" customHeight="1">
+    <row r="1" spans="1:11" ht="20.100000000000001" customHeight="1">
       <c r="A1" s="2" t="s">
         <v>4</v>
       </c>
@@ -4068,15 +4074,15 @@
 
 <file path=xl/worksheets/sheet6.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{9BC7A267-6069-4E38-AC2F-0C28241496B0}">
-  <dimension ref="A1:K3"/>
+  <dimension ref="A1:K4"/>
   <sheetViews>
     <sheetView zoomScaleNormal="100" workbookViewId="0"/>
   </sheetViews>
-  <sheetFormatPr baseColWidth="10" defaultColWidth="9" defaultRowHeight="16"/>
+  <sheetFormatPr defaultColWidth="9" defaultRowHeight="16.5"/>
   <cols>
     <col min="1" max="1" width="11" customWidth="1"/>
-    <col min="2" max="2" width="25.796875" customWidth="1"/>
-    <col min="3" max="3" width="35.796875" style="20" customWidth="1"/>
+    <col min="2" max="2" width="25.85546875" customWidth="1"/>
+    <col min="3" max="3" width="35.85546875" style="20" customWidth="1"/>
     <col min="4" max="4" width="16" customWidth="1"/>
     <col min="5" max="5" width="41" customWidth="1"/>
     <col min="6" max="8" width="21" customWidth="1"/>
@@ -4084,7 +4090,7 @@
     <col min="11" max="11" width="16" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:11" ht="20" customHeight="1">
+    <row r="1" spans="1:11" ht="20.100000000000001" customHeight="1">
       <c r="A1" s="2" t="s">
         <v>4</v>
       </c>
@@ -4119,69 +4125,98 @@
         <v>3</v>
       </c>
     </row>
-    <row r="2" spans="1:11" ht="30" customHeight="1">
+    <row r="2" spans="1:11" ht="20.100000000000001" customHeight="1">
       <c r="A2" s="6">
-        <v>1172</v>
+        <v>895</v>
       </c>
       <c r="B2" s="6" t="s">
-        <v>223</v>
+        <v>229</v>
       </c>
       <c r="C2" s="19" t="s">
-        <v>224</v>
+        <v>230</v>
       </c>
       <c r="D2" s="4" t="s">
         <v>16</v>
       </c>
-      <c r="E2" s="17" t="s">
-        <v>225</v>
-      </c>
-      <c r="F2" s="4"/>
+      <c r="E2" s="17"/>
+      <c r="F2" s="4" t="s">
+        <v>231</v>
+      </c>
       <c r="G2" s="4" t="s">
-        <v>44</v>
+        <v>45</v>
       </c>
       <c r="H2" s="4" t="s">
         <v>44</v>
       </c>
       <c r="I2" s="5">
-        <v>45511</v>
+        <v>45512</v>
       </c>
       <c r="J2" s="5"/>
       <c r="K2" s="4"/>
     </row>
     <row r="3" spans="1:11" ht="30" customHeight="1">
       <c r="A3" s="6">
-        <v>2454</v>
+        <v>1172</v>
       </c>
       <c r="B3" s="6" t="s">
-        <v>203</v>
+        <v>223</v>
       </c>
       <c r="C3" s="19" t="s">
-        <v>204</v>
+        <v>224</v>
       </c>
       <c r="D3" s="4" t="s">
         <v>16</v>
       </c>
       <c r="E3" s="17" t="s">
-        <v>222</v>
-      </c>
-      <c r="F3" s="4" t="s">
-        <v>158</v>
-      </c>
+        <v>225</v>
+      </c>
+      <c r="F3" s="4"/>
       <c r="G3" s="4" t="s">
-        <v>205</v>
+        <v>44</v>
       </c>
       <c r="H3" s="4" t="s">
         <v>44</v>
       </c>
       <c r="I3" s="5">
-        <v>45505</v>
+        <v>45511</v>
       </c>
       <c r="J3" s="5"/>
       <c r="K3" s="4"/>
     </row>
+    <row r="4" spans="1:11" ht="30" customHeight="1">
+      <c r="A4" s="6">
+        <v>2454</v>
+      </c>
+      <c r="B4" s="6" t="s">
+        <v>203</v>
+      </c>
+      <c r="C4" s="19" t="s">
+        <v>204</v>
+      </c>
+      <c r="D4" s="4" t="s">
+        <v>16</v>
+      </c>
+      <c r="E4" s="17" t="s">
+        <v>222</v>
+      </c>
+      <c r="F4" s="4" t="s">
+        <v>158</v>
+      </c>
+      <c r="G4" s="4" t="s">
+        <v>205</v>
+      </c>
+      <c r="H4" s="4" t="s">
+        <v>44</v>
+      </c>
+      <c r="I4" s="5">
+        <v>45505</v>
+      </c>
+      <c r="J4" s="5"/>
+      <c r="K4" s="4"/>
+    </row>
   </sheetData>
   <phoneticPr fontId="1" type="noConversion"/>
-  <conditionalFormatting sqref="D2:D3">
+  <conditionalFormatting sqref="D2:D4">
     <cfRule type="expression" dxfId="17" priority="1">
       <formula>D2="Easy"</formula>
     </cfRule>
@@ -4193,11 +4228,12 @@
     </cfRule>
   </conditionalFormatting>
   <hyperlinks>
-    <hyperlink ref="C3" r:id="rId1" xr:uid="{2A05BB37-BC02-459B-AC3A-04B564121776}"/>
-    <hyperlink ref="C2" r:id="rId2" xr:uid="{06DB2703-F6E1-40EC-B489-AF23524010D7}"/>
+    <hyperlink ref="C4" r:id="rId1" xr:uid="{2A05BB37-BC02-459B-AC3A-04B564121776}"/>
+    <hyperlink ref="C3" r:id="rId2" xr:uid="{06DB2703-F6E1-40EC-B489-AF23524010D7}"/>
+    <hyperlink ref="C2" r:id="rId3" xr:uid="{97AD58DC-D294-479E-8558-0A9E71B6BB4E}"/>
   </hyperlinks>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
-  <pageSetup paperSize="9" orientation="portrait" verticalDpi="0" r:id="rId3"/>
+  <pageSetup paperSize="9" orientation="portrait" verticalDpi="0" r:id="rId4"/>
   <headerFooter>
     <oddFooter>&amp;L_x000D_&amp;1#&amp;"Calibri"&amp;10&amp;K000000 General</oddFooter>
   </headerFooter>
@@ -4210,11 +4246,11 @@
   <sheetViews>
     <sheetView zoomScaleNormal="100" workbookViewId="0"/>
   </sheetViews>
-  <sheetFormatPr baseColWidth="10" defaultColWidth="9" defaultRowHeight="17"/>
+  <sheetFormatPr defaultColWidth="9" defaultRowHeight="16.5"/>
   <cols>
     <col min="1" max="1" width="11" customWidth="1"/>
     <col min="2" max="2" width="46" customWidth="1"/>
-    <col min="3" max="3" width="65.796875" style="9" customWidth="1"/>
+    <col min="3" max="3" width="65.85546875" style="9" customWidth="1"/>
     <col min="4" max="4" width="16" customWidth="1"/>
     <col min="5" max="5" width="36" customWidth="1"/>
     <col min="6" max="8" width="21" customWidth="1"/>
@@ -4222,7 +4258,7 @@
     <col min="11" max="11" width="16" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:11" ht="20" customHeight="1">
+    <row r="1" spans="1:11" ht="20.100000000000001" customHeight="1">
       <c r="A1" s="2" t="s">
         <v>4</v>
       </c>
@@ -4257,7 +4293,7 @@
         <v>3</v>
       </c>
     </row>
-    <row r="2" spans="1:11" ht="20" customHeight="1">
+    <row r="2" spans="1:11" ht="20.100000000000001" customHeight="1">
       <c r="A2" s="4">
         <v>208</v>
       </c>
@@ -4284,7 +4320,7 @@
       <c r="J2" s="5"/>
       <c r="K2" s="4"/>
     </row>
-    <row r="3" spans="1:11" ht="20" customHeight="1">
+    <row r="3" spans="1:11" ht="20.100000000000001" customHeight="1">
       <c r="A3" s="4">
         <v>211</v>
       </c>
@@ -4313,7 +4349,7 @@
       <c r="J3" s="5"/>
       <c r="K3" s="4"/>
     </row>
-    <row r="4" spans="1:11" ht="20" customHeight="1">
+    <row r="4" spans="1:11" ht="20.100000000000001" customHeight="1">
       <c r="A4" s="4">
         <v>386</v>
       </c>
@@ -4342,7 +4378,7 @@
       <c r="J4" s="5"/>
       <c r="K4" s="4"/>
     </row>
-    <row r="5" spans="1:11" ht="20" customHeight="1">
+    <row r="5" spans="1:11" ht="20.100000000000001" customHeight="1">
       <c r="A5" s="4">
         <v>648</v>
       </c>
@@ -4369,7 +4405,7 @@
       <c r="J5" s="5"/>
       <c r="K5" s="4"/>
     </row>
-    <row r="6" spans="1:11" ht="20" customHeight="1">
+    <row r="6" spans="1:11" ht="20.100000000000001" customHeight="1">
       <c r="A6" s="4">
         <v>677</v>
       </c>
@@ -4398,7 +4434,7 @@
       <c r="J6" s="5"/>
       <c r="K6" s="4"/>
     </row>
-    <row r="7" spans="1:11" ht="20" customHeight="1">
+    <row r="7" spans="1:11" ht="20.100000000000001" customHeight="1">
       <c r="A7" s="4">
         <v>720</v>
       </c>
@@ -4456,7 +4492,7 @@
       <c r="J8" s="5"/>
       <c r="K8" s="4"/>
     </row>
-    <row r="9" spans="1:11" ht="20" customHeight="1">
+    <row r="9" spans="1:11" ht="20.100000000000001" customHeight="1">
       <c r="A9" s="4">
         <v>1268</v>
       </c>
@@ -4552,10 +4588,10 @@
   <sheetViews>
     <sheetView zoomScaleNormal="100" workbookViewId="0"/>
   </sheetViews>
-  <sheetFormatPr baseColWidth="10" defaultColWidth="9" defaultRowHeight="17"/>
+  <sheetFormatPr defaultColWidth="9" defaultRowHeight="16.5"/>
   <cols>
     <col min="1" max="1" width="11" customWidth="1"/>
-    <col min="2" max="2" width="45.796875" customWidth="1"/>
+    <col min="2" max="2" width="45.85546875" customWidth="1"/>
     <col min="3" max="3" width="71" style="9" customWidth="1"/>
     <col min="4" max="4" width="16" customWidth="1"/>
     <col min="5" max="5" width="36" customWidth="1"/>
@@ -4564,7 +4600,7 @@
     <col min="11" max="11" width="16" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:11" ht="20" customHeight="1">
+    <row r="1" spans="1:11" ht="20.100000000000001" customHeight="1">
       <c r="A1" s="2" t="s">
         <v>4</v>
       </c>
@@ -4599,7 +4635,7 @@
         <v>3</v>
       </c>
     </row>
-    <row r="2" spans="1:11" ht="20" customHeight="1">
+    <row r="2" spans="1:11" ht="20.100000000000001" customHeight="1">
       <c r="A2" s="4">
         <v>3</v>
       </c>
@@ -4626,7 +4662,7 @@
       <c r="J2" s="5"/>
       <c r="K2" s="4"/>
     </row>
-    <row r="3" spans="1:11" ht="20" customHeight="1">
+    <row r="3" spans="1:11" ht="20.100000000000001" customHeight="1">
       <c r="A3" s="4">
         <v>1695</v>
       </c>
@@ -4683,11 +4719,11 @@
   <sheetViews>
     <sheetView zoomScaleNormal="100" workbookViewId="0"/>
   </sheetViews>
-  <sheetFormatPr baseColWidth="10" defaultColWidth="9" defaultRowHeight="17"/>
+  <sheetFormatPr defaultColWidth="9" defaultRowHeight="16.5"/>
   <cols>
     <col min="1" max="1" width="11" customWidth="1"/>
-    <col min="2" max="2" width="28.59765625" customWidth="1"/>
-    <col min="3" max="3" width="65.796875" style="9" customWidth="1"/>
+    <col min="2" max="2" width="28.5703125" customWidth="1"/>
+    <col min="3" max="3" width="65.85546875" style="9" customWidth="1"/>
     <col min="4" max="4" width="16" customWidth="1"/>
     <col min="5" max="5" width="36" customWidth="1"/>
     <col min="6" max="8" width="21" customWidth="1"/>
@@ -4695,7 +4731,7 @@
     <col min="11" max="11" width="16" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:11" ht="20" customHeight="1">
+    <row r="1" spans="1:11" ht="20.100000000000001" customHeight="1">
       <c r="A1" s="2" t="s">
         <v>4</v>
       </c>
@@ -4730,7 +4766,7 @@
         <v>3</v>
       </c>
     </row>
-    <row r="2" spans="1:11" ht="20" customHeight="1">
+    <row r="2" spans="1:11" ht="20.100000000000001" customHeight="1">
       <c r="A2" s="4">
         <v>41</v>
       </c>
@@ -4761,7 +4797,7 @@
       </c>
       <c r="K2" s="4"/>
     </row>
-    <row r="3" spans="1:11" ht="20" customHeight="1">
+    <row r="3" spans="1:11" ht="20.100000000000001" customHeight="1">
       <c r="A3" s="4">
         <v>287</v>
       </c>
@@ -4788,7 +4824,7 @@
       <c r="J3" s="5"/>
       <c r="K3" s="4"/>
     </row>
-    <row r="4" spans="1:11" ht="20" customHeight="1">
+    <row r="4" spans="1:11" ht="20.100000000000001" customHeight="1">
       <c r="A4" s="4">
         <v>645</v>
       </c>

</xml_diff>

<commit_message>
Completed multiple hard practices.
</commit_message>
<xml_diff>
--- a/LeetCode Techniques.xlsx
+++ b/LeetCode Techniques.xlsx
@@ -8,9 +8,9 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="/Users/blackjack625/Desktop/LeetCode/"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{B2CD0202-C13E-8E45-B85F-5F54908FE712}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{72C15E52-D151-644D-81F6-7417FDF820A5}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="0" yWindow="500" windowWidth="28800" windowHeight="16480" activeTab="8" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
+    <workbookView xWindow="0" yWindow="500" windowWidth="28800" windowHeight="16480" activeTab="3" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
   <sheets>
     <sheet name="DP" sheetId="8" r:id="rId1"/>
@@ -49,7 +49,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="1149" uniqueCount="475">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="1190" uniqueCount="492">
   <si>
     <t>Name</t>
   </si>
@@ -1730,10 +1730,6 @@
     <phoneticPr fontId="1" type="noConversion"/>
   </si>
   <si>
-    <t>Recursion.</t>
-    <phoneticPr fontId="1" type="noConversion"/>
-  </si>
-  <si>
     <t>Cinema Seat Allocation</t>
     <phoneticPr fontId="1" type="noConversion"/>
   </si>
@@ -1936,6 +1932,79 @@
   </si>
   <si>
     <t>https://leetcode.com/problems/maximum-points-you-can-obtain-from-cards/description/</t>
+    <phoneticPr fontId="1" type="noConversion"/>
+  </si>
+  <si>
+    <t>Contiguous Array</t>
+    <phoneticPr fontId="1" type="noConversion"/>
+  </si>
+  <si>
+    <t>https://leetcode.com/problems/contiguous-array/description/</t>
+    <phoneticPr fontId="1" type="noConversion"/>
+  </si>
+  <si>
+    <t>Subarray Product Less Than K</t>
+    <phoneticPr fontId="1" type="noConversion"/>
+  </si>
+  <si>
+    <t>https://leetcode.com/problems/subarray-product-less-than-k/description/</t>
+    <phoneticPr fontId="1" type="noConversion"/>
+  </si>
+  <si>
+    <t>Make Array Empty</t>
+    <phoneticPr fontId="1" type="noConversion"/>
+  </si>
+  <si>
+    <t>https://leetcode.com/problems/make-array-empty/description/</t>
+    <phoneticPr fontId="1" type="noConversion"/>
+  </si>
+  <si>
+    <t>Greedy</t>
+    <phoneticPr fontId="1" type="noConversion"/>
+  </si>
+  <si>
+    <t>Reverse Subarray To Maximize Array Value</t>
+    <phoneticPr fontId="15" type="noConversion"/>
+  </si>
+  <si>
+    <t>https://leetcode.com/problems/reverse-subarray-to-maximize-array-value/description/</t>
+    <phoneticPr fontId="15" type="noConversion"/>
+  </si>
+  <si>
+    <t>Find Servers That Handled Most Number of Requests</t>
+    <phoneticPr fontId="15" type="noConversion"/>
+  </si>
+  <si>
+    <t>https://leetcode.com/problems/find-servers-that-handled-most-number-of-requests/description/</t>
+    <phoneticPr fontId="15" type="noConversion"/>
+  </si>
+  <si>
+    <t>Binary Search, Greedy</t>
+    <phoneticPr fontId="1" type="noConversion"/>
+  </si>
+  <si>
+    <t>https://leetcode.com/problems/meeting-rooms-iii/description/</t>
+    <phoneticPr fontId="15" type="noConversion"/>
+  </si>
+  <si>
+    <t>Meeting Rooms III</t>
+    <phoneticPr fontId="1" type="noConversion"/>
+  </si>
+  <si>
+    <t>Heaps</t>
+    <phoneticPr fontId="1" type="noConversion"/>
+  </si>
+  <si>
+    <t>Set Intersection Size At Least Two</t>
+    <phoneticPr fontId="1" type="noConversion"/>
+  </si>
+  <si>
+    <t>https://leetcode.com/problems/set-intersection-size-at-least-two/description/</t>
+    <phoneticPr fontId="1" type="noConversion"/>
+  </si>
+  <si>
+    <t>Deal with more "interior-located"
+and smaller intervals first.</t>
     <phoneticPr fontId="1" type="noConversion"/>
   </si>
 </sst>
@@ -4139,18 +4208,19 @@
 
 <file path=xl/worksheets/sheet12.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{99BCE9F1-E6C6-6346-98A0-65D0C06C0EE4}">
-  <dimension ref="A1:K5"/>
+  <dimension ref="A1:K6"/>
   <sheetViews>
     <sheetView zoomScaleNormal="100" workbookViewId="0"/>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultColWidth="9" defaultRowHeight="16"/>
   <cols>
     <col min="1" max="1" width="11" customWidth="1"/>
-    <col min="2" max="2" width="46" customWidth="1"/>
+    <col min="2" max="2" width="56" customWidth="1"/>
     <col min="3" max="3" width="35.796875" style="11" customWidth="1"/>
     <col min="4" max="4" width="16" customWidth="1"/>
     <col min="5" max="5" width="41" customWidth="1"/>
-    <col min="6" max="8" width="21" customWidth="1"/>
+    <col min="6" max="6" width="23.59765625" customWidth="1"/>
+    <col min="7" max="8" width="21" customWidth="1"/>
     <col min="9" max="10" width="16" style="1" customWidth="1"/>
     <col min="11" max="11" width="16" customWidth="1"/>
   </cols>
@@ -4253,16 +4323,16 @@
         <v>1354</v>
       </c>
       <c r="B4" s="6" t="s">
+        <v>467</v>
+      </c>
+      <c r="C4" s="8" t="s">
         <v>468</v>
-      </c>
-      <c r="C4" s="8" t="s">
-        <v>469</v>
       </c>
       <c r="D4" s="4" t="s">
         <v>15</v>
       </c>
       <c r="E4" s="14" t="s">
-        <v>470</v>
+        <v>469</v>
       </c>
       <c r="F4" s="4"/>
       <c r="G4" s="4" t="s">
@@ -4279,41 +4349,70 @@
     </row>
     <row r="5" spans="1:11" ht="20" customHeight="1">
       <c r="A5" s="6">
-        <v>1845</v>
+        <v>1606</v>
       </c>
       <c r="B5" s="6" t="s">
-        <v>471</v>
+        <v>483</v>
       </c>
       <c r="C5" s="8" t="s">
-        <v>472</v>
+        <v>484</v>
       </c>
       <c r="D5" s="4" t="s">
-        <v>10</v>
+        <v>15</v>
       </c>
       <c r="E5" s="14"/>
-      <c r="F5" s="4"/>
+      <c r="F5" s="4" t="s">
+        <v>485</v>
+      </c>
       <c r="G5" s="4" t="s">
-        <v>13</v>
+        <v>12</v>
       </c>
       <c r="H5" s="4" t="s">
         <v>11</v>
       </c>
       <c r="I5" s="5">
-        <v>45568</v>
+        <v>45574</v>
       </c>
       <c r="J5" s="5"/>
       <c r="K5" s="4"/>
     </row>
+    <row r="6" spans="1:11" ht="20" customHeight="1">
+      <c r="A6" s="6">
+        <v>1845</v>
+      </c>
+      <c r="B6" s="6" t="s">
+        <v>470</v>
+      </c>
+      <c r="C6" s="8" t="s">
+        <v>471</v>
+      </c>
+      <c r="D6" s="4" t="s">
+        <v>10</v>
+      </c>
+      <c r="E6" s="14"/>
+      <c r="F6" s="4"/>
+      <c r="G6" s="4" t="s">
+        <v>13</v>
+      </c>
+      <c r="H6" s="4" t="s">
+        <v>11</v>
+      </c>
+      <c r="I6" s="5">
+        <v>45568</v>
+      </c>
+      <c r="J6" s="5"/>
+      <c r="K6" s="4"/>
+    </row>
   </sheetData>
   <phoneticPr fontId="1" type="noConversion"/>
-  <conditionalFormatting sqref="D2:E5">
-    <cfRule type="expression" dxfId="20" priority="1">
+  <conditionalFormatting sqref="D2:E6">
+    <cfRule type="expression" dxfId="20" priority="4">
       <formula>D2="Easy"</formula>
     </cfRule>
-    <cfRule type="expression" dxfId="19" priority="2">
+    <cfRule type="expression" dxfId="19" priority="5">
       <formula>D2="Medium"</formula>
     </cfRule>
-    <cfRule type="expression" dxfId="18" priority="3">
+    <cfRule type="expression" dxfId="18" priority="6">
       <formula>D2="Hard"</formula>
     </cfRule>
   </conditionalFormatting>
@@ -4321,10 +4420,11 @@
     <hyperlink ref="C3" r:id="rId1" xr:uid="{BD755528-4D9F-2E43-8D44-F83835331DEA}"/>
     <hyperlink ref="C2" r:id="rId2" xr:uid="{322F67A3-4E60-134A-9BA1-AF1822132017}"/>
     <hyperlink ref="C4" r:id="rId3" xr:uid="{8B0936F4-A412-3541-AF80-6424433632D0}"/>
-    <hyperlink ref="C5" r:id="rId4" xr:uid="{CA92A266-1266-FE4A-88E7-BEE47D7CBF4E}"/>
+    <hyperlink ref="C6" r:id="rId4" xr:uid="{CA92A266-1266-FE4A-88E7-BEE47D7CBF4E}"/>
+    <hyperlink ref="C5" r:id="rId5" xr:uid="{3D46B33F-B75E-E14C-85F8-97D14E32302E}"/>
   </hyperlinks>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
-  <pageSetup paperSize="9" orientation="portrait" verticalDpi="0" r:id="rId5"/>
+  <pageSetup paperSize="9" orientation="portrait" verticalDpi="0" r:id="rId6"/>
   <headerFooter>
     <oddFooter>&amp;L_x000D_&amp;1#&amp;"Calibri"&amp;10&amp;K000000 General</oddFooter>
   </headerFooter>
@@ -5755,16 +5855,16 @@
         <v>646</v>
       </c>
       <c r="B14" s="4" t="s">
+        <v>438</v>
+      </c>
+      <c r="C14" s="8" t="s">
         <v>439</v>
-      </c>
-      <c r="C14" s="8" t="s">
-        <v>440</v>
       </c>
       <c r="D14" s="4" t="s">
         <v>10</v>
       </c>
       <c r="E14" s="2" t="s">
-        <v>438</v>
+        <v>437</v>
       </c>
       <c r="F14" s="4"/>
       <c r="G14" s="4" t="s">
@@ -6597,19 +6697,21 @@
 
 <file path=xl/worksheets/sheet4.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{B15C51FE-E345-E84D-98FD-767C3C081D66}">
-  <dimension ref="A1:K5"/>
+  <dimension ref="A1:K8"/>
   <sheetViews>
-    <sheetView zoomScaleNormal="100" workbookViewId="0"/>
+    <sheetView tabSelected="1" zoomScaleNormal="100" workbookViewId="0"/>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultColWidth="9" defaultRowHeight="16"/>
   <cols>
     <col min="1" max="1" width="11" customWidth="1"/>
-    <col min="2" max="2" width="31" customWidth="1"/>
+    <col min="2" max="2" width="36" customWidth="1"/>
     <col min="3" max="3" width="35.796875" style="11" customWidth="1"/>
     <col min="4" max="4" width="16" customWidth="1"/>
-    <col min="5" max="5" width="41" customWidth="1"/>
-    <col min="6" max="8" width="21" customWidth="1"/>
-    <col min="9" max="10" width="16" style="1" customWidth="1"/>
+    <col min="5" max="5" width="36" customWidth="1"/>
+    <col min="6" max="6" width="23.59765625" customWidth="1"/>
+    <col min="7" max="8" width="21" customWidth="1"/>
+    <col min="9" max="9" width="18.59765625" style="1" customWidth="1"/>
+    <col min="10" max="10" width="16" style="1" customWidth="1"/>
     <col min="11" max="11" width="16" customWidth="1"/>
   </cols>
   <sheetData>
@@ -6665,7 +6767,7 @@
         <v>423</v>
       </c>
       <c r="F2" s="4" t="s">
-        <v>424</v>
+        <v>364</v>
       </c>
       <c r="G2" s="4" t="s">
         <v>12</v>
@@ -6696,7 +6798,7 @@
         <v>420</v>
       </c>
       <c r="F3" s="4" t="s">
-        <v>424</v>
+        <v>364</v>
       </c>
       <c r="G3" s="4" t="s">
         <v>12</v>
@@ -6715,10 +6817,10 @@
         <v>324</v>
       </c>
       <c r="B4" s="4" t="s">
+        <v>429</v>
+      </c>
+      <c r="C4" s="8" t="s">
         <v>430</v>
-      </c>
-      <c r="C4" s="8" t="s">
-        <v>431</v>
       </c>
       <c r="D4" s="4" t="s">
         <v>10</v>
@@ -6737,54 +6839,146 @@
       <c r="J4" s="5"/>
       <c r="K4" s="2"/>
     </row>
-    <row r="5" spans="1:11" ht="20" customHeight="1">
+    <row r="5" spans="1:11" ht="30" customHeight="1">
       <c r="A5" s="4">
-        <v>1386</v>
+        <v>757</v>
       </c>
       <c r="B5" s="4" t="s">
-        <v>425</v>
+        <v>489</v>
       </c>
       <c r="C5" s="8" t="s">
-        <v>426</v>
+        <v>490</v>
       </c>
       <c r="D5" s="4" t="s">
-        <v>10</v>
-      </c>
-      <c r="E5" s="4"/>
-      <c r="F5" s="4"/>
+        <v>15</v>
+      </c>
+      <c r="E5" s="14" t="s">
+        <v>491</v>
+      </c>
+      <c r="F5" s="4" t="s">
+        <v>485</v>
+      </c>
       <c r="G5" s="4" t="s">
         <v>12</v>
       </c>
       <c r="H5" s="4" t="s">
-        <v>28</v>
+        <v>11</v>
       </c>
       <c r="I5" s="5">
-        <v>45533</v>
+        <v>45575</v>
       </c>
       <c r="J5" s="5"/>
       <c r="K5" s="2"/>
     </row>
+    <row r="6" spans="1:11" ht="20" customHeight="1">
+      <c r="A6" s="4">
+        <v>1386</v>
+      </c>
+      <c r="B6" s="4" t="s">
+        <v>424</v>
+      </c>
+      <c r="C6" s="8" t="s">
+        <v>425</v>
+      </c>
+      <c r="D6" s="4" t="s">
+        <v>10</v>
+      </c>
+      <c r="E6" s="4"/>
+      <c r="F6" s="4"/>
+      <c r="G6" s="4" t="s">
+        <v>12</v>
+      </c>
+      <c r="H6" s="4" t="s">
+        <v>28</v>
+      </c>
+      <c r="I6" s="5">
+        <v>45533</v>
+      </c>
+      <c r="J6" s="5"/>
+      <c r="K6" s="2"/>
+    </row>
+    <row r="7" spans="1:11" ht="20" customHeight="1">
+      <c r="A7" s="6">
+        <v>2402</v>
+      </c>
+      <c r="B7" s="6" t="s">
+        <v>487</v>
+      </c>
+      <c r="C7" s="8" t="s">
+        <v>486</v>
+      </c>
+      <c r="D7" s="4" t="s">
+        <v>15</v>
+      </c>
+      <c r="E7" s="14"/>
+      <c r="F7" s="4" t="s">
+        <v>488</v>
+      </c>
+      <c r="G7" s="4" t="s">
+        <v>12</v>
+      </c>
+      <c r="H7" s="4" t="s">
+        <v>11</v>
+      </c>
+      <c r="I7" s="5">
+        <v>45574</v>
+      </c>
+      <c r="J7" s="5"/>
+      <c r="K7" s="4"/>
+    </row>
+    <row r="8" spans="1:11" ht="20" customHeight="1">
+      <c r="A8" s="4">
+        <v>2659</v>
+      </c>
+      <c r="B8" s="4" t="s">
+        <v>478</v>
+      </c>
+      <c r="C8" s="8" t="s">
+        <v>479</v>
+      </c>
+      <c r="D8" s="4" t="s">
+        <v>15</v>
+      </c>
+      <c r="E8" s="6"/>
+      <c r="F8" s="4" t="s">
+        <v>480</v>
+      </c>
+      <c r="G8" s="4" t="s">
+        <v>12</v>
+      </c>
+      <c r="H8" s="4" t="s">
+        <v>11</v>
+      </c>
+      <c r="I8" s="5">
+        <v>45403</v>
+      </c>
+      <c r="J8" s="5"/>
+      <c r="K8" s="2"/>
+    </row>
   </sheetData>
   <phoneticPr fontId="1" type="noConversion"/>
-  <conditionalFormatting sqref="D2:E5">
-    <cfRule type="expression" dxfId="44" priority="1">
+  <conditionalFormatting sqref="D2:E8">
+    <cfRule type="expression" dxfId="44" priority="4">
       <formula>D2="Easy"</formula>
     </cfRule>
-    <cfRule type="expression" dxfId="43" priority="2">
+    <cfRule type="expression" dxfId="43" priority="5">
       <formula>D2="Medium"</formula>
     </cfRule>
-    <cfRule type="expression" dxfId="42" priority="3">
+    <cfRule type="expression" dxfId="42" priority="6">
       <formula>D2="Hard"</formula>
     </cfRule>
   </conditionalFormatting>
   <hyperlinks>
     <hyperlink ref="C3" r:id="rId1" xr:uid="{5CD9AE50-AA9E-4A4B-861F-3841A5AD013F}"/>
     <hyperlink ref="C2" r:id="rId2" xr:uid="{BF96CE91-DED9-584B-BD53-695EAACF8656}"/>
-    <hyperlink ref="C5" r:id="rId3" xr:uid="{4791A1EA-B34F-6140-A8AF-3403CBC4BB3B}"/>
+    <hyperlink ref="C6" r:id="rId3" xr:uid="{4791A1EA-B34F-6140-A8AF-3403CBC4BB3B}"/>
     <hyperlink ref="C4" r:id="rId4" xr:uid="{D09CA923-D79F-7147-A238-200BD0D14D79}"/>
+    <hyperlink ref="C8" r:id="rId5" xr:uid="{15AF7E95-A712-CF46-80E2-8E66AEE8EF6A}"/>
+    <hyperlink ref="C7" r:id="rId6" xr:uid="{B471486E-8451-864F-9806-678B49CACA46}"/>
+    <hyperlink ref="C5" r:id="rId7" xr:uid="{9131687D-A6D4-444C-9270-AA4EFDFB268A}"/>
   </hyperlinks>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
-  <pageSetup paperSize="9" orientation="portrait" verticalDpi="0" r:id="rId5"/>
+  <pageSetup paperSize="9" orientation="portrait" verticalDpi="0" r:id="rId8"/>
   <headerFooter>
     <oddFooter>&amp;L_x000D_&amp;1#&amp;"Calibri"&amp;10&amp;K000000 General</oddFooter>
   </headerFooter>
@@ -6793,7 +6987,7 @@
 
 <file path=xl/worksheets/sheet5.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{89924C3E-917D-0945-8F52-65F70A8CFC07}">
-  <dimension ref="A1:K21"/>
+  <dimension ref="A1:K22"/>
   <sheetViews>
     <sheetView zoomScaleNormal="100" workbookViewId="0"/>
   </sheetViews>
@@ -6880,16 +7074,16 @@
         <v>334</v>
       </c>
       <c r="B3" s="6" t="s">
+        <v>435</v>
+      </c>
+      <c r="C3" s="8" t="s">
         <v>436</v>
-      </c>
-      <c r="C3" s="8" t="s">
-        <v>437</v>
       </c>
       <c r="D3" s="4" t="s">
         <v>10</v>
       </c>
       <c r="E3" s="14" t="s">
-        <v>438</v>
+        <v>437</v>
       </c>
       <c r="F3" s="4" t="s">
         <v>267</v>
@@ -6911,10 +7105,10 @@
         <v>624</v>
       </c>
       <c r="B4" s="6" t="s">
+        <v>431</v>
+      </c>
+      <c r="C4" s="8" t="s">
         <v>432</v>
-      </c>
-      <c r="C4" s="8" t="s">
-        <v>433</v>
       </c>
       <c r="D4" s="4" t="s">
         <v>10</v>
@@ -6967,17 +7161,17 @@
         <v>670</v>
       </c>
       <c r="B6" s="6" t="s">
+        <v>440</v>
+      </c>
+      <c r="C6" s="8" t="s">
         <v>441</v>
-      </c>
-      <c r="C6" s="8" t="s">
-        <v>442</v>
       </c>
       <c r="D6" s="4" t="s">
         <v>10</v>
       </c>
       <c r="E6" s="6"/>
       <c r="F6" s="4" t="s">
-        <v>429</v>
+        <v>428</v>
       </c>
       <c r="G6" s="4" t="s">
         <v>372</v>
@@ -7029,19 +7223,19 @@
         <v>768</v>
       </c>
       <c r="B8" s="6" t="s">
+        <v>444</v>
+      </c>
+      <c r="C8" s="8" t="s">
         <v>445</v>
-      </c>
-      <c r="C8" s="8" t="s">
-        <v>446</v>
       </c>
       <c r="D8" s="4" t="s">
         <v>15</v>
       </c>
       <c r="E8" s="14" t="s">
-        <v>461</v>
+        <v>460</v>
       </c>
       <c r="F8" s="4" t="s">
-        <v>460</v>
+        <v>459</v>
       </c>
       <c r="G8" s="4" t="s">
         <v>372</v>
@@ -7062,19 +7256,19 @@
         <v>769</v>
       </c>
       <c r="B9" s="6" t="s">
+        <v>442</v>
+      </c>
+      <c r="C9" s="8" t="s">
         <v>443</v>
-      </c>
-      <c r="C9" s="8" t="s">
-        <v>444</v>
       </c>
       <c r="D9" s="4" t="s">
         <v>10</v>
       </c>
       <c r="E9" s="14" t="s">
-        <v>461</v>
+        <v>460</v>
       </c>
       <c r="F9" s="4" t="s">
-        <v>460</v>
+        <v>459</v>
       </c>
       <c r="G9" s="4" t="s">
         <v>372</v>
@@ -7095,17 +7289,17 @@
         <v>781</v>
       </c>
       <c r="B10" s="6" t="s">
+        <v>464</v>
+      </c>
+      <c r="C10" s="8" t="s">
         <v>465</v>
-      </c>
-      <c r="C10" s="8" t="s">
-        <v>466</v>
       </c>
       <c r="D10" s="4" t="s">
         <v>10</v>
       </c>
       <c r="E10" s="14"/>
       <c r="F10" s="4" t="s">
-        <v>467</v>
+        <v>466</v>
       </c>
       <c r="G10" s="4" t="s">
         <v>372</v>
@@ -7124,10 +7318,10 @@
         <v>826</v>
       </c>
       <c r="B11" s="6" t="s">
+        <v>446</v>
+      </c>
+      <c r="C11" s="8" t="s">
         <v>447</v>
-      </c>
-      <c r="C11" s="8" t="s">
-        <v>448</v>
       </c>
       <c r="D11" s="4" t="s">
         <v>10</v>
@@ -7182,10 +7376,10 @@
         <v>954</v>
       </c>
       <c r="B13" s="6" t="s">
+        <v>455</v>
+      </c>
+      <c r="C13" s="8" t="s">
         <v>456</v>
-      </c>
-      <c r="C13" s="8" t="s">
-        <v>457</v>
       </c>
       <c r="D13" s="4" t="s">
         <v>10</v>
@@ -7211,23 +7405,23 @@
         <v>984</v>
       </c>
       <c r="B14" s="6" t="s">
+        <v>448</v>
+      </c>
+      <c r="C14" s="8" t="s">
         <v>449</v>
-      </c>
-      <c r="C14" s="8" t="s">
-        <v>450</v>
       </c>
       <c r="D14" s="4" t="s">
         <v>10</v>
       </c>
       <c r="E14" s="14" t="s">
-        <v>452</v>
+        <v>451</v>
       </c>
       <c r="F14" s="4"/>
       <c r="G14" s="4" t="s">
-        <v>453</v>
+        <v>452</v>
       </c>
       <c r="H14" s="4" t="s">
-        <v>451</v>
+        <v>450</v>
       </c>
       <c r="I14" s="5">
         <v>45562</v>
@@ -7273,10 +7467,10 @@
         <v>1144</v>
       </c>
       <c r="B16" s="6" t="s">
+        <v>433</v>
+      </c>
+      <c r="C16" s="8" t="s">
         <v>434</v>
-      </c>
-      <c r="C16" s="8" t="s">
-        <v>435</v>
       </c>
       <c r="D16" s="4" t="s">
         <v>10</v>
@@ -7297,51 +7491,47 @@
     </row>
     <row r="17" spans="1:11" ht="20" customHeight="1">
       <c r="A17" s="6">
-        <v>1363</v>
+        <v>1330</v>
       </c>
       <c r="B17" s="6" t="s">
-        <v>454</v>
+        <v>481</v>
       </c>
       <c r="C17" s="8" t="s">
-        <v>455</v>
+        <v>482</v>
       </c>
       <c r="D17" s="4" t="s">
         <v>15</v>
       </c>
       <c r="E17" s="14"/>
-      <c r="F17" s="4" t="s">
-        <v>429</v>
-      </c>
+      <c r="F17" s="4"/>
       <c r="G17" s="4" t="s">
         <v>372</v>
       </c>
       <c r="H17" s="4" t="s">
-        <v>43</v>
+        <v>28</v>
       </c>
       <c r="I17" s="5">
-        <v>45563</v>
-      </c>
-      <c r="J17" s="5">
-        <v>45567</v>
-      </c>
+        <v>45573</v>
+      </c>
+      <c r="J17" s="5"/>
       <c r="K17" s="4"/>
     </row>
     <row r="18" spans="1:11" ht="20" customHeight="1">
       <c r="A18" s="6">
-        <v>1481</v>
+        <v>1363</v>
       </c>
       <c r="B18" s="6" t="s">
-        <v>427</v>
+        <v>453</v>
       </c>
       <c r="C18" s="8" t="s">
-        <v>428</v>
+        <v>454</v>
       </c>
       <c r="D18" s="4" t="s">
-        <v>10</v>
+        <v>15</v>
       </c>
       <c r="E18" s="14"/>
       <c r="F18" s="4" t="s">
-        <v>429</v>
+        <v>428</v>
       </c>
       <c r="G18" s="4" t="s">
         <v>372</v>
@@ -7350,105 +7540,136 @@
         <v>43</v>
       </c>
       <c r="I18" s="5">
-        <v>45550</v>
-      </c>
-      <c r="J18" s="5"/>
+        <v>45563</v>
+      </c>
+      <c r="J18" s="5">
+        <v>45567</v>
+      </c>
       <c r="K18" s="4"/>
     </row>
     <row r="19" spans="1:11" ht="20" customHeight="1">
       <c r="A19" s="6">
-        <v>1713</v>
+        <v>1481</v>
       </c>
       <c r="B19" s="6" t="s">
-        <v>458</v>
+        <v>426</v>
       </c>
       <c r="C19" s="8" t="s">
-        <v>459</v>
+        <v>427</v>
       </c>
       <c r="D19" s="4" t="s">
-        <v>15</v>
-      </c>
-      <c r="E19" s="14" t="s">
-        <v>438</v>
-      </c>
+        <v>10</v>
+      </c>
+      <c r="E19" s="14"/>
       <c r="F19" s="4" t="s">
-        <v>267</v>
+        <v>428</v>
       </c>
       <c r="G19" s="4" t="s">
-        <v>309</v>
+        <v>372</v>
       </c>
       <c r="H19" s="4" t="s">
         <v>43</v>
       </c>
       <c r="I19" s="5">
-        <v>45563</v>
+        <v>45550</v>
       </c>
       <c r="J19" s="5"/>
       <c r="K19" s="4"/>
     </row>
-    <row r="20" spans="1:11" ht="30" customHeight="1">
+    <row r="20" spans="1:11" ht="20" customHeight="1">
       <c r="A20" s="6">
-        <v>2202</v>
+        <v>1713</v>
       </c>
       <c r="B20" s="6" t="s">
-        <v>462</v>
+        <v>457</v>
       </c>
       <c r="C20" s="8" t="s">
-        <v>463</v>
+        <v>458</v>
       </c>
       <c r="D20" s="4" t="s">
-        <v>10</v>
+        <v>15</v>
       </c>
       <c r="E20" s="14" t="s">
-        <v>464</v>
-      </c>
-      <c r="F20" s="4"/>
+        <v>437</v>
+      </c>
+      <c r="F20" s="4" t="s">
+        <v>267</v>
+      </c>
       <c r="G20" s="4" t="s">
-        <v>255</v>
+        <v>309</v>
       </c>
       <c r="H20" s="4" t="s">
-        <v>28</v>
+        <v>43</v>
       </c>
       <c r="I20" s="5">
-        <v>45568</v>
+        <v>45563</v>
       </c>
       <c r="J20" s="5"/>
       <c r="K20" s="4"/>
     </row>
     <row r="21" spans="1:11" ht="30" customHeight="1">
       <c r="A21" s="6">
-        <v>2208</v>
+        <v>2202</v>
       </c>
       <c r="B21" s="6" t="s">
-        <v>403</v>
+        <v>461</v>
       </c>
       <c r="C21" s="8" t="s">
-        <v>404</v>
+        <v>462</v>
       </c>
       <c r="D21" s="4" t="s">
         <v>10</v>
       </c>
       <c r="E21" s="14" t="s">
-        <v>407</v>
-      </c>
-      <c r="F21" s="4" t="s">
-        <v>413</v>
-      </c>
+        <v>463</v>
+      </c>
+      <c r="F21" s="4"/>
       <c r="G21" s="4" t="s">
-        <v>405</v>
+        <v>255</v>
       </c>
       <c r="H21" s="4" t="s">
-        <v>43</v>
+        <v>28</v>
       </c>
       <c r="I21" s="5">
-        <v>45548</v>
+        <v>45568</v>
       </c>
       <c r="J21" s="5"/>
       <c r="K21" s="4"/>
     </row>
+    <row r="22" spans="1:11" ht="30" customHeight="1">
+      <c r="A22" s="6">
+        <v>2208</v>
+      </c>
+      <c r="B22" s="6" t="s">
+        <v>403</v>
+      </c>
+      <c r="C22" s="8" t="s">
+        <v>404</v>
+      </c>
+      <c r="D22" s="4" t="s">
+        <v>10</v>
+      </c>
+      <c r="E22" s="14" t="s">
+        <v>407</v>
+      </c>
+      <c r="F22" s="4" t="s">
+        <v>413</v>
+      </c>
+      <c r="G22" s="4" t="s">
+        <v>405</v>
+      </c>
+      <c r="H22" s="4" t="s">
+        <v>43</v>
+      </c>
+      <c r="I22" s="5">
+        <v>45548</v>
+      </c>
+      <c r="J22" s="5"/>
+      <c r="K22" s="4"/>
+    </row>
   </sheetData>
   <phoneticPr fontId="1" type="noConversion"/>
-  <conditionalFormatting sqref="D2:E21">
+  <conditionalFormatting sqref="D2:E22">
     <cfRule type="expression" dxfId="41" priority="10">
       <formula>D2="Easy"</formula>
     </cfRule>
@@ -7464,9 +7685,9 @@
     <hyperlink ref="C5" r:id="rId2" xr:uid="{36C30514-0199-314C-B206-B46F26E6E895}"/>
     <hyperlink ref="C15" r:id="rId3" xr:uid="{A61EDB76-3F1B-FA4B-A484-FF203AB7B891}"/>
     <hyperlink ref="C7" r:id="rId4" xr:uid="{14F26B79-16C3-8A42-AA1C-424413893725}"/>
-    <hyperlink ref="C21" r:id="rId5" xr:uid="{532B70B2-4EA8-D54B-9765-F0F8FB4A7228}"/>
+    <hyperlink ref="C22" r:id="rId5" xr:uid="{532B70B2-4EA8-D54B-9765-F0F8FB4A7228}"/>
     <hyperlink ref="C12" r:id="rId6" xr:uid="{E0EF768C-A209-C344-A308-201CBA67EFDA}"/>
-    <hyperlink ref="C18" r:id="rId7" xr:uid="{98E20983-FDF7-AC45-A77E-381E42FA3D7E}"/>
+    <hyperlink ref="C19" r:id="rId7" xr:uid="{98E20983-FDF7-AC45-A77E-381E42FA3D7E}"/>
     <hyperlink ref="C4" r:id="rId8" xr:uid="{93109F7A-39AF-394A-8F0E-7C9872B616F2}"/>
     <hyperlink ref="C16" r:id="rId9" xr:uid="{C5BC2EF5-2492-454F-9C71-DDEE7A2E3E98}"/>
     <hyperlink ref="C3" r:id="rId10" xr:uid="{74E3D31C-3C7B-114C-841C-89AAD24C4905}"/>
@@ -7475,14 +7696,15 @@
     <hyperlink ref="C9" r:id="rId13" xr:uid="{D1A42B51-B36E-E640-B035-BA6DA18FBA31}"/>
     <hyperlink ref="C11" r:id="rId14" xr:uid="{200A1572-C064-7B45-8135-A89DFAE16BF8}"/>
     <hyperlink ref="C14" r:id="rId15" xr:uid="{1C03B438-9BDB-D34F-BD78-ED5E5562BF65}"/>
-    <hyperlink ref="C17" r:id="rId16" xr:uid="{C01F0CDD-3830-7E4F-BA4D-F73C5F99952F}"/>
+    <hyperlink ref="C18" r:id="rId16" xr:uid="{C01F0CDD-3830-7E4F-BA4D-F73C5F99952F}"/>
     <hyperlink ref="C13" r:id="rId17" xr:uid="{AD3FCB87-A1B2-2A49-8380-673BAAF1CB03}"/>
-    <hyperlink ref="C19" r:id="rId18" xr:uid="{78660B06-7405-C049-A32B-24A1D90AF311}"/>
-    <hyperlink ref="C20" r:id="rId19" xr:uid="{A4D38E4E-BEF9-7E4B-91E4-A344DBE2326F}"/>
+    <hyperlink ref="C20" r:id="rId18" xr:uid="{78660B06-7405-C049-A32B-24A1D90AF311}"/>
+    <hyperlink ref="C21" r:id="rId19" xr:uid="{A4D38E4E-BEF9-7E4B-91E4-A344DBE2326F}"/>
     <hyperlink ref="C10" r:id="rId20" xr:uid="{3085500C-981B-3640-9778-9E0E68921A9C}"/>
+    <hyperlink ref="C17" r:id="rId21" xr:uid="{DE2E7DCF-21D8-D143-8908-D8983E22C6CE}"/>
   </hyperlinks>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
-  <pageSetup paperSize="9" orientation="portrait" verticalDpi="0" r:id="rId21"/>
+  <pageSetup paperSize="9" orientation="portrait" verticalDpi="0" r:id="rId22"/>
   <headerFooter>
     <oddFooter>&amp;L_x000D_&amp;1#&amp;"Calibri"&amp;10&amp;K000000 General</oddFooter>
   </headerFooter>
@@ -7502,7 +7724,8 @@
     <col min="3" max="3" width="71" style="11" customWidth="1"/>
     <col min="4" max="4" width="16" customWidth="1"/>
     <col min="5" max="5" width="36" customWidth="1"/>
-    <col min="6" max="8" width="21" customWidth="1"/>
+    <col min="6" max="6" width="18.59765625" customWidth="1"/>
+    <col min="7" max="8" width="21" customWidth="1"/>
     <col min="9" max="10" width="16" style="1" customWidth="1"/>
     <col min="11" max="11" width="16" customWidth="1"/>
   </cols>
@@ -8795,9 +9018,9 @@
 
 <file path=xl/worksheets/sheet9.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{8380FC83-7509-9643-8CC5-E365761A27D0}">
-  <dimension ref="A1:K15"/>
+  <dimension ref="A1:K17"/>
   <sheetViews>
-    <sheetView tabSelected="1" zoomScaleNormal="100" workbookViewId="0"/>
+    <sheetView zoomScaleNormal="100" workbookViewId="0"/>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultColWidth="9" defaultRowHeight="16"/>
   <cols>
@@ -8902,79 +9125,79 @@
     </row>
     <row r="4" spans="1:11" ht="20" customHeight="1">
       <c r="A4" s="6">
-        <v>528</v>
+        <v>525</v>
       </c>
       <c r="B4" s="6" t="s">
-        <v>292</v>
+        <v>474</v>
       </c>
       <c r="C4" s="8" t="s">
-        <v>291</v>
+        <v>475</v>
       </c>
       <c r="D4" s="4" t="s">
         <v>10</v>
       </c>
       <c r="E4" s="14"/>
-      <c r="F4" s="4" t="s">
-        <v>267</v>
-      </c>
+      <c r="F4" s="4"/>
       <c r="G4" s="4" t="s">
-        <v>13</v>
+        <v>11</v>
       </c>
       <c r="H4" s="4" t="s">
         <v>11</v>
       </c>
       <c r="I4" s="5">
-        <v>45525</v>
+        <v>45570</v>
       </c>
       <c r="J4" s="5"/>
       <c r="K4" s="4"/>
     </row>
     <row r="5" spans="1:11" ht="20" customHeight="1">
       <c r="A5" s="6">
-        <v>560</v>
+        <v>528</v>
       </c>
       <c r="B5" s="6" t="s">
-        <v>399</v>
+        <v>292</v>
       </c>
       <c r="C5" s="8" t="s">
-        <v>400</v>
+        <v>291</v>
       </c>
       <c r="D5" s="4" t="s">
         <v>10</v>
       </c>
-      <c r="E5" s="14" t="s">
-        <v>402</v>
-      </c>
+      <c r="E5" s="14"/>
       <c r="F5" s="4" t="s">
-        <v>401</v>
+        <v>267</v>
       </c>
       <c r="G5" s="4" t="s">
-        <v>11</v>
+        <v>13</v>
       </c>
       <c r="H5" s="4" t="s">
         <v>11</v>
       </c>
       <c r="I5" s="5">
-        <v>45547</v>
+        <v>45525</v>
       </c>
       <c r="J5" s="5"/>
       <c r="K5" s="4"/>
     </row>
     <row r="6" spans="1:11" ht="20" customHeight="1">
       <c r="A6" s="6">
-        <v>848</v>
+        <v>560</v>
       </c>
       <c r="B6" s="6" t="s">
-        <v>294</v>
+        <v>399</v>
       </c>
       <c r="C6" s="8" t="s">
-        <v>293</v>
+        <v>400</v>
       </c>
       <c r="D6" s="4" t="s">
         <v>10</v>
       </c>
-      <c r="E6" s="14"/>
-      <c r="F6" s="4"/>
+      <c r="E6" s="14" t="s">
+        <v>402</v>
+      </c>
+      <c r="F6" s="4" t="s">
+        <v>401</v>
+      </c>
       <c r="G6" s="4" t="s">
         <v>11</v>
       </c>
@@ -8982,23 +9205,23 @@
         <v>11</v>
       </c>
       <c r="I6" s="5">
-        <v>45525</v>
+        <v>45547</v>
       </c>
       <c r="J6" s="5"/>
       <c r="K6" s="4"/>
     </row>
     <row r="7" spans="1:11" ht="20" customHeight="1">
       <c r="A7" s="6">
-        <v>862</v>
+        <v>713</v>
       </c>
       <c r="B7" s="6" t="s">
-        <v>286</v>
+        <v>476</v>
       </c>
       <c r="C7" s="8" t="s">
-        <v>287</v>
+        <v>477</v>
       </c>
       <c r="D7" s="4" t="s">
-        <v>15</v>
+        <v>10</v>
       </c>
       <c r="E7" s="14"/>
       <c r="F7" s="4" t="s">
@@ -9011,32 +9234,26 @@
         <v>11</v>
       </c>
       <c r="I7" s="5">
-        <v>45381</v>
-      </c>
-      <c r="J7" s="5">
-        <v>45525</v>
-      </c>
+        <v>45570</v>
+      </c>
+      <c r="J7" s="5"/>
       <c r="K7" s="4"/>
     </row>
-    <row r="8" spans="1:11" ht="30" customHeight="1">
+    <row r="8" spans="1:11" ht="20" customHeight="1">
       <c r="A8" s="6">
-        <v>930</v>
+        <v>848</v>
       </c>
       <c r="B8" s="6" t="s">
-        <v>295</v>
+        <v>294</v>
       </c>
       <c r="C8" s="8" t="s">
-        <v>296</v>
+        <v>293</v>
       </c>
       <c r="D8" s="4" t="s">
         <v>10</v>
       </c>
-      <c r="E8" s="14" t="s">
-        <v>297</v>
-      </c>
-      <c r="F8" s="4" t="s">
-        <v>258</v>
-      </c>
+      <c r="E8" s="14"/>
+      <c r="F8" s="4"/>
       <c r="G8" s="4" t="s">
         <v>11</v>
       </c>
@@ -9044,29 +9261,27 @@
         <v>11</v>
       </c>
       <c r="I8" s="5">
-        <v>45524</v>
+        <v>45525</v>
       </c>
       <c r="J8" s="5"/>
       <c r="K8" s="4"/>
     </row>
     <row r="9" spans="1:11" ht="20" customHeight="1">
       <c r="A9" s="6">
-        <v>1124</v>
+        <v>862</v>
       </c>
       <c r="B9" s="6" t="s">
-        <v>374</v>
+        <v>286</v>
       </c>
       <c r="C9" s="8" t="s">
-        <v>375</v>
+        <v>287</v>
       </c>
       <c r="D9" s="4" t="s">
-        <v>10</v>
-      </c>
-      <c r="E9" s="14" t="s">
-        <v>376</v>
-      </c>
+        <v>15</v>
+      </c>
+      <c r="E9" s="14"/>
       <c r="F9" s="4" t="s">
-        <v>324</v>
+        <v>258</v>
       </c>
       <c r="G9" s="4" t="s">
         <v>11</v>
@@ -9075,26 +9290,32 @@
         <v>11</v>
       </c>
       <c r="I9" s="5">
-        <v>45539</v>
-      </c>
-      <c r="J9" s="5"/>
+        <v>45381</v>
+      </c>
+      <c r="J9" s="5">
+        <v>45525</v>
+      </c>
       <c r="K9" s="4"/>
     </row>
-    <row r="10" spans="1:11" ht="20" customHeight="1">
+    <row r="10" spans="1:11" ht="30" customHeight="1">
       <c r="A10" s="6">
-        <v>1423</v>
+        <v>930</v>
       </c>
       <c r="B10" s="6" t="s">
-        <v>473</v>
+        <v>295</v>
       </c>
       <c r="C10" s="8" t="s">
-        <v>474</v>
+        <v>296</v>
       </c>
       <c r="D10" s="4" t="s">
         <v>10</v>
       </c>
-      <c r="E10" s="14"/>
-      <c r="F10" s="4"/>
+      <c r="E10" s="14" t="s">
+        <v>297</v>
+      </c>
+      <c r="F10" s="4" t="s">
+        <v>258</v>
+      </c>
       <c r="G10" s="4" t="s">
         <v>11</v>
       </c>
@@ -9102,78 +9323,78 @@
         <v>11</v>
       </c>
       <c r="I10" s="5">
-        <v>45569</v>
+        <v>45524</v>
       </c>
       <c r="J10" s="5"/>
       <c r="K10" s="4"/>
     </row>
     <row r="11" spans="1:11" ht="20" customHeight="1">
       <c r="A11" s="6">
-        <v>1524</v>
+        <v>1124</v>
       </c>
       <c r="B11" s="6" t="s">
-        <v>299</v>
+        <v>374</v>
       </c>
       <c r="C11" s="8" t="s">
-        <v>298</v>
+        <v>375</v>
       </c>
       <c r="D11" s="4" t="s">
         <v>10</v>
       </c>
-      <c r="E11" s="14"/>
-      <c r="F11" s="4"/>
+      <c r="E11" s="14" t="s">
+        <v>376</v>
+      </c>
+      <c r="F11" s="4" t="s">
+        <v>324</v>
+      </c>
       <c r="G11" s="4" t="s">
         <v>11</v>
       </c>
       <c r="H11" s="4" t="s">
-        <v>28</v>
+        <v>11</v>
       </c>
       <c r="I11" s="5">
-        <v>45524</v>
+        <v>45539</v>
       </c>
       <c r="J11" s="5"/>
       <c r="K11" s="4"/>
     </row>
-    <row r="12" spans="1:11" ht="30" customHeight="1">
+    <row r="12" spans="1:11" ht="20" customHeight="1">
       <c r="A12" s="6">
-        <v>1862</v>
+        <v>1423</v>
       </c>
       <c r="B12" s="6" t="s">
-        <v>275</v>
+        <v>472</v>
       </c>
       <c r="C12" s="8" t="s">
-        <v>274</v>
+        <v>473</v>
       </c>
       <c r="D12" s="4" t="s">
-        <v>15</v>
-      </c>
-      <c r="E12" s="14" t="s">
-        <v>278</v>
-      </c>
-      <c r="F12" s="4" t="s">
-        <v>324</v>
-      </c>
+        <v>10</v>
+      </c>
+      <c r="E12" s="14"/>
+      <c r="F12" s="4"/>
       <c r="G12" s="4" t="s">
-        <v>276</v>
+        <v>11</v>
       </c>
       <c r="H12" s="4" t="s">
-        <v>277</v>
+        <v>11</v>
       </c>
       <c r="I12" s="5">
-        <v>45521</v>
+        <v>45569</v>
       </c>
       <c r="J12" s="5"/>
       <c r="K12" s="4"/>
     </row>
-    <row r="13" spans="1:11" ht="30" customHeight="1">
+    <row r="13" spans="1:11" ht="20" customHeight="1">
       <c r="A13" s="6">
-        <v>1894</v>
+        <v>1524</v>
       </c>
       <c r="B13" s="6" t="s">
-        <v>300</v>
+        <v>299</v>
       </c>
       <c r="C13" s="8" t="s">
-        <v>301</v>
+        <v>298</v>
       </c>
       <c r="D13" s="4" t="s">
         <v>10</v>
@@ -9187,74 +9408,132 @@
         <v>28</v>
       </c>
       <c r="I13" s="5">
-        <v>45525</v>
+        <v>45524</v>
       </c>
       <c r="J13" s="5"/>
       <c r="K13" s="4"/>
     </row>
-    <row r="14" spans="1:11" ht="45" customHeight="1">
+    <row r="14" spans="1:11" ht="30" customHeight="1">
       <c r="A14" s="6">
-        <v>2302</v>
+        <v>1862</v>
       </c>
       <c r="B14" s="6" t="s">
-        <v>283</v>
+        <v>275</v>
       </c>
       <c r="C14" s="8" t="s">
-        <v>284</v>
+        <v>274</v>
       </c>
       <c r="D14" s="4" t="s">
         <v>15</v>
       </c>
       <c r="E14" s="14" t="s">
-        <v>285</v>
-      </c>
-      <c r="F14" s="4"/>
+        <v>278</v>
+      </c>
+      <c r="F14" s="4" t="s">
+        <v>324</v>
+      </c>
       <c r="G14" s="4" t="s">
-        <v>11</v>
+        <v>276</v>
       </c>
       <c r="H14" s="4" t="s">
-        <v>11</v>
+        <v>277</v>
       </c>
       <c r="I14" s="5">
-        <v>45501</v>
-      </c>
-      <c r="J14" s="5">
-        <v>45525</v>
-      </c>
+        <v>45521</v>
+      </c>
+      <c r="J14" s="5"/>
       <c r="K14" s="4"/>
     </row>
-    <row r="15" spans="1:11" ht="20" customHeight="1">
+    <row r="15" spans="1:11" ht="30" customHeight="1">
       <c r="A15" s="6">
-        <v>2438</v>
+        <v>1894</v>
       </c>
       <c r="B15" s="6" t="s">
-        <v>304</v>
+        <v>300</v>
       </c>
       <c r="C15" s="8" t="s">
-        <v>305</v>
+        <v>301</v>
       </c>
       <c r="D15" s="4" t="s">
         <v>10</v>
       </c>
       <c r="E15" s="14"/>
-      <c r="F15" s="4" t="s">
-        <v>306</v>
-      </c>
+      <c r="F15" s="4"/>
       <c r="G15" s="4" t="s">
         <v>11</v>
       </c>
       <c r="H15" s="4" t="s">
-        <v>11</v>
+        <v>28</v>
       </c>
       <c r="I15" s="5">
-        <v>45526</v>
+        <v>45525</v>
       </c>
       <c r="J15" s="5"/>
       <c r="K15" s="4"/>
     </row>
+    <row r="16" spans="1:11" ht="45" customHeight="1">
+      <c r="A16" s="6">
+        <v>2302</v>
+      </c>
+      <c r="B16" s="6" t="s">
+        <v>283</v>
+      </c>
+      <c r="C16" s="8" t="s">
+        <v>284</v>
+      </c>
+      <c r="D16" s="4" t="s">
+        <v>15</v>
+      </c>
+      <c r="E16" s="14" t="s">
+        <v>285</v>
+      </c>
+      <c r="F16" s="4"/>
+      <c r="G16" s="4" t="s">
+        <v>11</v>
+      </c>
+      <c r="H16" s="4" t="s">
+        <v>11</v>
+      </c>
+      <c r="I16" s="5">
+        <v>45501</v>
+      </c>
+      <c r="J16" s="5">
+        <v>45525</v>
+      </c>
+      <c r="K16" s="4"/>
+    </row>
+    <row r="17" spans="1:11" ht="20" customHeight="1">
+      <c r="A17" s="6">
+        <v>2438</v>
+      </c>
+      <c r="B17" s="6" t="s">
+        <v>304</v>
+      </c>
+      <c r="C17" s="8" t="s">
+        <v>305</v>
+      </c>
+      <c r="D17" s="4" t="s">
+        <v>10</v>
+      </c>
+      <c r="E17" s="14"/>
+      <c r="F17" s="4" t="s">
+        <v>306</v>
+      </c>
+      <c r="G17" s="4" t="s">
+        <v>11</v>
+      </c>
+      <c r="H17" s="4" t="s">
+        <v>11</v>
+      </c>
+      <c r="I17" s="5">
+        <v>45526</v>
+      </c>
+      <c r="J17" s="5"/>
+      <c r="K17" s="4"/>
+    </row>
   </sheetData>
   <phoneticPr fontId="1" type="noConversion"/>
-  <conditionalFormatting sqref="D2:D15">
+  <conditionalFormatting sqref="D2:D17">
     <cfRule type="expression" dxfId="29" priority="1">
       <formula>D2="Easy"</formula>
     </cfRule>
@@ -9266,23 +9545,25 @@
     </cfRule>
   </conditionalFormatting>
   <hyperlinks>
-    <hyperlink ref="C12" r:id="rId1" xr:uid="{C9816A24-406A-ED4A-8FB2-059B74B03BB2}"/>
-    <hyperlink ref="C14" r:id="rId2" xr:uid="{28FFE997-242B-BD43-92E3-903DCE08758F}"/>
-    <hyperlink ref="C7" r:id="rId3" xr:uid="{713E12F1-D139-8D4B-A787-71F735A42312}"/>
+    <hyperlink ref="C14" r:id="rId1" xr:uid="{C9816A24-406A-ED4A-8FB2-059B74B03BB2}"/>
+    <hyperlink ref="C16" r:id="rId2" xr:uid="{28FFE997-242B-BD43-92E3-903DCE08758F}"/>
+    <hyperlink ref="C9" r:id="rId3" xr:uid="{713E12F1-D139-8D4B-A787-71F735A42312}"/>
     <hyperlink ref="C3" r:id="rId4" xr:uid="{4696FB6F-B483-AC44-BEE2-62362C4172F1}"/>
-    <hyperlink ref="C4" r:id="rId5" xr:uid="{9012EA63-8820-A141-81DD-5424D597639B}"/>
-    <hyperlink ref="C6" r:id="rId6" xr:uid="{A1E4E21C-AD81-7A4F-9657-2A59703E46FD}"/>
-    <hyperlink ref="C8" r:id="rId7" xr:uid="{1D2D6E50-9921-6340-B74B-D89FEEF6E1D7}"/>
-    <hyperlink ref="C11" r:id="rId8" xr:uid="{5132C615-5239-494D-BC2B-CBB9213F1F81}"/>
-    <hyperlink ref="C13" r:id="rId9" xr:uid="{37463C6E-3673-6B4E-B37B-EDCC87E8E8F6}"/>
+    <hyperlink ref="C5" r:id="rId5" xr:uid="{9012EA63-8820-A141-81DD-5424D597639B}"/>
+    <hyperlink ref="C8" r:id="rId6" xr:uid="{A1E4E21C-AD81-7A4F-9657-2A59703E46FD}"/>
+    <hyperlink ref="C10" r:id="rId7" xr:uid="{1D2D6E50-9921-6340-B74B-D89FEEF6E1D7}"/>
+    <hyperlink ref="C13" r:id="rId8" xr:uid="{5132C615-5239-494D-BC2B-CBB9213F1F81}"/>
+    <hyperlink ref="C15" r:id="rId9" xr:uid="{37463C6E-3673-6B4E-B37B-EDCC87E8E8F6}"/>
     <hyperlink ref="C2" r:id="rId10" xr:uid="{F2C0EEF0-CA41-144C-99D0-D977BE50C774}"/>
-    <hyperlink ref="C15" r:id="rId11" xr:uid="{E65C4F39-2706-6341-ABDD-FBB95C5EAB8F}"/>
-    <hyperlink ref="C9" r:id="rId12" xr:uid="{05FE1C59-7DCD-914E-B21B-0AC59222C12C}"/>
-    <hyperlink ref="C5" r:id="rId13" xr:uid="{080E83A5-4B4C-6F49-8912-BD3CB12E2CCF}"/>
-    <hyperlink ref="C10" r:id="rId14" xr:uid="{78A63C4F-C7A2-D848-989D-EC49CCD8FF5E}"/>
+    <hyperlink ref="C17" r:id="rId11" xr:uid="{E65C4F39-2706-6341-ABDD-FBB95C5EAB8F}"/>
+    <hyperlink ref="C11" r:id="rId12" xr:uid="{05FE1C59-7DCD-914E-B21B-0AC59222C12C}"/>
+    <hyperlink ref="C6" r:id="rId13" xr:uid="{080E83A5-4B4C-6F49-8912-BD3CB12E2CCF}"/>
+    <hyperlink ref="C12" r:id="rId14" xr:uid="{78A63C4F-C7A2-D848-989D-EC49CCD8FF5E}"/>
+    <hyperlink ref="C4" r:id="rId15" xr:uid="{A749378D-FA25-D04B-B30B-F8CA027A3CB9}"/>
+    <hyperlink ref="C7" r:id="rId16" xr:uid="{7954D8C8-FB4B-E344-A66B-452D4F05C5E9}"/>
   </hyperlinks>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
-  <pageSetup paperSize="9" orientation="portrait" verticalDpi="0" r:id="rId15"/>
+  <pageSetup paperSize="9" orientation="portrait" verticalDpi="0" r:id="rId17"/>
   <headerFooter>
     <oddFooter>&amp;L_x000D_&amp;1#&amp;"Calibri"&amp;10&amp;K000000 General</oddFooter>
   </headerFooter>

</xml_diff>

<commit_message>
Improved several problems' efficiency.
</commit_message>
<xml_diff>
--- a/LeetCode Techniques.xlsx
+++ b/LeetCode Techniques.xlsx
@@ -8,9 +8,9 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="/Users/blackjack625/Desktop/LeetCode/"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{779439FF-D28B-2C4C-BEA2-AA398F2D8428}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{A10589E8-C88A-6E46-9D2D-C66CAF9EE515}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="0" yWindow="500" windowWidth="28800" windowHeight="16440" activeTab="5" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
+    <workbookView xWindow="0" yWindow="500" windowWidth="28800" windowHeight="16440" activeTab="9" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
   <sheets>
     <sheet name="DP" sheetId="8" r:id="rId1"/>
@@ -50,7 +50,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="1356" uniqueCount="562">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="1355" uniqueCount="562">
   <si>
     <t>Name</t>
   </si>
@@ -880,11 +880,6 @@
     <phoneticPr fontId="1" type="noConversion"/>
   </si>
   <si>
-    <t>Use 2nd stack for 2nd next greater.
-Binary sort secures 2nd stack order.</t>
-    <phoneticPr fontId="1" type="noConversion"/>
-  </si>
-  <si>
     <t>Dinner Plate Stacks</t>
   </si>
   <si>
@@ -2297,6 +2292,10 @@
   </si>
   <si>
     <t>https://leetcode.com/problems/three-equal-parts/description/</t>
+    <phoneticPr fontId="1" type="noConversion"/>
+  </si>
+  <si>
+    <t>Transporter list ensures monotonicity.</t>
     <phoneticPr fontId="1" type="noConversion"/>
   </si>
 </sst>
@@ -3695,16 +3694,16 @@
         <v>264</v>
       </c>
       <c r="B11" s="4" t="s">
+        <v>496</v>
+      </c>
+      <c r="C11" s="8" t="s">
         <v>497</v>
-      </c>
-      <c r="C11" s="8" t="s">
-        <v>498</v>
       </c>
       <c r="D11" s="4" t="s">
         <v>48</v>
       </c>
       <c r="E11" s="6" t="s">
-        <v>502</v>
+        <v>501</v>
       </c>
       <c r="F11" s="4"/>
       <c r="G11" s="4" t="s">
@@ -3733,7 +3732,7 @@
         <v>48</v>
       </c>
       <c r="E12" s="14" t="s">
-        <v>499</v>
+        <v>498</v>
       </c>
       <c r="F12" s="4"/>
       <c r="G12" s="4" t="s">
@@ -3753,20 +3752,20 @@
         <v>313</v>
       </c>
       <c r="B13" s="4" t="s">
+        <v>499</v>
+      </c>
+      <c r="C13" s="8" t="s">
         <v>500</v>
-      </c>
-      <c r="C13" s="8" t="s">
-        <v>501</v>
       </c>
       <c r="D13" s="4" t="s">
         <v>48</v>
       </c>
       <c r="E13" s="14" t="s">
-        <v>503</v>
+        <v>502</v>
       </c>
       <c r="F13" s="4"/>
       <c r="G13" s="4" t="s">
-        <v>504</v>
+        <v>503</v>
       </c>
       <c r="H13" s="4" t="s">
         <v>11</v>
@@ -3960,16 +3959,16 @@
         <v>918</v>
       </c>
       <c r="B20" s="4" t="s">
+        <v>512</v>
+      </c>
+      <c r="C20" s="8" t="s">
         <v>513</v>
-      </c>
-      <c r="C20" s="8" t="s">
-        <v>514</v>
       </c>
       <c r="D20" s="4" t="s">
         <v>10</v>
       </c>
       <c r="E20" s="14" t="s">
-        <v>515</v>
+        <v>514</v>
       </c>
       <c r="F20" s="4"/>
       <c r="G20" s="4" t="s">
@@ -4016,17 +4015,17 @@
         <v>975</v>
       </c>
       <c r="B22" s="4" t="s">
+        <v>525</v>
+      </c>
+      <c r="C22" s="8" t="s">
         <v>526</v>
-      </c>
-      <c r="C22" s="8" t="s">
-        <v>527</v>
       </c>
       <c r="D22" s="4" t="s">
         <v>15</v>
       </c>
       <c r="E22" s="2"/>
       <c r="F22" s="4" t="s">
-        <v>264</v>
+        <v>263</v>
       </c>
       <c r="G22" s="4" t="s">
         <v>12</v>
@@ -4188,19 +4187,19 @@
         <v>1425</v>
       </c>
       <c r="B28" s="4" t="s">
+        <v>252</v>
+      </c>
+      <c r="C28" s="8" t="s">
         <v>253</v>
-      </c>
-      <c r="C28" s="8" t="s">
-        <v>254</v>
       </c>
       <c r="D28" s="4" t="s">
         <v>15</v>
       </c>
       <c r="E28" s="14" t="s">
-        <v>256</v>
+        <v>255</v>
       </c>
       <c r="F28" s="4" t="s">
-        <v>255</v>
+        <v>254</v>
       </c>
       <c r="G28" s="4" t="s">
         <v>11</v>
@@ -4248,17 +4247,17 @@
         <v>3041</v>
       </c>
       <c r="B30" s="4" t="s">
+        <v>535</v>
+      </c>
+      <c r="C30" s="8" t="s">
         <v>536</v>
-      </c>
-      <c r="C30" s="8" t="s">
-        <v>537</v>
       </c>
       <c r="D30" s="4" t="s">
         <v>15</v>
       </c>
       <c r="E30" s="13"/>
       <c r="F30" s="4" t="s">
-        <v>413</v>
+        <v>412</v>
       </c>
       <c r="G30" s="4" t="s">
         <v>12</v>
@@ -4327,7 +4326,7 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{9BC7A267-6069-4E38-AC2F-0C28241496B0}">
   <dimension ref="A1:K9"/>
   <sheetViews>
-    <sheetView zoomScaleNormal="100" workbookViewId="0"/>
+    <sheetView tabSelected="1" zoomScaleNormal="100" workbookViewId="0"/>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultColWidth="9" defaultRowHeight="16"/>
   <cols>
@@ -4382,16 +4381,16 @@
         <v>42</v>
       </c>
       <c r="B2" s="6" t="s">
+        <v>551</v>
+      </c>
+      <c r="C2" s="8" t="s">
         <v>552</v>
-      </c>
-      <c r="C2" s="8" t="s">
-        <v>553</v>
       </c>
       <c r="D2" s="4" t="s">
         <v>15</v>
       </c>
       <c r="E2" s="14" t="s">
-        <v>554</v>
+        <v>553</v>
       </c>
       <c r="F2" s="4"/>
       <c r="G2" s="4" t="s">
@@ -4411,16 +4410,16 @@
         <v>84</v>
       </c>
       <c r="B3" s="6" t="s">
+        <v>545</v>
+      </c>
+      <c r="C3" s="8" t="s">
         <v>546</v>
-      </c>
-      <c r="C3" s="8" t="s">
-        <v>547</v>
       </c>
       <c r="D3" s="4" t="s">
         <v>15</v>
       </c>
       <c r="E3" s="14" t="s">
-        <v>548</v>
+        <v>547</v>
       </c>
       <c r="F3" s="4"/>
       <c r="G3" s="4" t="s">
@@ -4440,17 +4439,17 @@
         <v>895</v>
       </c>
       <c r="B4" s="6" t="s">
+        <v>219</v>
+      </c>
+      <c r="C4" s="8" t="s">
         <v>220</v>
-      </c>
-      <c r="C4" s="8" t="s">
-        <v>221</v>
       </c>
       <c r="D4" s="4" t="s">
         <v>15</v>
       </c>
       <c r="E4" s="14"/>
       <c r="F4" s="4" t="s">
-        <v>222</v>
+        <v>221</v>
       </c>
       <c r="G4" s="4" t="s">
         <v>28</v>
@@ -4469,16 +4468,16 @@
         <v>1172</v>
       </c>
       <c r="B5" s="6" t="s">
+        <v>213</v>
+      </c>
+      <c r="C5" s="8" t="s">
         <v>214</v>
-      </c>
-      <c r="C5" s="8" t="s">
-        <v>215</v>
       </c>
       <c r="D5" s="4" t="s">
         <v>15</v>
       </c>
       <c r="E5" s="14" t="s">
-        <v>216</v>
+        <v>215</v>
       </c>
       <c r="F5" s="4"/>
       <c r="G5" s="4" t="s">
@@ -4498,17 +4497,17 @@
         <v>1856</v>
       </c>
       <c r="B6" s="6" t="s">
+        <v>516</v>
+      </c>
+      <c r="C6" s="8" t="s">
         <v>517</v>
-      </c>
-      <c r="C6" s="8" t="s">
-        <v>518</v>
       </c>
       <c r="D6" s="4" t="s">
         <v>10</v>
       </c>
       <c r="E6" s="14"/>
       <c r="F6" s="4" t="s">
-        <v>380</v>
+        <v>379</v>
       </c>
       <c r="G6" s="4" t="s">
         <v>11</v>
@@ -4527,16 +4526,16 @@
         <v>1944</v>
       </c>
       <c r="B7" s="6" t="s">
+        <v>523</v>
+      </c>
+      <c r="C7" s="8" t="s">
         <v>524</v>
-      </c>
-      <c r="C7" s="8" t="s">
-        <v>525</v>
       </c>
       <c r="D7" s="4" t="s">
         <v>15</v>
       </c>
       <c r="E7" s="14" t="s">
-        <v>555</v>
+        <v>554</v>
       </c>
       <c r="F7" s="4"/>
       <c r="G7" s="4" t="s">
@@ -4556,16 +4555,16 @@
         <v>2334</v>
       </c>
       <c r="B8" s="6" t="s">
+        <v>549</v>
+      </c>
+      <c r="C8" s="8" t="s">
         <v>550</v>
-      </c>
-      <c r="C8" s="8" t="s">
-        <v>551</v>
       </c>
       <c r="D8" s="4" t="s">
         <v>15</v>
       </c>
       <c r="E8" s="14" t="s">
-        <v>548</v>
+        <v>547</v>
       </c>
       <c r="F8" s="4"/>
       <c r="G8" s="4" t="s">
@@ -4580,7 +4579,7 @@
       <c r="J8" s="5"/>
       <c r="K8" s="4"/>
     </row>
-    <row r="9" spans="1:11" ht="30" customHeight="1">
+    <row r="9" spans="1:11" ht="20" customHeight="1">
       <c r="A9" s="6">
         <v>2454</v>
       </c>
@@ -4594,13 +4593,11 @@
         <v>15</v>
       </c>
       <c r="E9" s="14" t="s">
-        <v>213</v>
-      </c>
-      <c r="F9" s="4" t="s">
-        <v>151</v>
-      </c>
+        <v>561</v>
+      </c>
+      <c r="F9" s="4"/>
       <c r="G9" s="4" t="s">
-        <v>12</v>
+        <v>11</v>
       </c>
       <c r="H9" s="4" t="s">
         <v>43</v>
@@ -4608,7 +4605,9 @@
       <c r="I9" s="5">
         <v>45505</v>
       </c>
-      <c r="J9" s="5"/>
+      <c r="J9" s="5">
+        <v>45599</v>
+      </c>
       <c r="K9" s="4"/>
     </row>
   </sheetData>
@@ -4700,10 +4699,10 @@
         <v>239</v>
       </c>
       <c r="B2" s="6" t="s">
+        <v>249</v>
+      </c>
+      <c r="C2" s="8" t="s">
         <v>250</v>
-      </c>
-      <c r="C2" s="8" t="s">
-        <v>251</v>
       </c>
       <c r="D2" s="4" t="s">
         <v>15</v>
@@ -4714,7 +4713,7 @@
         <v>43</v>
       </c>
       <c r="H2" s="4" t="s">
-        <v>252</v>
+        <v>251</v>
       </c>
       <c r="I2" s="5">
         <v>45386</v>
@@ -4729,23 +4728,23 @@
         <v>1352</v>
       </c>
       <c r="B3" s="6" t="s">
+        <v>393</v>
+      </c>
+      <c r="C3" s="8" t="s">
         <v>394</v>
-      </c>
-      <c r="C3" s="8" t="s">
-        <v>395</v>
       </c>
       <c r="D3" s="4" t="s">
         <v>10</v>
       </c>
       <c r="E3" s="14"/>
       <c r="F3" s="4" t="s">
-        <v>456</v>
+        <v>455</v>
       </c>
       <c r="G3" s="4" t="s">
-        <v>393</v>
+        <v>392</v>
       </c>
       <c r="H3" s="4" t="s">
-        <v>369</v>
+        <v>368</v>
       </c>
       <c r="I3" s="5">
         <v>45387</v>
@@ -4760,10 +4759,10 @@
         <v>1438</v>
       </c>
       <c r="B4" s="6" t="s">
+        <v>247</v>
+      </c>
+      <c r="C4" s="8" t="s">
         <v>248</v>
-      </c>
-      <c r="C4" s="8" t="s">
-        <v>249</v>
       </c>
       <c r="D4" s="4" t="s">
         <v>10</v>
@@ -4789,10 +4788,10 @@
         <v>2526</v>
       </c>
       <c r="B5" s="6" t="s">
+        <v>390</v>
+      </c>
+      <c r="C5" s="8" t="s">
         <v>391</v>
-      </c>
-      <c r="C5" s="8" t="s">
-        <v>392</v>
       </c>
       <c r="D5" s="4" t="s">
         <v>10</v>
@@ -4800,10 +4799,10 @@
       <c r="E5" s="14"/>
       <c r="F5" s="4"/>
       <c r="G5" s="4" t="s">
-        <v>393</v>
+        <v>392</v>
       </c>
       <c r="H5" s="4" t="s">
-        <v>393</v>
+        <v>392</v>
       </c>
       <c r="I5" s="5">
         <v>45387</v>
@@ -4897,16 +4896,16 @@
         <v>295</v>
       </c>
       <c r="B2" s="4" t="s">
+        <v>241</v>
+      </c>
+      <c r="C2" s="8" t="s">
         <v>242</v>
-      </c>
-      <c r="C2" s="8" t="s">
-        <v>243</v>
       </c>
       <c r="D2" s="4" t="s">
         <v>15</v>
       </c>
       <c r="E2" s="4" t="s">
-        <v>317</v>
+        <v>316</v>
       </c>
       <c r="F2" s="2"/>
       <c r="G2" s="4" t="s">
@@ -4928,10 +4927,10 @@
         <v>355</v>
       </c>
       <c r="B3" s="6" t="s">
+        <v>314</v>
+      </c>
+      <c r="C3" s="8" t="s">
         <v>315</v>
-      </c>
-      <c r="C3" s="8" t="s">
-        <v>316</v>
       </c>
       <c r="D3" s="4" t="s">
         <v>10</v>
@@ -4939,10 +4938,10 @@
       <c r="E3" s="6"/>
       <c r="F3" s="4"/>
       <c r="G3" s="4" t="s">
+        <v>311</v>
+      </c>
+      <c r="H3" s="4" t="s">
         <v>312</v>
-      </c>
-      <c r="H3" s="4" t="s">
-        <v>313</v>
       </c>
       <c r="I3" s="5">
         <v>45528</v>
@@ -4955,16 +4954,16 @@
         <v>1354</v>
       </c>
       <c r="B4" s="6" t="s">
+        <v>463</v>
+      </c>
+      <c r="C4" s="8" t="s">
         <v>464</v>
-      </c>
-      <c r="C4" s="8" t="s">
-        <v>465</v>
       </c>
       <c r="D4" s="4" t="s">
         <v>15</v>
       </c>
       <c r="E4" s="14" t="s">
-        <v>466</v>
+        <v>465</v>
       </c>
       <c r="F4" s="4"/>
       <c r="G4" s="4" t="s">
@@ -4984,17 +4983,17 @@
         <v>1606</v>
       </c>
       <c r="B5" s="6" t="s">
+        <v>479</v>
+      </c>
+      <c r="C5" s="8" t="s">
         <v>480</v>
-      </c>
-      <c r="C5" s="8" t="s">
-        <v>481</v>
       </c>
       <c r="D5" s="4" t="s">
         <v>15</v>
       </c>
       <c r="E5" s="14"/>
       <c r="F5" s="4" t="s">
-        <v>482</v>
+        <v>481</v>
       </c>
       <c r="G5" s="4" t="s">
         <v>12</v>
@@ -5013,10 +5012,10 @@
         <v>1845</v>
       </c>
       <c r="B6" s="6" t="s">
+        <v>466</v>
+      </c>
+      <c r="C6" s="8" t="s">
         <v>467</v>
-      </c>
-      <c r="C6" s="8" t="s">
-        <v>468</v>
       </c>
       <c r="D6" s="4" t="s">
         <v>10</v>
@@ -5122,20 +5121,20 @@
         <v>31</v>
       </c>
       <c r="B2" s="4" t="s">
+        <v>366</v>
+      </c>
+      <c r="C2" s="8" t="s">
         <v>367</v>
-      </c>
-      <c r="C2" s="8" t="s">
-        <v>368</v>
       </c>
       <c r="D2" s="4" t="s">
         <v>10</v>
       </c>
       <c r="E2" s="14" t="s">
-        <v>370</v>
+        <v>369</v>
       </c>
       <c r="F2" s="4"/>
       <c r="G2" s="4" t="s">
-        <v>369</v>
+        <v>368</v>
       </c>
       <c r="H2" s="4" t="s">
         <v>44</v>
@@ -5151,20 +5150,20 @@
         <v>658</v>
       </c>
       <c r="B3" s="4" t="s">
-        <v>318</v>
+        <v>317</v>
       </c>
       <c r="C3" s="8" t="s">
-        <v>320</v>
+        <v>319</v>
       </c>
       <c r="D3" s="4" t="s">
         <v>10</v>
       </c>
       <c r="E3" s="14"/>
       <c r="F3" s="4" t="s">
-        <v>307</v>
+        <v>306</v>
       </c>
       <c r="G3" s="4" t="s">
-        <v>319</v>
+        <v>318</v>
       </c>
       <c r="H3" s="4" t="s">
         <v>44</v>
@@ -5180,16 +5179,16 @@
         <v>1163</v>
       </c>
       <c r="B4" s="4" t="s">
+        <v>337</v>
+      </c>
+      <c r="C4" s="8" t="s">
         <v>338</v>
-      </c>
-      <c r="C4" s="8" t="s">
-        <v>339</v>
       </c>
       <c r="D4" s="4" t="s">
         <v>15</v>
       </c>
       <c r="E4" s="14" t="s">
-        <v>340</v>
+        <v>339</v>
       </c>
       <c r="F4" s="4"/>
       <c r="G4" s="4" t="s">
@@ -5209,16 +5208,16 @@
         <v>1793</v>
       </c>
       <c r="B5" s="4" t="s">
+        <v>243</v>
+      </c>
+      <c r="C5" s="8" t="s">
         <v>244</v>
-      </c>
-      <c r="C5" s="8" t="s">
-        <v>245</v>
       </c>
       <c r="D5" s="4" t="s">
         <v>15</v>
       </c>
       <c r="E5" s="14" t="s">
-        <v>549</v>
+        <v>548</v>
       </c>
       <c r="F5" s="4"/>
       <c r="G5" s="4" t="s">
@@ -5662,10 +5661,10 @@
         <v>60</v>
       </c>
       <c r="B2" s="4" t="s">
+        <v>256</v>
+      </c>
+      <c r="C2" s="8" t="s">
         <v>257</v>
-      </c>
-      <c r="C2" s="8" t="s">
-        <v>258</v>
       </c>
       <c r="D2" s="4" t="s">
         <v>15</v>
@@ -5716,7 +5715,7 @@
         <v>779</v>
       </c>
       <c r="B4" s="4" t="s">
-        <v>341</v>
+        <v>340</v>
       </c>
       <c r="C4" s="8" t="s">
         <v>59</v>
@@ -5725,7 +5724,7 @@
         <v>48</v>
       </c>
       <c r="E4" s="14" t="s">
-        <v>342</v>
+        <v>341</v>
       </c>
       <c r="F4" s="4"/>
       <c r="G4" s="4" t="s">
@@ -5825,17 +5824,17 @@
         <v>187</v>
       </c>
       <c r="B2" s="6" t="s">
+        <v>267</v>
+      </c>
+      <c r="C2" s="8" t="s">
         <v>268</v>
-      </c>
-      <c r="C2" s="8" t="s">
-        <v>269</v>
       </c>
       <c r="D2" s="4" t="s">
         <v>10</v>
       </c>
       <c r="E2" s="14"/>
       <c r="F2" s="4" t="s">
-        <v>321</v>
+        <v>320</v>
       </c>
       <c r="G2" s="4" t="s">
         <v>11</v>
@@ -5856,16 +5855,16 @@
         <v>2444</v>
       </c>
       <c r="B3" s="6" t="s">
+        <v>264</v>
+      </c>
+      <c r="C3" s="8" t="s">
         <v>265</v>
-      </c>
-      <c r="C3" s="8" t="s">
-        <v>266</v>
       </c>
       <c r="D3" s="4" t="s">
         <v>15</v>
       </c>
       <c r="E3" s="14" t="s">
-        <v>267</v>
+        <v>266</v>
       </c>
       <c r="F3" s="4"/>
       <c r="G3" s="4" t="s">
@@ -5885,17 +5884,17 @@
         <v>3134</v>
       </c>
       <c r="B4" s="6" t="s">
+        <v>532</v>
+      </c>
+      <c r="C4" s="8" t="s">
         <v>533</v>
-      </c>
-      <c r="C4" s="8" t="s">
-        <v>534</v>
       </c>
       <c r="D4" s="4" t="s">
         <v>15</v>
       </c>
       <c r="E4" s="14"/>
       <c r="F4" s="4" t="s">
-        <v>535</v>
+        <v>534</v>
       </c>
       <c r="G4" s="4" t="s">
         <v>12</v>
@@ -6002,7 +6001,7 @@
       </c>
       <c r="E2" s="4"/>
       <c r="F2" s="4" t="s">
-        <v>321</v>
+        <v>320</v>
       </c>
       <c r="G2" s="4" t="s">
         <v>43</v>
@@ -6167,10 +6166,10 @@
         <v>22</v>
       </c>
       <c r="B2" s="4" t="s">
+        <v>518</v>
+      </c>
+      <c r="C2" s="8" t="s">
         <v>519</v>
-      </c>
-      <c r="C2" s="8" t="s">
-        <v>520</v>
       </c>
       <c r="D2" s="4" t="s">
         <v>10</v>
@@ -6178,10 +6177,10 @@
       <c r="E2" s="4"/>
       <c r="F2" s="4"/>
       <c r="G2" s="4" t="s">
-        <v>523</v>
+        <v>522</v>
       </c>
       <c r="H2" s="4" t="s">
-        <v>523</v>
+        <v>522</v>
       </c>
       <c r="I2" s="5">
         <v>45419</v>
@@ -6194,10 +6193,10 @@
         <v>46</v>
       </c>
       <c r="B3" s="4" t="s">
+        <v>520</v>
+      </c>
+      <c r="C3" s="8" t="s">
         <v>521</v>
-      </c>
-      <c r="C3" s="8" t="s">
-        <v>522</v>
       </c>
       <c r="D3" s="4" t="s">
         <v>48</v>
@@ -6205,10 +6204,10 @@
       <c r="E3" s="4"/>
       <c r="F3" s="4"/>
       <c r="G3" s="4" t="s">
-        <v>523</v>
+        <v>522</v>
       </c>
       <c r="H3" s="4" t="s">
-        <v>523</v>
+        <v>522</v>
       </c>
       <c r="I3" s="5">
         <v>45582</v>
@@ -6311,19 +6310,19 @@
         <v>33</v>
       </c>
       <c r="B2" s="4" t="s">
+        <v>353</v>
+      </c>
+      <c r="C2" s="8" t="s">
         <v>354</v>
-      </c>
-      <c r="C2" s="8" t="s">
-        <v>355</v>
       </c>
       <c r="D2" s="4" t="s">
         <v>10</v>
       </c>
       <c r="E2" s="4" t="s">
-        <v>358</v>
+        <v>357</v>
       </c>
       <c r="F2" s="4" t="s">
-        <v>361</v>
+        <v>360</v>
       </c>
       <c r="G2" s="4" t="s">
         <v>13</v>
@@ -6344,10 +6343,10 @@
         <v>34</v>
       </c>
       <c r="B3" s="4" t="s">
+        <v>355</v>
+      </c>
+      <c r="C3" s="8" t="s">
         <v>356</v>
-      </c>
-      <c r="C3" s="8" t="s">
-        <v>357</v>
       </c>
       <c r="D3" s="4" t="s">
         <v>10</v>
@@ -6402,17 +6401,17 @@
         <v>81</v>
       </c>
       <c r="B5" s="4" t="s">
+        <v>358</v>
+      </c>
+      <c r="C5" s="8" t="s">
         <v>359</v>
-      </c>
-      <c r="C5" s="8" t="s">
-        <v>360</v>
       </c>
       <c r="D5" s="4" t="s">
         <v>10</v>
       </c>
       <c r="E5" s="4"/>
       <c r="F5" s="4" t="s">
-        <v>361</v>
+        <v>360</v>
       </c>
       <c r="G5" s="4" t="s">
         <v>13</v>
@@ -6469,7 +6468,7 @@
         <v>10</v>
       </c>
       <c r="E7" s="14" t="s">
-        <v>352</v>
+        <v>351</v>
       </c>
       <c r="F7" s="4"/>
       <c r="G7" s="4" t="s">
@@ -6549,19 +6548,19 @@
         <v>400</v>
       </c>
       <c r="B10" s="4" t="s">
+        <v>361</v>
+      </c>
+      <c r="C10" s="8" t="s">
         <v>362</v>
-      </c>
-      <c r="C10" s="8" t="s">
-        <v>363</v>
       </c>
       <c r="D10" s="4" t="s">
         <v>10</v>
       </c>
       <c r="E10" s="2" t="s">
-        <v>364</v>
+        <v>363</v>
       </c>
       <c r="F10" s="4" t="s">
-        <v>321</v>
+        <v>320</v>
       </c>
       <c r="G10" s="4" t="s">
         <v>13</v>
@@ -6649,7 +6648,7 @@
         <v>14</v>
       </c>
       <c r="G13" s="4" t="s">
-        <v>353</v>
+        <v>352</v>
       </c>
       <c r="H13" s="4" t="s">
         <v>11</v>
@@ -6665,16 +6664,16 @@
         <v>646</v>
       </c>
       <c r="B14" s="4" t="s">
+        <v>434</v>
+      </c>
+      <c r="C14" s="8" t="s">
         <v>435</v>
-      </c>
-      <c r="C14" s="8" t="s">
-        <v>436</v>
       </c>
       <c r="D14" s="4" t="s">
         <v>10</v>
       </c>
       <c r="E14" s="2" t="s">
-        <v>434</v>
+        <v>433</v>
       </c>
       <c r="F14" s="4"/>
       <c r="G14" s="4" t="s">
@@ -6694,10 +6693,10 @@
         <v>668</v>
       </c>
       <c r="B15" s="4" t="s">
+        <v>276</v>
+      </c>
+      <c r="C15" s="8" t="s">
         <v>277</v>
-      </c>
-      <c r="C15" s="8" t="s">
-        <v>278</v>
       </c>
       <c r="D15" s="4" t="s">
         <v>57</v>
@@ -6705,7 +6704,7 @@
       <c r="E15" s="4"/>
       <c r="F15" s="4"/>
       <c r="G15" s="4" t="s">
-        <v>279</v>
+        <v>278</v>
       </c>
       <c r="H15" s="4" t="s">
         <v>28</v>
@@ -6787,7 +6786,7 @@
         <v>82</v>
       </c>
       <c r="F18" s="4" t="s">
-        <v>321</v>
+        <v>320</v>
       </c>
       <c r="G18" s="4" t="s">
         <v>12</v>
@@ -6808,19 +6807,19 @@
         <v>1671</v>
       </c>
       <c r="B19" s="4" t="s">
+        <v>527</v>
+      </c>
+      <c r="C19" s="8" t="s">
         <v>528</v>
-      </c>
-      <c r="C19" s="8" t="s">
-        <v>529</v>
       </c>
       <c r="D19" s="4" t="s">
         <v>57</v>
       </c>
       <c r="E19" s="14" t="s">
-        <v>530</v>
+        <v>529</v>
       </c>
       <c r="F19" s="4" t="s">
-        <v>321</v>
+        <v>320</v>
       </c>
       <c r="G19" s="4" t="s">
         <v>12</v>
@@ -7057,10 +7056,10 @@
         <v>80</v>
       </c>
       <c r="B3" s="4" t="s">
+        <v>229</v>
+      </c>
+      <c r="C3" s="8" t="s">
         <v>230</v>
-      </c>
-      <c r="C3" s="8" t="s">
-        <v>231</v>
       </c>
       <c r="D3" s="4" t="s">
         <v>10</v>
@@ -7084,10 +7083,10 @@
         <v>347</v>
       </c>
       <c r="B4" s="4" t="s">
+        <v>233</v>
+      </c>
+      <c r="C4" s="8" t="s">
         <v>234</v>
-      </c>
-      <c r="C4" s="8" t="s">
-        <v>235</v>
       </c>
       <c r="D4" s="4" t="s">
         <v>10</v>
@@ -7111,16 +7110,16 @@
         <v>381</v>
       </c>
       <c r="B5" s="4" t="s">
+        <v>216</v>
+      </c>
+      <c r="C5" s="8" t="s">
         <v>217</v>
-      </c>
-      <c r="C5" s="8" t="s">
-        <v>218</v>
       </c>
       <c r="D5" s="4" t="s">
         <v>15</v>
       </c>
       <c r="E5" s="14" t="s">
-        <v>219</v>
+        <v>218</v>
       </c>
       <c r="F5" s="4"/>
       <c r="G5" s="4" t="s">
@@ -7140,10 +7139,10 @@
         <v>432</v>
       </c>
       <c r="B6" s="4" t="s">
+        <v>227</v>
+      </c>
+      <c r="C6" s="8" t="s">
         <v>228</v>
-      </c>
-      <c r="C6" s="8" t="s">
-        <v>229</v>
       </c>
       <c r="D6" s="4" t="s">
         <v>15</v>
@@ -7167,10 +7166,10 @@
         <v>460</v>
       </c>
       <c r="B7" s="4" t="s">
+        <v>225</v>
+      </c>
+      <c r="C7" s="8" t="s">
         <v>226</v>
-      </c>
-      <c r="C7" s="8" t="s">
-        <v>227</v>
       </c>
       <c r="D7" s="4" t="s">
         <v>15</v>
@@ -7194,19 +7193,19 @@
         <v>659</v>
       </c>
       <c r="B8" s="4" t="s">
+        <v>510</v>
+      </c>
+      <c r="C8" s="8" t="s">
         <v>511</v>
-      </c>
-      <c r="C8" s="8" t="s">
-        <v>512</v>
       </c>
       <c r="D8" s="4" t="s">
         <v>10</v>
       </c>
       <c r="E8" s="14" t="s">
-        <v>516</v>
+        <v>515</v>
       </c>
       <c r="F8" s="4" t="s">
-        <v>477</v>
+        <v>476</v>
       </c>
       <c r="G8" s="4" t="s">
         <v>11</v>
@@ -7225,10 +7224,10 @@
         <v>692</v>
       </c>
       <c r="B9" s="4" t="s">
+        <v>239</v>
+      </c>
+      <c r="C9" s="8" t="s">
         <v>240</v>
-      </c>
-      <c r="C9" s="8" t="s">
-        <v>241</v>
       </c>
       <c r="D9" s="4" t="s">
         <v>10</v>
@@ -7252,16 +7251,16 @@
         <v>710</v>
       </c>
       <c r="B10" s="4" t="s">
+        <v>258</v>
+      </c>
+      <c r="C10" s="8" t="s">
         <v>259</v>
-      </c>
-      <c r="C10" s="8" t="s">
-        <v>260</v>
       </c>
       <c r="D10" s="4" t="s">
         <v>15</v>
       </c>
       <c r="E10" s="14" t="s">
-        <v>261</v>
+        <v>260</v>
       </c>
       <c r="F10" s="4"/>
       <c r="G10" s="4" t="s">
@@ -7281,17 +7280,17 @@
         <v>718</v>
       </c>
       <c r="B11" s="4" t="s">
-        <v>366</v>
+        <v>365</v>
       </c>
       <c r="C11" s="8" t="s">
-        <v>365</v>
+        <v>364</v>
       </c>
       <c r="D11" s="4" t="s">
         <v>10</v>
       </c>
       <c r="E11" s="14"/>
       <c r="F11" s="4" t="s">
-        <v>264</v>
+        <v>263</v>
       </c>
       <c r="G11" s="4" t="s">
         <v>12</v>
@@ -7310,19 +7309,19 @@
         <v>1044</v>
       </c>
       <c r="B12" s="4" t="s">
+        <v>261</v>
+      </c>
+      <c r="C12" s="8" t="s">
         <v>262</v>
-      </c>
-      <c r="C12" s="8" t="s">
-        <v>263</v>
       </c>
       <c r="D12" s="4" t="s">
         <v>15</v>
       </c>
       <c r="E12" s="14" t="s">
-        <v>270</v>
+        <v>269</v>
       </c>
       <c r="F12" s="4" t="s">
-        <v>264</v>
+        <v>263</v>
       </c>
       <c r="G12" s="4" t="s">
         <v>12</v>
@@ -7341,10 +7340,10 @@
         <v>1206</v>
       </c>
       <c r="B13" s="4" t="s">
+        <v>222</v>
+      </c>
+      <c r="C13" s="8" t="s">
         <v>223</v>
-      </c>
-      <c r="C13" s="8" t="s">
-        <v>224</v>
       </c>
       <c r="D13" s="4" t="s">
         <v>15</v>
@@ -7368,10 +7367,10 @@
         <v>1224</v>
       </c>
       <c r="B14" s="4" t="s">
+        <v>245</v>
+      </c>
+      <c r="C14" s="8" t="s">
         <v>246</v>
-      </c>
-      <c r="C14" s="8" t="s">
-        <v>247</v>
       </c>
       <c r="D14" s="4" t="s">
         <v>15</v>
@@ -7395,10 +7394,10 @@
         <v>1338</v>
       </c>
       <c r="B15" s="4" t="s">
+        <v>231</v>
+      </c>
+      <c r="C15" s="8" t="s">
         <v>232</v>
-      </c>
-      <c r="C15" s="8" t="s">
-        <v>233</v>
       </c>
       <c r="D15" s="4" t="s">
         <v>10</v>
@@ -7453,10 +7452,10 @@
         <v>2262</v>
       </c>
       <c r="B17" s="4" t="s">
+        <v>530</v>
+      </c>
+      <c r="C17" s="8" t="s">
         <v>531</v>
-      </c>
-      <c r="C17" s="8" t="s">
-        <v>532</v>
       </c>
       <c r="D17" s="4" t="s">
         <v>15</v>
@@ -7480,10 +7479,10 @@
         <v>2342</v>
       </c>
       <c r="B18" s="4" t="s">
+        <v>404</v>
+      </c>
+      <c r="C18" s="8" t="s">
         <v>405</v>
-      </c>
-      <c r="C18" s="8" t="s">
-        <v>406</v>
       </c>
       <c r="D18" s="4" t="s">
         <v>10</v>
@@ -7507,10 +7506,10 @@
         <v>2453</v>
       </c>
       <c r="B19" s="4" t="s">
+        <v>237</v>
+      </c>
+      <c r="C19" s="8" t="s">
         <v>238</v>
-      </c>
-      <c r="C19" s="8" t="s">
-        <v>239</v>
       </c>
       <c r="D19" s="4" t="s">
         <v>10</v>
@@ -7534,10 +7533,10 @@
         <v>3039</v>
       </c>
       <c r="B20" s="4" t="s">
+        <v>235</v>
+      </c>
+      <c r="C20" s="8" t="s">
         <v>236</v>
-      </c>
-      <c r="C20" s="8" t="s">
-        <v>237</v>
       </c>
       <c r="D20" s="4" t="s">
         <v>10</v>
@@ -7658,19 +7657,19 @@
         <v>56</v>
       </c>
       <c r="B2" s="4" t="s">
+        <v>417</v>
+      </c>
+      <c r="C2" s="8" t="s">
         <v>418</v>
-      </c>
-      <c r="C2" s="8" t="s">
-        <v>419</v>
       </c>
       <c r="D2" s="4" t="s">
         <v>10</v>
       </c>
       <c r="E2" s="4" t="s">
-        <v>420</v>
+        <v>419</v>
       </c>
       <c r="F2" s="4" t="s">
-        <v>361</v>
+        <v>360</v>
       </c>
       <c r="G2" s="4" t="s">
         <v>12</v>
@@ -7689,19 +7688,19 @@
         <v>179</v>
       </c>
       <c r="B3" s="4" t="s">
+        <v>414</v>
+      </c>
+      <c r="C3" s="8" t="s">
         <v>415</v>
-      </c>
-      <c r="C3" s="8" t="s">
-        <v>416</v>
       </c>
       <c r="D3" s="4" t="s">
         <v>10</v>
       </c>
       <c r="E3" s="4" t="s">
-        <v>417</v>
+        <v>416</v>
       </c>
       <c r="F3" s="4" t="s">
-        <v>361</v>
+        <v>360</v>
       </c>
       <c r="G3" s="4" t="s">
         <v>12</v>
@@ -7720,10 +7719,10 @@
         <v>324</v>
       </c>
       <c r="B4" s="4" t="s">
+        <v>425</v>
+      </c>
+      <c r="C4" s="8" t="s">
         <v>426</v>
-      </c>
-      <c r="C4" s="8" t="s">
-        <v>427</v>
       </c>
       <c r="D4" s="4" t="s">
         <v>10</v>
@@ -7747,19 +7746,19 @@
         <v>757</v>
       </c>
       <c r="B5" s="4" t="s">
+        <v>485</v>
+      </c>
+      <c r="C5" s="8" t="s">
         <v>486</v>
-      </c>
-      <c r="C5" s="8" t="s">
-        <v>487</v>
       </c>
       <c r="D5" s="4" t="s">
         <v>15</v>
       </c>
       <c r="E5" s="14" t="s">
-        <v>488</v>
+        <v>487</v>
       </c>
       <c r="F5" s="4" t="s">
-        <v>482</v>
+        <v>481</v>
       </c>
       <c r="G5" s="4" t="s">
         <v>12</v>
@@ -7778,10 +7777,10 @@
         <v>891</v>
       </c>
       <c r="B6" s="4" t="s">
+        <v>490</v>
+      </c>
+      <c r="C6" s="8" t="s">
         <v>491</v>
-      </c>
-      <c r="C6" s="8" t="s">
-        <v>492</v>
       </c>
       <c r="D6" s="4" t="s">
         <v>15</v>
@@ -7805,10 +7804,10 @@
         <v>1386</v>
       </c>
       <c r="B7" s="4" t="s">
+        <v>420</v>
+      </c>
+      <c r="C7" s="8" t="s">
         <v>421</v>
-      </c>
-      <c r="C7" s="8" t="s">
-        <v>422</v>
       </c>
       <c r="D7" s="4" t="s">
         <v>10</v>
@@ -7832,17 +7831,17 @@
         <v>2402</v>
       </c>
       <c r="B8" s="6" t="s">
-        <v>484</v>
+        <v>483</v>
       </c>
       <c r="C8" s="8" t="s">
-        <v>483</v>
+        <v>482</v>
       </c>
       <c r="D8" s="4" t="s">
         <v>15</v>
       </c>
       <c r="E8" s="14"/>
       <c r="F8" s="4" t="s">
-        <v>485</v>
+        <v>484</v>
       </c>
       <c r="G8" s="4" t="s">
         <v>12</v>
@@ -7861,17 +7860,17 @@
         <v>2659</v>
       </c>
       <c r="B9" s="4" t="s">
+        <v>474</v>
+      </c>
+      <c r="C9" s="8" t="s">
         <v>475</v>
-      </c>
-      <c r="C9" s="8" t="s">
-        <v>476</v>
       </c>
       <c r="D9" s="4" t="s">
         <v>15</v>
       </c>
       <c r="E9" s="6"/>
       <c r="F9" s="4" t="s">
-        <v>477</v>
+        <v>476</v>
       </c>
       <c r="G9" s="4" t="s">
         <v>12</v>
@@ -7890,16 +7889,16 @@
         <v>2681</v>
       </c>
       <c r="B10" s="4" t="s">
+        <v>488</v>
+      </c>
+      <c r="C10" s="8" t="s">
         <v>489</v>
-      </c>
-      <c r="C10" s="8" t="s">
-        <v>490</v>
       </c>
       <c r="D10" s="4" t="s">
         <v>15</v>
       </c>
       <c r="E10" s="14" t="s">
-        <v>493</v>
+        <v>492</v>
       </c>
       <c r="F10" s="4"/>
       <c r="G10" s="4" t="s">
@@ -8005,16 +8004,16 @@
         <v>45</v>
       </c>
       <c r="B2" s="4" t="s">
+        <v>504</v>
+      </c>
+      <c r="C2" s="8" t="s">
         <v>505</v>
-      </c>
-      <c r="C2" s="8" t="s">
-        <v>506</v>
       </c>
       <c r="D2" s="4" t="s">
         <v>10</v>
       </c>
       <c r="E2" s="14" t="s">
-        <v>510</v>
+        <v>509</v>
       </c>
       <c r="F2" s="4"/>
       <c r="G2" s="4" t="s">
@@ -8034,16 +8033,16 @@
         <v>55</v>
       </c>
       <c r="B3" s="4" t="s">
+        <v>506</v>
+      </c>
+      <c r="C3" s="8" t="s">
         <v>507</v>
-      </c>
-      <c r="C3" s="8" t="s">
-        <v>508</v>
       </c>
       <c r="D3" s="4" t="s">
         <v>10</v>
       </c>
       <c r="E3" s="2" t="s">
-        <v>509</v>
+        <v>508</v>
       </c>
       <c r="F3" s="4"/>
       <c r="G3" s="4" t="s">
@@ -8063,19 +8062,19 @@
         <v>135</v>
       </c>
       <c r="B4" s="4" t="s">
+        <v>386</v>
+      </c>
+      <c r="C4" s="8" t="s">
         <v>387</v>
-      </c>
-      <c r="C4" s="8" t="s">
-        <v>388</v>
       </c>
       <c r="D4" s="4" t="s">
         <v>15</v>
       </c>
       <c r="E4" s="2" t="s">
-        <v>414</v>
+        <v>413</v>
       </c>
       <c r="F4" s="4" t="s">
-        <v>407</v>
+        <v>406</v>
       </c>
       <c r="G4" s="4" t="s">
         <v>11</v>
@@ -8094,22 +8093,22 @@
         <v>334</v>
       </c>
       <c r="B5" s="6" t="s">
+        <v>431</v>
+      </c>
+      <c r="C5" s="8" t="s">
         <v>432</v>
-      </c>
-      <c r="C5" s="8" t="s">
-        <v>433</v>
       </c>
       <c r="D5" s="4" t="s">
         <v>10</v>
       </c>
       <c r="E5" s="14" t="s">
-        <v>434</v>
+        <v>433</v>
       </c>
       <c r="F5" s="4" t="s">
-        <v>264</v>
+        <v>263</v>
       </c>
       <c r="G5" s="4" t="s">
-        <v>306</v>
+        <v>305</v>
       </c>
       <c r="H5" s="4" t="s">
         <v>28</v>
@@ -8125,10 +8124,10 @@
         <v>624</v>
       </c>
       <c r="B6" s="6" t="s">
+        <v>427</v>
+      </c>
+      <c r="C6" s="8" t="s">
         <v>428</v>
-      </c>
-      <c r="C6" s="8" t="s">
-        <v>429</v>
       </c>
       <c r="D6" s="4" t="s">
         <v>10</v>
@@ -8136,7 +8135,7 @@
       <c r="E6" s="6"/>
       <c r="F6" s="4"/>
       <c r="G6" s="4" t="s">
-        <v>369</v>
+        <v>368</v>
       </c>
       <c r="H6" s="4" t="s">
         <v>28</v>
@@ -8152,20 +8151,20 @@
         <v>649</v>
       </c>
       <c r="B7" s="6" t="s">
+        <v>388</v>
+      </c>
+      <c r="C7" s="8" t="s">
         <v>389</v>
-      </c>
-      <c r="C7" s="8" t="s">
-        <v>390</v>
       </c>
       <c r="D7" s="4" t="s">
         <v>10</v>
       </c>
       <c r="E7" s="6"/>
       <c r="F7" s="4" t="s">
-        <v>409</v>
+        <v>408</v>
       </c>
       <c r="G7" s="4" t="s">
-        <v>369</v>
+        <v>368</v>
       </c>
       <c r="H7" s="4" t="s">
         <v>43</v>
@@ -8181,20 +8180,20 @@
         <v>670</v>
       </c>
       <c r="B8" s="6" t="s">
+        <v>436</v>
+      </c>
+      <c r="C8" s="8" t="s">
         <v>437</v>
-      </c>
-      <c r="C8" s="8" t="s">
-        <v>438</v>
       </c>
       <c r="D8" s="4" t="s">
         <v>10</v>
       </c>
       <c r="E8" s="6"/>
       <c r="F8" s="4" t="s">
-        <v>425</v>
+        <v>424</v>
       </c>
       <c r="G8" s="4" t="s">
-        <v>369</v>
+        <v>368</v>
       </c>
       <c r="H8" s="4" t="s">
         <v>43</v>
@@ -8210,22 +8209,22 @@
         <v>767</v>
       </c>
       <c r="B9" s="6" t="s">
+        <v>307</v>
+      </c>
+      <c r="C9" s="8" t="s">
         <v>308</v>
-      </c>
-      <c r="C9" s="8" t="s">
-        <v>309</v>
       </c>
       <c r="D9" s="4" t="s">
         <v>10</v>
       </c>
       <c r="E9" s="14" t="s">
-        <v>403</v>
+        <v>402</v>
       </c>
       <c r="F9" s="4" t="s">
-        <v>408</v>
+        <v>407</v>
       </c>
       <c r="G9" s="4" t="s">
-        <v>306</v>
+        <v>305</v>
       </c>
       <c r="H9" s="4" t="s">
         <v>43</v>
@@ -8243,22 +8242,22 @@
         <v>768</v>
       </c>
       <c r="B10" s="6" t="s">
+        <v>440</v>
+      </c>
+      <c r="C10" s="8" t="s">
         <v>441</v>
-      </c>
-      <c r="C10" s="8" t="s">
-        <v>442</v>
       </c>
       <c r="D10" s="4" t="s">
         <v>15</v>
       </c>
       <c r="E10" s="14" t="s">
-        <v>457</v>
+        <v>456</v>
       </c>
       <c r="F10" s="4" t="s">
-        <v>456</v>
+        <v>455</v>
       </c>
       <c r="G10" s="4" t="s">
-        <v>369</v>
+        <v>368</v>
       </c>
       <c r="H10" s="4" t="s">
         <v>43</v>
@@ -8276,22 +8275,22 @@
         <v>769</v>
       </c>
       <c r="B11" s="6" t="s">
+        <v>438</v>
+      </c>
+      <c r="C11" s="8" t="s">
         <v>439</v>
-      </c>
-      <c r="C11" s="8" t="s">
-        <v>440</v>
       </c>
       <c r="D11" s="4" t="s">
         <v>10</v>
       </c>
       <c r="E11" s="14" t="s">
-        <v>457</v>
+        <v>456</v>
       </c>
       <c r="F11" s="4" t="s">
-        <v>456</v>
+        <v>455</v>
       </c>
       <c r="G11" s="4" t="s">
-        <v>369</v>
+        <v>368</v>
       </c>
       <c r="H11" s="4" t="s">
         <v>43</v>
@@ -8309,20 +8308,20 @@
         <v>781</v>
       </c>
       <c r="B12" s="6" t="s">
+        <v>460</v>
+      </c>
+      <c r="C12" s="8" t="s">
         <v>461</v>
-      </c>
-      <c r="C12" s="8" t="s">
-        <v>462</v>
       </c>
       <c r="D12" s="4" t="s">
         <v>10</v>
       </c>
       <c r="E12" s="14"/>
       <c r="F12" s="4" t="s">
-        <v>463</v>
+        <v>462</v>
       </c>
       <c r="G12" s="4" t="s">
-        <v>369</v>
+        <v>368</v>
       </c>
       <c r="H12" s="4" t="s">
         <v>43</v>
@@ -8338,20 +8337,20 @@
         <v>826</v>
       </c>
       <c r="B13" s="6" t="s">
+        <v>442</v>
+      </c>
+      <c r="C13" s="8" t="s">
         <v>443</v>
-      </c>
-      <c r="C13" s="8" t="s">
-        <v>444</v>
       </c>
       <c r="D13" s="4" t="s">
         <v>10</v>
       </c>
       <c r="E13" s="14"/>
       <c r="F13" s="4" t="s">
-        <v>264</v>
+        <v>263</v>
       </c>
       <c r="G13" s="4" t="s">
-        <v>306</v>
+        <v>305</v>
       </c>
       <c r="H13" s="4" t="s">
         <v>43</v>
@@ -8367,20 +8366,20 @@
         <v>945</v>
       </c>
       <c r="B14" s="6" t="s">
+        <v>410</v>
+      </c>
+      <c r="C14" s="8" t="s">
         <v>411</v>
-      </c>
-      <c r="C14" s="8" t="s">
-        <v>412</v>
       </c>
       <c r="D14" s="4" t="s">
         <v>10</v>
       </c>
       <c r="E14" s="14"/>
       <c r="F14" s="4" t="s">
-        <v>413</v>
+        <v>412</v>
       </c>
       <c r="G14" s="4" t="s">
-        <v>306</v>
+        <v>305</v>
       </c>
       <c r="H14" s="4" t="s">
         <v>43</v>
@@ -8396,20 +8395,20 @@
         <v>954</v>
       </c>
       <c r="B15" s="6" t="s">
+        <v>451</v>
+      </c>
+      <c r="C15" s="8" t="s">
         <v>452</v>
-      </c>
-      <c r="C15" s="8" t="s">
-        <v>453</v>
       </c>
       <c r="D15" s="4" t="s">
         <v>10</v>
       </c>
       <c r="E15" s="14"/>
       <c r="F15" s="4" t="s">
-        <v>407</v>
+        <v>406</v>
       </c>
       <c r="G15" s="4" t="s">
-        <v>369</v>
+        <v>368</v>
       </c>
       <c r="H15" s="4" t="s">
         <v>43</v>
@@ -8425,23 +8424,23 @@
         <v>984</v>
       </c>
       <c r="B16" s="6" t="s">
+        <v>444</v>
+      </c>
+      <c r="C16" s="8" t="s">
         <v>445</v>
-      </c>
-      <c r="C16" s="8" t="s">
-        <v>446</v>
       </c>
       <c r="D16" s="4" t="s">
         <v>10</v>
       </c>
       <c r="E16" s="14" t="s">
-        <v>448</v>
+        <v>447</v>
       </c>
       <c r="F16" s="4"/>
       <c r="G16" s="4" t="s">
-        <v>449</v>
+        <v>448</v>
       </c>
       <c r="H16" s="4" t="s">
-        <v>447</v>
+        <v>446</v>
       </c>
       <c r="I16" s="5">
         <v>45562</v>
@@ -8454,22 +8453,22 @@
         <v>1054</v>
       </c>
       <c r="B17" s="6" t="s">
+        <v>303</v>
+      </c>
+      <c r="C17" s="8" t="s">
         <v>304</v>
-      </c>
-      <c r="C17" s="8" t="s">
-        <v>305</v>
       </c>
       <c r="D17" s="4" t="s">
         <v>10</v>
       </c>
       <c r="E17" s="14" t="s">
-        <v>403</v>
+        <v>402</v>
       </c>
       <c r="F17" s="4" t="s">
-        <v>408</v>
+        <v>407</v>
       </c>
       <c r="G17" s="4" t="s">
-        <v>306</v>
+        <v>305</v>
       </c>
       <c r="H17" s="4" t="s">
         <v>43</v>
@@ -8487,10 +8486,10 @@
         <v>1144</v>
       </c>
       <c r="B18" s="6" t="s">
+        <v>429</v>
+      </c>
+      <c r="C18" s="8" t="s">
         <v>430</v>
-      </c>
-      <c r="C18" s="8" t="s">
-        <v>431</v>
       </c>
       <c r="D18" s="4" t="s">
         <v>10</v>
@@ -8498,7 +8497,7 @@
       <c r="E18" s="14"/>
       <c r="F18" s="4"/>
       <c r="G18" s="4" t="s">
-        <v>369</v>
+        <v>368</v>
       </c>
       <c r="H18" s="4" t="s">
         <v>43</v>
@@ -8514,10 +8513,10 @@
         <v>1330</v>
       </c>
       <c r="B19" s="6" t="s">
+        <v>477</v>
+      </c>
+      <c r="C19" s="8" t="s">
         <v>478</v>
-      </c>
-      <c r="C19" s="8" t="s">
-        <v>479</v>
       </c>
       <c r="D19" s="4" t="s">
         <v>15</v>
@@ -8525,7 +8524,7 @@
       <c r="E19" s="14"/>
       <c r="F19" s="4"/>
       <c r="G19" s="4" t="s">
-        <v>369</v>
+        <v>368</v>
       </c>
       <c r="H19" s="4" t="s">
         <v>28</v>
@@ -8541,20 +8540,20 @@
         <v>1363</v>
       </c>
       <c r="B20" s="6" t="s">
+        <v>449</v>
+      </c>
+      <c r="C20" s="8" t="s">
         <v>450</v>
-      </c>
-      <c r="C20" s="8" t="s">
-        <v>451</v>
       </c>
       <c r="D20" s="4" t="s">
         <v>15</v>
       </c>
       <c r="E20" s="14"/>
       <c r="F20" s="4" t="s">
-        <v>425</v>
+        <v>424</v>
       </c>
       <c r="G20" s="4" t="s">
-        <v>369</v>
+        <v>368</v>
       </c>
       <c r="H20" s="4" t="s">
         <v>43</v>
@@ -8572,20 +8571,20 @@
         <v>1481</v>
       </c>
       <c r="B21" s="6" t="s">
+        <v>422</v>
+      </c>
+      <c r="C21" s="8" t="s">
         <v>423</v>
-      </c>
-      <c r="C21" s="8" t="s">
-        <v>424</v>
       </c>
       <c r="D21" s="4" t="s">
         <v>10</v>
       </c>
       <c r="E21" s="14"/>
       <c r="F21" s="4" t="s">
-        <v>425</v>
+        <v>424</v>
       </c>
       <c r="G21" s="4" t="s">
-        <v>369</v>
+        <v>368</v>
       </c>
       <c r="H21" s="4" t="s">
         <v>43</v>
@@ -8601,22 +8600,22 @@
         <v>1713</v>
       </c>
       <c r="B22" s="6" t="s">
+        <v>453</v>
+      </c>
+      <c r="C22" s="8" t="s">
         <v>454</v>
-      </c>
-      <c r="C22" s="8" t="s">
-        <v>455</v>
       </c>
       <c r="D22" s="4" t="s">
         <v>15</v>
       </c>
       <c r="E22" s="14" t="s">
-        <v>434</v>
+        <v>433</v>
       </c>
       <c r="F22" s="4" t="s">
-        <v>264</v>
+        <v>263</v>
       </c>
       <c r="G22" s="4" t="s">
-        <v>306</v>
+        <v>305</v>
       </c>
       <c r="H22" s="4" t="s">
         <v>43</v>
@@ -8632,20 +8631,20 @@
         <v>2202</v>
       </c>
       <c r="B23" s="6" t="s">
+        <v>457</v>
+      </c>
+      <c r="C23" s="8" t="s">
         <v>458</v>
-      </c>
-      <c r="C23" s="8" t="s">
-        <v>459</v>
       </c>
       <c r="D23" s="4" t="s">
         <v>10</v>
       </c>
       <c r="E23" s="14" t="s">
-        <v>460</v>
+        <v>459</v>
       </c>
       <c r="F23" s="4"/>
       <c r="G23" s="4" t="s">
-        <v>252</v>
+        <v>251</v>
       </c>
       <c r="H23" s="4" t="s">
         <v>28</v>
@@ -8661,22 +8660,22 @@
         <v>2208</v>
       </c>
       <c r="B24" s="6" t="s">
+        <v>399</v>
+      </c>
+      <c r="C24" s="8" t="s">
         <v>400</v>
-      </c>
-      <c r="C24" s="8" t="s">
-        <v>401</v>
       </c>
       <c r="D24" s="4" t="s">
         <v>10</v>
       </c>
       <c r="E24" s="14" t="s">
-        <v>404</v>
+        <v>403</v>
       </c>
       <c r="F24" s="4" t="s">
-        <v>410</v>
+        <v>409</v>
       </c>
       <c r="G24" s="4" t="s">
-        <v>402</v>
+        <v>401</v>
       </c>
       <c r="H24" s="4" t="s">
         <v>43</v>
@@ -8692,20 +8691,20 @@
         <v>2412</v>
       </c>
       <c r="B25" s="6" t="s">
+        <v>493</v>
+      </c>
+      <c r="C25" s="8" t="s">
         <v>494</v>
-      </c>
-      <c r="C25" s="8" t="s">
-        <v>495</v>
       </c>
       <c r="D25" s="4" t="s">
         <v>15</v>
       </c>
       <c r="E25" s="14" t="s">
-        <v>496</v>
+        <v>495</v>
       </c>
       <c r="F25" s="4"/>
       <c r="G25" s="4" t="s">
-        <v>369</v>
+        <v>368</v>
       </c>
       <c r="H25" s="4" t="s">
         <v>28</v>
@@ -8767,7 +8766,7 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{ED305095-EC1E-B844-B25D-94A4272C0C0B}">
   <dimension ref="A1:K15"/>
   <sheetViews>
-    <sheetView tabSelected="1" zoomScaleNormal="100" workbookViewId="0"/>
+    <sheetView zoomScaleNormal="100" workbookViewId="0"/>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultColWidth="9" defaultRowHeight="16"/>
   <cols>
@@ -8823,16 +8822,16 @@
         <v>201</v>
       </c>
       <c r="B2" s="4" t="s">
+        <v>321</v>
+      </c>
+      <c r="C2" s="8" t="s">
         <v>322</v>
-      </c>
-      <c r="C2" s="8" t="s">
-        <v>323</v>
       </c>
       <c r="D2" s="4" t="s">
         <v>10</v>
       </c>
       <c r="E2" s="14" t="s">
-        <v>324</v>
+        <v>323</v>
       </c>
       <c r="F2" s="2"/>
       <c r="G2" s="4" t="s">
@@ -8852,16 +8851,16 @@
         <v>371</v>
       </c>
       <c r="B3" s="4" t="s">
+        <v>326</v>
+      </c>
+      <c r="C3" s="8" t="s">
         <v>327</v>
-      </c>
-      <c r="C3" s="8" t="s">
-        <v>328</v>
       </c>
       <c r="D3" s="4" t="s">
         <v>10</v>
       </c>
       <c r="E3" s="14" t="s">
-        <v>329</v>
+        <v>328</v>
       </c>
       <c r="F3" s="4"/>
       <c r="G3" s="4" t="s">
@@ -8883,10 +8882,10 @@
         <v>397</v>
       </c>
       <c r="B4" s="4" t="s">
+        <v>324</v>
+      </c>
+      <c r="C4" s="8" t="s">
         <v>325</v>
-      </c>
-      <c r="C4" s="8" t="s">
-        <v>326</v>
       </c>
       <c r="D4" s="4" t="s">
         <v>10</v>
@@ -8912,16 +8911,16 @@
         <v>477</v>
       </c>
       <c r="B5" s="4" t="s">
+        <v>345</v>
+      </c>
+      <c r="C5" s="8" t="s">
         <v>346</v>
-      </c>
-      <c r="C5" s="8" t="s">
-        <v>347</v>
       </c>
       <c r="D5" s="4" t="s">
         <v>10</v>
       </c>
       <c r="E5" s="6" t="s">
-        <v>348</v>
+        <v>347</v>
       </c>
       <c r="F5" s="4"/>
       <c r="G5" s="4" t="s">
@@ -8941,17 +8940,17 @@
         <v>600</v>
       </c>
       <c r="B6" s="4" t="s">
+        <v>537</v>
+      </c>
+      <c r="C6" s="8" t="s">
         <v>538</v>
-      </c>
-      <c r="C6" s="8" t="s">
-        <v>539</v>
       </c>
       <c r="D6" s="4" t="s">
         <v>15</v>
       </c>
       <c r="E6" s="6"/>
       <c r="F6" s="4" t="s">
-        <v>540</v>
+        <v>539</v>
       </c>
       <c r="G6" s="4" t="s">
         <v>13</v>
@@ -8970,10 +8969,10 @@
         <v>927</v>
       </c>
       <c r="B7" s="4" t="s">
+        <v>559</v>
+      </c>
+      <c r="C7" s="8" t="s">
         <v>560</v>
-      </c>
-      <c r="C7" s="8" t="s">
-        <v>561</v>
       </c>
       <c r="D7" s="4" t="s">
         <v>15</v>
@@ -8997,19 +8996,19 @@
         <v>1310</v>
       </c>
       <c r="B8" s="4" t="s">
+        <v>377</v>
+      </c>
+      <c r="C8" s="8" t="s">
         <v>378</v>
-      </c>
-      <c r="C8" s="8" t="s">
-        <v>379</v>
       </c>
       <c r="D8" s="4" t="s">
         <v>10</v>
       </c>
       <c r="E8" s="4" t="s">
-        <v>381</v>
+        <v>380</v>
       </c>
       <c r="F8" s="4" t="s">
-        <v>380</v>
+        <v>379</v>
       </c>
       <c r="G8" s="4" t="s">
         <v>11</v>
@@ -9028,10 +9027,10 @@
         <v>1404</v>
       </c>
       <c r="B9" s="4" t="s">
+        <v>329</v>
+      </c>
+      <c r="C9" s="8" t="s">
         <v>330</v>
-      </c>
-      <c r="C9" s="8" t="s">
-        <v>331</v>
       </c>
       <c r="D9" s="4" t="s">
         <v>10</v>
@@ -9055,16 +9054,16 @@
         <v>1734</v>
       </c>
       <c r="B10" s="4" t="s">
+        <v>374</v>
+      </c>
+      <c r="C10" s="8" t="s">
         <v>375</v>
-      </c>
-      <c r="C10" s="8" t="s">
-        <v>376</v>
       </c>
       <c r="D10" s="4" t="s">
         <v>10</v>
       </c>
       <c r="E10" s="4" t="s">
-        <v>377</v>
+        <v>376</v>
       </c>
       <c r="F10" s="4"/>
       <c r="G10" s="4" t="s">
@@ -9084,17 +9083,17 @@
         <v>1829</v>
       </c>
       <c r="B11" s="4" t="s">
+        <v>384</v>
+      </c>
+      <c r="C11" s="8" t="s">
         <v>385</v>
-      </c>
-      <c r="C11" s="8" t="s">
-        <v>386</v>
       </c>
       <c r="D11" s="4" t="s">
         <v>10</v>
       </c>
       <c r="E11" s="4"/>
       <c r="F11" s="4" t="s">
-        <v>380</v>
+        <v>379</v>
       </c>
       <c r="G11" s="4" t="s">
         <v>11</v>
@@ -9113,16 +9112,16 @@
         <v>2419</v>
       </c>
       <c r="B12" s="4" t="s">
+        <v>331</v>
+      </c>
+      <c r="C12" s="8" t="s">
         <v>332</v>
-      </c>
-      <c r="C12" s="8" t="s">
-        <v>333</v>
       </c>
       <c r="D12" s="4" t="s">
         <v>10</v>
       </c>
       <c r="E12" s="4" t="s">
-        <v>334</v>
+        <v>333</v>
       </c>
       <c r="F12" s="4"/>
       <c r="G12" s="4" t="s">
@@ -9142,16 +9141,16 @@
         <v>2425</v>
       </c>
       <c r="B13" s="4" t="s">
+        <v>342</v>
+      </c>
+      <c r="C13" s="8" t="s">
         <v>343</v>
-      </c>
-      <c r="C13" s="8" t="s">
-        <v>344</v>
       </c>
       <c r="D13" s="4" t="s">
         <v>10</v>
       </c>
       <c r="E13" s="4" t="s">
-        <v>345</v>
+        <v>344</v>
       </c>
       <c r="F13" s="4"/>
       <c r="G13" s="4" t="s">
@@ -9171,16 +9170,16 @@
         <v>2429</v>
       </c>
       <c r="B14" s="4" t="s">
+        <v>381</v>
+      </c>
+      <c r="C14" s="8" t="s">
         <v>382</v>
-      </c>
-      <c r="C14" s="8" t="s">
-        <v>383</v>
       </c>
       <c r="D14" s="4" t="s">
         <v>10</v>
       </c>
       <c r="E14" s="2" t="s">
-        <v>384</v>
+        <v>383</v>
       </c>
       <c r="F14" s="4"/>
       <c r="G14" s="4" t="s">
@@ -9200,16 +9199,16 @@
         <v>2683</v>
       </c>
       <c r="B15" s="4" t="s">
+        <v>334</v>
+      </c>
+      <c r="C15" s="8" t="s">
         <v>335</v>
-      </c>
-      <c r="C15" s="8" t="s">
-        <v>336</v>
       </c>
       <c r="D15" s="4" t="s">
         <v>10</v>
       </c>
       <c r="E15" s="6" t="s">
-        <v>337</v>
+        <v>336</v>
       </c>
       <c r="F15" s="4"/>
       <c r="G15" s="4" t="s">
@@ -9319,23 +9318,23 @@
         <v>23</v>
       </c>
       <c r="B2" s="4" t="s">
+        <v>309</v>
+      </c>
+      <c r="C2" s="8" t="s">
         <v>310</v>
-      </c>
-      <c r="C2" s="8" t="s">
-        <v>311</v>
       </c>
       <c r="D2" s="4" t="s">
         <v>15</v>
       </c>
       <c r="E2" s="6"/>
       <c r="F2" s="4" t="s">
-        <v>314</v>
+        <v>313</v>
       </c>
       <c r="G2" s="4" t="s">
+        <v>311</v>
+      </c>
+      <c r="H2" s="4" t="s">
         <v>312</v>
-      </c>
-      <c r="H2" s="4" t="s">
-        <v>313</v>
       </c>
       <c r="I2" s="5">
         <v>45503</v>
@@ -9537,7 +9536,7 @@
         <v>48</v>
       </c>
       <c r="E9" s="6" t="s">
-        <v>374</v>
+        <v>373</v>
       </c>
       <c r="F9" s="4"/>
       <c r="G9" s="4" t="s">
@@ -9877,7 +9876,7 @@
         <v>48</v>
       </c>
       <c r="E7" s="4" t="s">
-        <v>225</v>
+        <v>224</v>
       </c>
       <c r="F7" s="4" t="s">
         <v>125</v>
@@ -10018,7 +10017,7 @@
         <v>48</v>
       </c>
       <c r="E12" s="6" t="s">
-        <v>276</v>
+        <v>275</v>
       </c>
       <c r="F12" s="4"/>
       <c r="G12" s="4" t="s">
@@ -10038,16 +10037,16 @@
         <v>968</v>
       </c>
       <c r="B13" s="4" t="s">
+        <v>348</v>
+      </c>
+      <c r="C13" s="8" t="s">
         <v>349</v>
-      </c>
-      <c r="C13" s="8" t="s">
-        <v>350</v>
       </c>
       <c r="D13" s="4" t="s">
         <v>48</v>
       </c>
       <c r="E13" s="14" t="s">
-        <v>351</v>
+        <v>350</v>
       </c>
       <c r="F13" s="4"/>
       <c r="G13" s="4" t="s">
@@ -10186,10 +10185,10 @@
         <v>238</v>
       </c>
       <c r="B2" s="6" t="s">
+        <v>298</v>
+      </c>
+      <c r="C2" s="8" t="s">
         <v>299</v>
-      </c>
-      <c r="C2" s="8" t="s">
-        <v>300</v>
       </c>
       <c r="D2" s="4" t="s">
         <v>10</v>
@@ -10213,10 +10212,10 @@
         <v>304</v>
       </c>
       <c r="B3" s="6" t="s">
-        <v>285</v>
+        <v>284</v>
       </c>
       <c r="C3" s="8" t="s">
-        <v>287</v>
+        <v>286</v>
       </c>
       <c r="D3" s="4" t="s">
         <v>10</v>
@@ -10227,7 +10226,7 @@
         <v>28</v>
       </c>
       <c r="H3" s="4" t="s">
-        <v>286</v>
+        <v>285</v>
       </c>
       <c r="I3" s="5">
         <v>45526</v>
@@ -10240,10 +10239,10 @@
         <v>525</v>
       </c>
       <c r="B4" s="6" t="s">
+        <v>470</v>
+      </c>
+      <c r="C4" s="8" t="s">
         <v>471</v>
-      </c>
-      <c r="C4" s="8" t="s">
-        <v>472</v>
       </c>
       <c r="D4" s="4" t="s">
         <v>10</v>
@@ -10267,17 +10266,17 @@
         <v>528</v>
       </c>
       <c r="B5" s="6" t="s">
-        <v>289</v>
+        <v>288</v>
       </c>
       <c r="C5" s="8" t="s">
-        <v>288</v>
+        <v>287</v>
       </c>
       <c r="D5" s="4" t="s">
         <v>10</v>
       </c>
       <c r="E5" s="14"/>
       <c r="F5" s="4" t="s">
-        <v>264</v>
+        <v>263</v>
       </c>
       <c r="G5" s="4" t="s">
         <v>13</v>
@@ -10296,19 +10295,19 @@
         <v>560</v>
       </c>
       <c r="B6" s="6" t="s">
+        <v>395</v>
+      </c>
+      <c r="C6" s="8" t="s">
         <v>396</v>
-      </c>
-      <c r="C6" s="8" t="s">
-        <v>397</v>
       </c>
       <c r="D6" s="4" t="s">
         <v>10</v>
       </c>
       <c r="E6" s="14" t="s">
-        <v>399</v>
+        <v>398</v>
       </c>
       <c r="F6" s="4" t="s">
-        <v>398</v>
+        <v>397</v>
       </c>
       <c r="G6" s="4" t="s">
         <v>11</v>
@@ -10327,17 +10326,17 @@
         <v>713</v>
       </c>
       <c r="B7" s="6" t="s">
+        <v>472</v>
+      </c>
+      <c r="C7" s="8" t="s">
         <v>473</v>
-      </c>
-      <c r="C7" s="8" t="s">
-        <v>474</v>
       </c>
       <c r="D7" s="4" t="s">
         <v>10</v>
       </c>
       <c r="E7" s="14"/>
       <c r="F7" s="4" t="s">
-        <v>255</v>
+        <v>254</v>
       </c>
       <c r="G7" s="4" t="s">
         <v>11</v>
@@ -10356,10 +10355,10 @@
         <v>848</v>
       </c>
       <c r="B8" s="6" t="s">
-        <v>291</v>
+        <v>290</v>
       </c>
       <c r="C8" s="8" t="s">
-        <v>290</v>
+        <v>289</v>
       </c>
       <c r="D8" s="4" t="s">
         <v>10</v>
@@ -10383,17 +10382,17 @@
         <v>862</v>
       </c>
       <c r="B9" s="6" t="s">
+        <v>282</v>
+      </c>
+      <c r="C9" s="8" t="s">
         <v>283</v>
-      </c>
-      <c r="C9" s="8" t="s">
-        <v>284</v>
       </c>
       <c r="D9" s="4" t="s">
         <v>15</v>
       </c>
       <c r="E9" s="14"/>
       <c r="F9" s="4" t="s">
-        <v>255</v>
+        <v>254</v>
       </c>
       <c r="G9" s="4" t="s">
         <v>11</v>
@@ -10414,19 +10413,19 @@
         <v>930</v>
       </c>
       <c r="B10" s="6" t="s">
+        <v>291</v>
+      </c>
+      <c r="C10" s="8" t="s">
         <v>292</v>
-      </c>
-      <c r="C10" s="8" t="s">
-        <v>293</v>
       </c>
       <c r="D10" s="4" t="s">
         <v>10</v>
       </c>
       <c r="E10" s="14" t="s">
-        <v>294</v>
+        <v>293</v>
       </c>
       <c r="F10" s="4" t="s">
-        <v>255</v>
+        <v>254</v>
       </c>
       <c r="G10" s="4" t="s">
         <v>11</v>
@@ -10445,19 +10444,19 @@
         <v>1124</v>
       </c>
       <c r="B11" s="6" t="s">
+        <v>370</v>
+      </c>
+      <c r="C11" s="8" t="s">
         <v>371</v>
-      </c>
-      <c r="C11" s="8" t="s">
-        <v>372</v>
       </c>
       <c r="D11" s="4" t="s">
         <v>10</v>
       </c>
       <c r="E11" s="14" t="s">
-        <v>373</v>
+        <v>372</v>
       </c>
       <c r="F11" s="4" t="s">
-        <v>321</v>
+        <v>320</v>
       </c>
       <c r="G11" s="4" t="s">
         <v>11</v>
@@ -10476,10 +10475,10 @@
         <v>1423</v>
       </c>
       <c r="B12" s="6" t="s">
+        <v>468</v>
+      </c>
+      <c r="C12" s="8" t="s">
         <v>469</v>
-      </c>
-      <c r="C12" s="8" t="s">
-        <v>470</v>
       </c>
       <c r="D12" s="4" t="s">
         <v>10</v>
@@ -10503,10 +10502,10 @@
         <v>1524</v>
       </c>
       <c r="B13" s="6" t="s">
-        <v>296</v>
+        <v>295</v>
       </c>
       <c r="C13" s="8" t="s">
-        <v>295</v>
+        <v>294</v>
       </c>
       <c r="D13" s="4" t="s">
         <v>10</v>
@@ -10530,25 +10529,25 @@
         <v>1862</v>
       </c>
       <c r="B14" s="6" t="s">
-        <v>272</v>
+        <v>271</v>
       </c>
       <c r="C14" s="8" t="s">
-        <v>271</v>
+        <v>270</v>
       </c>
       <c r="D14" s="4" t="s">
         <v>15</v>
       </c>
       <c r="E14" s="14" t="s">
-        <v>275</v>
+        <v>274</v>
       </c>
       <c r="F14" s="4" t="s">
-        <v>321</v>
+        <v>320</v>
       </c>
       <c r="G14" s="4" t="s">
+        <v>272</v>
+      </c>
+      <c r="H14" s="4" t="s">
         <v>273</v>
-      </c>
-      <c r="H14" s="4" t="s">
-        <v>274</v>
       </c>
       <c r="I14" s="5">
         <v>45521</v>
@@ -10561,10 +10560,10 @@
         <v>1894</v>
       </c>
       <c r="B15" s="6" t="s">
+        <v>296</v>
+      </c>
+      <c r="C15" s="8" t="s">
         <v>297</v>
-      </c>
-      <c r="C15" s="8" t="s">
-        <v>298</v>
       </c>
       <c r="D15" s="4" t="s">
         <v>10</v>
@@ -10588,19 +10587,19 @@
         <v>2025</v>
       </c>
       <c r="B16" s="6" t="s">
+        <v>555</v>
+      </c>
+      <c r="C16" s="8" t="s">
         <v>556</v>
-      </c>
-      <c r="C16" s="8" t="s">
-        <v>557</v>
       </c>
       <c r="D16" s="4" t="s">
         <v>15</v>
       </c>
       <c r="E16" s="14" t="s">
-        <v>559</v>
+        <v>558</v>
       </c>
       <c r="F16" s="4" t="s">
-        <v>558</v>
+        <v>557</v>
       </c>
       <c r="G16" s="4" t="s">
         <v>12</v>
@@ -10619,16 +10618,16 @@
         <v>2302</v>
       </c>
       <c r="B17" s="6" t="s">
+        <v>279</v>
+      </c>
+      <c r="C17" s="8" t="s">
         <v>280</v>
-      </c>
-      <c r="C17" s="8" t="s">
-        <v>281</v>
       </c>
       <c r="D17" s="4" t="s">
         <v>15</v>
       </c>
       <c r="E17" s="14" t="s">
-        <v>282</v>
+        <v>281</v>
       </c>
       <c r="F17" s="4"/>
       <c r="G17" s="4" t="s">
@@ -10650,17 +10649,17 @@
         <v>2382</v>
       </c>
       <c r="B18" s="6" t="s">
+        <v>542</v>
+      </c>
+      <c r="C18" s="8" t="s">
         <v>543</v>
-      </c>
-      <c r="C18" s="8" t="s">
-        <v>544</v>
       </c>
       <c r="D18" s="4" t="s">
         <v>15</v>
       </c>
       <c r="E18" s="14"/>
       <c r="F18" s="6" t="s">
-        <v>545</v>
+        <v>544</v>
       </c>
       <c r="G18" s="4" t="s">
         <v>12</v>
@@ -10679,17 +10678,17 @@
         <v>2438</v>
       </c>
       <c r="B19" s="6" t="s">
+        <v>300</v>
+      </c>
+      <c r="C19" s="8" t="s">
         <v>301</v>
-      </c>
-      <c r="C19" s="8" t="s">
-        <v>302</v>
       </c>
       <c r="D19" s="4" t="s">
         <v>10</v>
       </c>
       <c r="E19" s="14"/>
       <c r="F19" s="4" t="s">
-        <v>303</v>
+        <v>302</v>
       </c>
       <c r="G19" s="4" t="s">
         <v>11</v>
@@ -10708,17 +10707,17 @@
         <v>2488</v>
       </c>
       <c r="B20" s="6" t="s">
+        <v>540</v>
+      </c>
+      <c r="C20" s="8" t="s">
         <v>541</v>
-      </c>
-      <c r="C20" s="8" t="s">
-        <v>542</v>
       </c>
       <c r="D20" s="4" t="s">
         <v>15</v>
       </c>
       <c r="E20" s="14"/>
       <c r="F20" s="4" t="s">
-        <v>321</v>
+        <v>320</v>
       </c>
       <c r="G20" s="4" t="s">
         <v>11</v>

</xml_diff>